<commit_message>
preenchimento da planilha com os produtos p controle
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF05F5A3-599D-428F-A7E7-B9D53CEB15E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24C213D-6E69-45AB-9842-B619E55DF6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
   <si>
     <t>CÓDIGO DO PRODUTO</t>
   </si>
@@ -47,339 +47,12 @@
     <t>CATEGORIA</t>
   </si>
   <si>
-    <t>Anda Cavalinho Com Som Azul - Xalingo SITE</t>
-  </si>
-  <si>
     <t>PEDAGÓGICO</t>
   </si>
   <si>
-    <t>002 - Balanço De Ursinho Infantil Xalingo Sem Gancho COM Cinto SITE</t>
-  </si>
-  <si>
-    <t>003 - Balanço Fofossauro 3 Em 1 Encosto Regulável Xalingo SITE</t>
-  </si>
-  <si>
-    <t>004 - Balanço Infantil 3 Em 1 Barra Proteção Unicórnio Xalingo SITTE</t>
-  </si>
-  <si>
-    <t>005 - Balanço Infantil Borboletinha Trava Cordas Reforçado SITE</t>
-  </si>
-  <si>
-    <t>006 - Balanço infantil Mickey Mouse Xalingo 19798 cor vermelho e preto SITE</t>
-  </si>
-  <si>
-    <t>007 - Balanço infantil Minnie Mouse 3 em 1 rosa playground Xalingo SITE</t>
-  </si>
-  <si>
-    <t>008 - Balanço Infantil Para Bebê  E Criança - Playground - Diversão  SITE</t>
-  </si>
-  <si>
-    <t>009 - Balanço Patrulha Canina Encosto Cinto Infantil Bebê Até 36m SITE</t>
-  </si>
-  <si>
-    <t>010 - Balanço Spider Man Super Hero Adventure Xalingo Homem Aranha SITE</t>
-  </si>
-  <si>
-    <t>011 - banner arvore da vida site</t>
-  </si>
-  <si>
-    <t>012 - banner cardapio da semana site</t>
-  </si>
-  <si>
-    <t>013 - banner celula vegetal e animal site</t>
-  </si>
-  <si>
-    <t>014 - banner plantas site</t>
-  </si>
-  <si>
-    <t>015 - banner tabuada adição site</t>
-  </si>
-  <si>
-    <t>016 - banner ajudante do dia site</t>
-  </si>
-  <si>
-    <t>017 - banner alfabeto</t>
-  </si>
-  <si>
-    <t>018 - banner animais vertebrados aves site</t>
-  </si>
-  <si>
-    <t>019 - banner animais vertebrados anfibios site</t>
-  </si>
-  <si>
-    <t>020 - banner animais vertebrados mamiferos site</t>
-  </si>
-  <si>
-    <t>021 - banner animais vertebrados peixes site</t>
-  </si>
-  <si>
-    <t>022 -banner aniversariante do mes site</t>
-  </si>
-  <si>
-    <t>023 - banner aprenda a lavar a mao corretamente</t>
-  </si>
-  <si>
-    <t>024 - banner bioma do brasil site</t>
-  </si>
-  <si>
-    <t>025 - banner boa convivencia site</t>
-  </si>
-  <si>
-    <t>026 - banner calendario site</t>
-  </si>
-  <si>
-    <t>027 - banner cantinho da leitura site</t>
-  </si>
-  <si>
-    <t>028 - banner chamadinha site</t>
-  </si>
-  <si>
-    <t>029 - banner ciclo da agua</t>
-  </si>
-  <si>
-    <t>030 - banner clima do brasil</t>
-  </si>
-  <si>
-    <t>031 - banner clima site</t>
-  </si>
-  <si>
-    <t>032 - banner combinados da turma</t>
-  </si>
-  <si>
-    <t>033 - banner diga nao ao bulling site</t>
-  </si>
-  <si>
-    <t>034 - banner divisão site</t>
-  </si>
-  <si>
-    <t>035 - BANNER ESQUELETO HUMANO</t>
-  </si>
-  <si>
-    <t>036 - banner formas  geometricas</t>
-  </si>
-  <si>
-    <t>037 - banner formas geometricas completa</t>
-  </si>
-  <si>
-    <t>038 - banner fraçao site</t>
-  </si>
-  <si>
-    <t>039 - banner generos textuais site</t>
-  </si>
-  <si>
-    <t>040 - banner geografia</t>
-  </si>
-  <si>
-    <t>041 - banner hino nacional brasileiro site</t>
-  </si>
-  <si>
-    <t>042 - banner mapa de são paulo site</t>
-  </si>
-  <si>
-    <t>043 - banner mapa do brasil</t>
-  </si>
-  <si>
-    <t>044 - banner mapa economico brasileiro site</t>
-  </si>
-  <si>
-    <t>045 - banner mapa mundi site</t>
-  </si>
-  <si>
-    <t>046 - banner mapa municipal de sao paulo site</t>
-  </si>
-  <si>
-    <t>047 - Banner Meses do Ano - 80 x 120 cm (L x A)</t>
-  </si>
-  <si>
-    <t>048 - banner montagem silabica  site</t>
-  </si>
-  <si>
-    <t>049 - banner numerais de 0 a 100 site</t>
-  </si>
-  <si>
-    <t>050 - banner numerais e escritas</t>
-  </si>
-  <si>
-    <t>051 - banner numeros romanos site</t>
-  </si>
-  <si>
-    <t>052 - Banner ou painel corpo humano material gratuito</t>
-  </si>
-  <si>
-    <t>053 - banner palavrinhas magicas site</t>
-  </si>
-  <si>
-    <t>054 - banner pedagogico animais vertebrados répteis site</t>
-  </si>
-  <si>
-    <t>055 - banner personalizado conforme a solicitação do cliente site</t>
-  </si>
-  <si>
-    <t>056 - banner presidentes do brasil site</t>
-  </si>
-  <si>
-    <t>057 - banner regras do porque site</t>
-  </si>
-  <si>
-    <t>058 - banner regras matematica</t>
-  </si>
-  <si>
-    <t>059 - banner silabario simples site</t>
-  </si>
-  <si>
-    <t>060 - banner sinais de pontuacao site</t>
-  </si>
-  <si>
-    <t>070 - banner sistema muscular site</t>
-  </si>
-  <si>
-    <t>071 - banner subtracao site</t>
-  </si>
-  <si>
-    <t>072 - banner tabela periodica</t>
-  </si>
-  <si>
-    <t>073 - banner tabuada site</t>
-  </si>
-  <si>
-    <t>074 - banner texto narrativo site</t>
-  </si>
-  <si>
-    <t>075 - banner vogais e consuantes</t>
-  </si>
-  <si>
-    <t>076 - banner vogais site</t>
-  </si>
-  <si>
-    <t>077 - Baú Infantil Hipo Roxo - Xalingo SITE</t>
-  </si>
-  <si>
-    <t>078 - Brinquedo Gangorra Individual Pluto Amarelo Xalingo SITE</t>
-  </si>
-  <si>
-    <t>079 - Brinquedo Infantil Minnie Com Empurrador E Proteção Xalingo SITE</t>
-  </si>
-  <si>
-    <t>080 - Caixa de Areia Infantil Estrela do Mar Vermelha Xalingo site</t>
-  </si>
-  <si>
-    <t>081 - Carrinho Infantil Xalingo Cozy Couple Little Tikes Ref.59110 Cor Vermelho SITE</t>
-  </si>
-  <si>
-    <t>082 - Carrinho Velotrol Infantil Criança Bebê COM empurrador SITE</t>
-  </si>
-  <si>
-    <t>083 -Carrossel Gira Pato Xalingo SITE</t>
-  </si>
-  <si>
-    <t>084 - Cercadinho Infantil Colorido Xalingo site</t>
-  </si>
-  <si>
-    <t>085 - Escorregador com Balanço Xalingo SITE</t>
-  </si>
-  <si>
-    <t>086 - Escorregador Infantil Desmontável Vermelho Xalingo SITE</t>
-  </si>
-  <si>
-    <t>087 - Escorregador Infantil Master Laranja Xalingo SITE</t>
-  </si>
-  <si>
-    <t>088 - Gangorra 2 Lugares Disney SITE</t>
-  </si>
-  <si>
-    <t>089 - Gangorra Anda Cavalinho Pocoto Vermelho Xalingo SITE</t>
-  </si>
-  <si>
-    <t>090 - Gangorra Bidu Turma Da Mônica Xalingo</t>
-  </si>
-  <si>
-    <t>091 - Gangorra Cavalinho Balanço Infantil Criança Azul - Xalingo SITE</t>
-  </si>
-  <si>
-    <t>092 - Gangorra Cavalinho Infantil Nhoca SITE</t>
-  </si>
-  <si>
-    <t>093 - Gangorra Dinossauro DUPLO SITE</t>
-  </si>
-  <si>
-    <t>094 - Gangorra Infantil Dupla Fofossauros Xalingo SITE 3</t>
-  </si>
-  <si>
-    <t>095 - Gangorra Infantil Minhoca Verde Xalingo SITE</t>
-  </si>
-  <si>
-    <t>096 - Gangorra Infantil Mini Moto Parquinhos Xalingo Cor Laranja SITE</t>
-  </si>
-  <si>
-    <t>097 - Gangorra Infantil Scooter Do Mickey Disney Xalingo - 1874.3 Cor Vermelho SITE</t>
-  </si>
-  <si>
-    <t>098 - Gangorra Infantil Tigrão Disney Baby - Xalingo SITE</t>
-  </si>
-  <si>
-    <t>099 - Img Kits Profissões</t>
-  </si>
-  <si>
-    <t>100 - kit 4 banners infanto-juvenil site</t>
-  </si>
-  <si>
-    <t>101 - Mesa Sirizinho Xalingo Com Bancos Acoplados SITE</t>
-  </si>
-  <si>
-    <t>102 - Motoquinha Triciclo Infantil Com Pedal Tigrão Xalingo SITE</t>
-  </si>
-  <si>
-    <t>103 - Motoquinha Triciclo Infantil Joaninha Xalingo Com Pedal SITE</t>
-  </si>
-  <si>
-    <t>104 - New Big Playground site</t>
-  </si>
-  <si>
-    <t>105 - Play Dog House - Xalingo site</t>
-  </si>
-  <si>
-    <t>106 - Playground Barco Pirata Little Tikes Xalingo SITE</t>
-  </si>
-  <si>
-    <t>107 - Playground Casinha Infantil Cabana De Campo Little Tikes SITE</t>
-  </si>
-  <si>
-    <t>108 - Playground Castelo Medieval Xalingo site</t>
-  </si>
-  <si>
-    <t>109 - Playground Infantil Xalingo Dupla Diversão Little Tikes SITE</t>
-  </si>
-  <si>
-    <t>110 - Playground Parquinho De Atividades site</t>
-  </si>
-  <si>
-    <t>111 - Playground Trenzinho Da Alegria Xalingo SITE</t>
-  </si>
-  <si>
-    <t>112 - Rede De Dormir Infantil Berço site</t>
-  </si>
-  <si>
-    <t>113 - Triciclo Motoca Infantil Fofossauros Verde Laranja Xalingo SITE</t>
-  </si>
-  <si>
-    <t>114 - Triciclo Peixinho Com Empurrador cestinha Xalingo  SITE</t>
-  </si>
-  <si>
     <t>115 - Trave De Plático Futebol Golzinho Desmontável</t>
   </si>
   <si>
-    <t>116 - Triciclo Blue Race 3 Em 1 Xalingo Carrinho De Passeio SITE</t>
-  </si>
-  <si>
-    <t>117 - Triciclo Cachorrinho Empurrador Proteção E Cestinha Xalingo  SITE</t>
-  </si>
-  <si>
-    <t>118 - Triciclo Com Empurrador E Proteção Mickey Xalingo Vermelho SITE</t>
-  </si>
-  <si>
-    <t>119 - Triciclo Fox Racer - Xalingo SITE</t>
-  </si>
-  <si>
     <t>120 - Triciclo Infantil Borboletinha Rosa Com Pedal Xalingo SITE</t>
   </si>
   <si>
@@ -510,6 +183,594 @@
   </si>
   <si>
     <t>163 - Ventilador Oscilante Mesa Turbo 30cm 110v Vermelho Ventisol</t>
+  </si>
+  <si>
+    <t>164 - Ventilador Oscilante De Parede 50cm 6 Pás Ventisol Monta Fácil 135w Preto 220v</t>
+  </si>
+  <si>
+    <t>165 - Ventilador Oscliante De Parede Premium 50cm Venti Delta Preto Bivolt</t>
+  </si>
+  <si>
+    <t>166 - Ventilador Ventisilva Delta Oscilante Parede 50 Cm Bivolt Preto</t>
+  </si>
+  <si>
+    <t>167 - Ventilador Ventisilva Coluna Mesa 2 Em 1</t>
+  </si>
+  <si>
+    <t>168 - mototico passeio e pedal azul</t>
+  </si>
+  <si>
+    <t>169 - mototico passeio e pedal rosa</t>
+  </si>
+  <si>
+    <t>170 - mototico patrulha canina passeio e pedal</t>
+  </si>
+  <si>
+    <t>171 - mototico peppa pig passeio e pedal</t>
+  </si>
+  <si>
+    <t>172 - tonkinha doggy passeio e pedal</t>
+  </si>
+  <si>
+    <t>173 - tonkinha gatinha passeio e pedal</t>
+  </si>
+  <si>
+    <t>174 - triciclo europa (vermelho)</t>
+  </si>
+  <si>
+    <t>175 - triciclo europa passeio e pedal (rosa)</t>
+  </si>
+  <si>
+    <t>176 - triciclo europa passeio e pedal azul</t>
+  </si>
+  <si>
+    <t>178 - triciclo europa rosa</t>
+  </si>
+  <si>
+    <t>179 - velobaby passeio e pedal rosa</t>
+  </si>
+  <si>
+    <t>180 - velobaby passeio e pedal</t>
+  </si>
+  <si>
+    <t>181 - velobaby reclinavel com capota passeio e pedal azul</t>
+  </si>
+  <si>
+    <t>182 - Cone</t>
+  </si>
+  <si>
+    <t>183 - Piso molhado</t>
+  </si>
+  <si>
+    <t>184 - Dispenser para copo de água e café</t>
+  </si>
+  <si>
+    <t>185 - Dispensers1</t>
+  </si>
+  <si>
+    <t>186 - Dispensers2</t>
+  </si>
+  <si>
+    <t>187 - Fita demarcação</t>
+  </si>
+  <si>
+    <t>188 - Canecas Personalizadas</t>
+  </si>
+  <si>
+    <t>189 - Garrafa Personalizada</t>
+  </si>
+  <si>
+    <t>190 - Necessaires</t>
+  </si>
+  <si>
+    <t>191 - Tacas Personalizadas</t>
+  </si>
+  <si>
+    <t>192 - Pedestal unitario e em corrente plastica</t>
+  </si>
+  <si>
+    <t>193 - Suporte para copos de água e café</t>
+  </si>
+  <si>
+    <t>194 - Tapete Sanitizante</t>
+  </si>
+  <si>
+    <t>195 - Totens para alcool em gel</t>
+  </si>
+  <si>
+    <t>196 - Totem dispenser de alcool em gel e termometro por sensor</t>
+  </si>
+  <si>
+    <t>197 - Conjunto Completo - Tênis De Mesa - Ping Pong - Rede E Raquete STE</t>
+  </si>
+  <si>
+    <t>198 - Jogo De Botão Brasileirão Xalingo SITE</t>
+  </si>
+  <si>
+    <t>199 - Jogo De Ping Pong Simples - Xalingo SITE</t>
+  </si>
+  <si>
+    <t>200 - Mesa de pebolim Xalingo Super copa cor verde  SITE</t>
+  </si>
+  <si>
+    <t>201 - Mesa E Jogo De Futebol De Botão Com 2 Marcadores Xalingo SITE</t>
+  </si>
+  <si>
+    <t>202 - Mesa Para Ping Pong  Tênis De Mesa Azul COM  Pés Dobráveis SITE</t>
+  </si>
+  <si>
+    <t>203 - Tabela Basquete Mdf 9mm Aro 36 Cm Basketball Master Xalingo SITE</t>
+  </si>
+  <si>
+    <t>204 - Tabela De Basquete infantil SITE</t>
+  </si>
+  <si>
+    <t>205 - Xalingo tabela cesta de basquete com bola SITE</t>
+  </si>
+  <si>
+    <t>206 - Rede Cadeira Balanço Descanso Teto Suspensa Luxo Varanda</t>
+  </si>
+  <si>
+    <t>207 - Rede De Berço Baby 100 por cento algodão</t>
+  </si>
+  <si>
+    <t>208 - Rede De Descanso Infantil 1,50m  Azul</t>
+  </si>
+  <si>
+    <t>209 - Rede De Dormir Descanso Grande Artesanal Varias Cores</t>
+  </si>
+  <si>
+    <t>210 - Rede De Dormir Descanso Grande Resistente</t>
+  </si>
+  <si>
+    <t>211 - 1 Metro - Tecido Nylon 70 Emborrachado 100 por cento Impermeavel SITE</t>
+  </si>
+  <si>
+    <t>212 - 1 Metro De Tecido Tricoline Misto Liso (1,00mx1,47m) SITE</t>
+  </si>
+  <si>
+    <t>213 - 1 Rolo Vies Tecido Helanca Cortado 2,5cm SITE</t>
+  </si>
+  <si>
+    <t>214 - 1m - Tecido Voil Voal 3 Metros De Largura Para Cortinas SITE</t>
+  </si>
+  <si>
+    <t>215 - 1m Tecido Cetim SITE</t>
+  </si>
+  <si>
+    <t>216 - 10m Tecido Tule Liso - Diversas Cores - 100% Poliéster SITE</t>
+  </si>
+  <si>
+    <t>217 - Tecido Algodão Cru 160gr M2 Larg 1,60  SITE</t>
+  </si>
+  <si>
+    <t>218 - Tecido Chita 100% Algodão 3m X 1,40cm  SITE</t>
+  </si>
+  <si>
+    <t>219 - Tecido De Juta P9 - Rolo Fechado SITE</t>
+  </si>
+  <si>
+    <t>220 - Tecido Napa Bagum Bagun Impermeavel SITE</t>
+  </si>
+  <si>
+    <t>221 - Tecido Oxford Liso 5 Cores (5,00mx1,47m SITE</t>
+  </si>
+  <si>
+    <t>222 - Tecido Suede Liso SITE</t>
+  </si>
+  <si>
+    <t>223 - Tecido Viscose Lisa site</t>
+  </si>
+  <si>
+    <t>224 - Tecidos Malha Veludo Cristal Liso 1 X 1,50 Metro SITE</t>
+  </si>
+  <si>
+    <t>225 - Tnt Preto Tecido  1,40mx 3 Metros Liso SITE</t>
+  </si>
+  <si>
+    <t>226 - banner ajudante do dia</t>
+  </si>
+  <si>
+    <t>227 - banner aniversariante do mes</t>
+  </si>
+  <si>
+    <t>228 - banner chamadinha</t>
+  </si>
+  <si>
+    <t>229 - boas maneiras, regrinhas de convivencia</t>
+  </si>
+  <si>
+    <t>230 - emborrachado de calendario personalizavel</t>
+  </si>
+  <si>
+    <t>231 - defina seu cardapio da semana</t>
+  </si>
+  <si>
+    <t>232 - boneca 1</t>
+  </si>
+  <si>
+    <t>233 - boneca 2</t>
+  </si>
+  <si>
+    <t>234 - boneca 3</t>
+  </si>
+  <si>
+    <t>235 - boneca 4</t>
+  </si>
+  <si>
+    <t>236 - boneca 5</t>
+  </si>
+  <si>
+    <t>237 - boneca 6</t>
+  </si>
+  <si>
+    <t>238 - boneca 7</t>
+  </si>
+  <si>
+    <t>239 - cozinha infantil retro branca</t>
+  </si>
+  <si>
+    <t>240 - cozinha infantil retro noruega</t>
+  </si>
+  <si>
+    <t>241 - cozinha infantil retro verde agua</t>
+  </si>
+  <si>
+    <t>242 - cozinha infantil retro vermelha</t>
+  </si>
+  <si>
+    <t>243 - cozinha infantil retro vintage</t>
+  </si>
+  <si>
+    <t>244 - Mordedor Bolinha Baby Ball</t>
+  </si>
+  <si>
+    <t>245 - Carrinhos Mordedores Sortidos</t>
+  </si>
+  <si>
+    <t>246 - Chocalho ursinho com LED</t>
+  </si>
+  <si>
+    <t>247 - Chocalho mordedor com formato de ursinho</t>
+  </si>
+  <si>
+    <t>248 - Brinquedo de Borracha - Mamãe pata e seus patinhos</t>
+  </si>
+  <si>
+    <t>249 - Brinquedo de Borracha - Mamãe sapa e seus sapinhos</t>
+  </si>
+  <si>
+    <t>250 - pézinho baby rosa e azul</t>
+  </si>
+  <si>
+    <t>177 - cozinha infantil classica paris</t>
+  </si>
+  <si>
+    <t>1 - Anda Cavalinho com Som (azul) - Xalingo</t>
+  </si>
+  <si>
+    <t>2 - Balanço de ursinho Infantil Xalingo sem Gancho com Cinto</t>
+  </si>
+  <si>
+    <t>3 - Balanço fofossauro 3 Em 1 encosto regulável Xalingo</t>
+  </si>
+  <si>
+    <t>4 - Balanço Infantil 3 Em 1 Barra Proteção Unicórnio Xalingo</t>
+  </si>
+  <si>
+    <t>5 - Balanço Infantil Borboletinha Trava Cordas Reforçado</t>
+  </si>
+  <si>
+    <t>6 - Balanço infantil Mickey Mouse Xalingo 19798 cor vermelho e preto</t>
+  </si>
+  <si>
+    <t>7 - Balanço infantil Minnie Mouse 3 em 1 rosa playground Xalingo</t>
+  </si>
+  <si>
+    <t>8 - Balanço Infantil Para Bebê  E Criança - Playground - Diversão</t>
+  </si>
+  <si>
+    <t>9 - Balanço Patrulha Canina Encosto Cinto Infantil Bebê Até 36m</t>
+  </si>
+  <si>
+    <t>10 - Balanço Spider Man Super Hero Adventure Xalingo Homem Aranha</t>
+  </si>
+  <si>
+    <t>11 - banner arvore da vida site</t>
+  </si>
+  <si>
+    <t>12 - banner cardapio da semana site</t>
+  </si>
+  <si>
+    <t>13 - banner celula vegetal e animal site</t>
+  </si>
+  <si>
+    <t>14 - banner plantas site</t>
+  </si>
+  <si>
+    <t>15 - banner tabuada adição site</t>
+  </si>
+  <si>
+    <t>16 - banner ajudante do dia site</t>
+  </si>
+  <si>
+    <t>17 - banner alfabeto</t>
+  </si>
+  <si>
+    <t>18 - banner animais vertebrados aves site</t>
+  </si>
+  <si>
+    <t>19 - banner animais vertebrados anfibios site</t>
+  </si>
+  <si>
+    <t>20 - banner animais vertebrados mamiferos site</t>
+  </si>
+  <si>
+    <t>21 - banner animais vertebrados peixes site</t>
+  </si>
+  <si>
+    <t>22 -banner aniversariante do mes site</t>
+  </si>
+  <si>
+    <t>23 - banner aprenda a lavar a mao corretamente</t>
+  </si>
+  <si>
+    <t>24 - banner bioma do brasil site</t>
+  </si>
+  <si>
+    <t>25 - banner boa convivencia site</t>
+  </si>
+  <si>
+    <t>26 - banner calendario site</t>
+  </si>
+  <si>
+    <t>27 - banner cantinho da leitura site</t>
+  </si>
+  <si>
+    <t>28 - banner chamadinha site</t>
+  </si>
+  <si>
+    <t>29 - banner ciclo da agua</t>
+  </si>
+  <si>
+    <t>30 - banner clima do brasil</t>
+  </si>
+  <si>
+    <t>31 - banner clima site</t>
+  </si>
+  <si>
+    <t>32 - banner combinados da turma</t>
+  </si>
+  <si>
+    <t>33 - banner diga nao ao bulling site</t>
+  </si>
+  <si>
+    <t>34 - banner divisão site</t>
+  </si>
+  <si>
+    <t>35 - BANNER ESQUELETO HUMANO</t>
+  </si>
+  <si>
+    <t>36 - banner formas  geometricas</t>
+  </si>
+  <si>
+    <t>37 - banner formas geometricas completa</t>
+  </si>
+  <si>
+    <t>38 - banner fraçao site</t>
+  </si>
+  <si>
+    <t>39 - banner generos textuais site</t>
+  </si>
+  <si>
+    <t>40 - banner geografia</t>
+  </si>
+  <si>
+    <t>41 - banner hino nacional brasileiro site</t>
+  </si>
+  <si>
+    <t>42 - banner mapa de são paulo site</t>
+  </si>
+  <si>
+    <t>43 - banner mapa do brasil</t>
+  </si>
+  <si>
+    <t>44 - banner mapa economico brasileiro site</t>
+  </si>
+  <si>
+    <t>45 - banner mapa mundi site</t>
+  </si>
+  <si>
+    <t>46 - banner mapa municipal de sao paulo site</t>
+  </si>
+  <si>
+    <t>47 - Banner Meses do Ano - 80 x 120 cm (L x A)</t>
+  </si>
+  <si>
+    <t>48 - banner montagem silabica  site</t>
+  </si>
+  <si>
+    <t>49 - banner numerais de 0 a 100 site</t>
+  </si>
+  <si>
+    <t>50 - banner numerais e escritas</t>
+  </si>
+  <si>
+    <t>51 - banner numeros romanos site</t>
+  </si>
+  <si>
+    <t>52 - Banner ou painel corpo humano material gratuito</t>
+  </si>
+  <si>
+    <t>53 - banner palavrinhas magicas site</t>
+  </si>
+  <si>
+    <t>54 - banner pedagogico animais vertebrados répteis site</t>
+  </si>
+  <si>
+    <t>55 - banner personalizado conforme a solicitação do cliente site</t>
+  </si>
+  <si>
+    <t>56 - banner presidentes do brasil site</t>
+  </si>
+  <si>
+    <t>57 - banner regras do porque site</t>
+  </si>
+  <si>
+    <t>58 - banner regras matematica</t>
+  </si>
+  <si>
+    <t>59 - banner silabario simples site</t>
+  </si>
+  <si>
+    <t>60 - banner sinais de pontuacao site</t>
+  </si>
+  <si>
+    <t>70 - banner sistema muscular site</t>
+  </si>
+  <si>
+    <t>71 - banner subtracao site</t>
+  </si>
+  <si>
+    <t>72 - banner tabela periodica</t>
+  </si>
+  <si>
+    <t>73 - banner tabuada site</t>
+  </si>
+  <si>
+    <t>74 - banner texto narrativo site</t>
+  </si>
+  <si>
+    <t>75 - banner vogais e consuantes</t>
+  </si>
+  <si>
+    <t>76 - banner vogais site</t>
+  </si>
+  <si>
+    <t>77 - Baú Infantil Hipo Roxo - Xalingo</t>
+  </si>
+  <si>
+    <t>78 - Gangorra Individual - Pluto Xalingo</t>
+  </si>
+  <si>
+    <t>79 - Brinquedo Infantil Minnie Com Empurrador E Proteção Xalingo</t>
+  </si>
+  <si>
+    <t>80 - Caixa de Areia Infantil Estrela do Mar Vermelha Xalingo</t>
+  </si>
+  <si>
+    <t>81 - Carrinho Infantil Xalingo Cozy Couple Little Tikes Ref.59110 Cor Vermelho</t>
+  </si>
+  <si>
+    <t>82 - Carrinho Velotrol Infantil Criança Bebê COM empurrador</t>
+  </si>
+  <si>
+    <t>83 -Carrossel Gira Pato Xalingo</t>
+  </si>
+  <si>
+    <t>84 - Cercadinho Infantil Colorido Xalingo</t>
+  </si>
+  <si>
+    <t>85 - Escorregador com Balanço Xalingo</t>
+  </si>
+  <si>
+    <t>86 - Escorregador Infantil Desmontável Vermelho Xalingo</t>
+  </si>
+  <si>
+    <t>87 - Escorregador Infantil Master Laranja Xalingo</t>
+  </si>
+  <si>
+    <t>88 - Gangorra 2 Lugares Disney</t>
+  </si>
+  <si>
+    <t>89 - Gangorra Anda Cavalinho Pocoto Vermelho Xalingo</t>
+  </si>
+  <si>
+    <t>90 - Gangorra Bidu Turma Da Mônica Xalingo</t>
+  </si>
+  <si>
+    <t>91 - Gangorra Cavalinho Balanço Infantil Criança Azul - Xalingo</t>
+  </si>
+  <si>
+    <t>92 - Gangorra Cavalinho Infantil Nhoca</t>
+  </si>
+  <si>
+    <t>93 - Gangorra Dinossauro duplo</t>
+  </si>
+  <si>
+    <t>94 - Gangorra Infantil Dupla Fofossauros Xalingo</t>
+  </si>
+  <si>
+    <t>95 - Gangorra Infantil Minhoca Verde Xalingo</t>
+  </si>
+  <si>
+    <t>96 - Gangorra Infantil Mini Moto Parquinhos Xalingo Cor Laranja</t>
+  </si>
+  <si>
+    <t>97 - Gangorra Infantil Scooter Do Mickey Disney Xalingo - 1874.3 Cor Vermelho</t>
+  </si>
+  <si>
+    <t>98 - Gangorra Infantil Tigrão Disney Baby - Xalingo</t>
+  </si>
+  <si>
+    <t>99 - Imagem Kits Profissões</t>
+  </si>
+  <si>
+    <t>100 - kit 4 banners infanto-juvenil</t>
+  </si>
+  <si>
+    <t>101 - Mesa Sirizinho Xalingo Com Bancos Acoplados</t>
+  </si>
+  <si>
+    <t>102 - Motoquinha Triciclo Infantil Com Pedal Tigrão Xalingo</t>
+  </si>
+  <si>
+    <t>103 - Motoquinha Triciclo Infantil Joaninha Xalingo Com Pedal</t>
+  </si>
+  <si>
+    <t>104 - New Big Playground</t>
+  </si>
+  <si>
+    <t>105 - Play Dog House - Xalingo</t>
+  </si>
+  <si>
+    <t>106 - Playground Barco Pirata Little Tikes Xalingo</t>
+  </si>
+  <si>
+    <t>107 - Playground Casinha Infantil Cabana De Campo Little Tikes</t>
+  </si>
+  <si>
+    <t>108 - Playground Castelo Medieval Xalingo</t>
+  </si>
+  <si>
+    <t>109 - Playground Infantil Xalingo Dupla Diversão Little Tikes</t>
+  </si>
+  <si>
+    <t>110 - Playground Parquinho De Atividades</t>
+  </si>
+  <si>
+    <t>111 - Playground Trenzinho Da Alegria Xalingo</t>
+  </si>
+  <si>
+    <t>112 - Rede De Dormir Infantil Berço</t>
+  </si>
+  <si>
+    <t>113 - Triciclo Motoca Infantil Fofossauros Verde Laranja Xalingo</t>
+  </si>
+  <si>
+    <t>114 - Triciclo Peixinho Com Empurrador cestinha Xalingo</t>
+  </si>
+  <si>
+    <t>116 - Triciclo Blue Race 3 Em 1 Xalingo Carrinho De Passeio</t>
+  </si>
+  <si>
+    <t>117 - Triciclo Cachorrinho Empurrador Proteção E Cestinha Xalingo</t>
+  </si>
+  <si>
+    <t>118 - Triciclo Com Empurrador E Proteção Mickey Xalingo Vermelho</t>
+  </si>
+  <si>
+    <t>119 - Triciclo Fox Racer - Xalingo</t>
   </si>
 </sst>
 </file>
@@ -935,7 +1196,7 @@
   <dimension ref="A1:C251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,10 +1222,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -972,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -981,7 +1242,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -990,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -999,7 +1260,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1008,7 +1269,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>141</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1017,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>142</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -1026,7 +1287,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1035,7 +1296,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -1044,7 +1305,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -1053,7 +1314,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>14</v>
+        <v>146</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -1062,7 +1323,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>15</v>
+        <v>147</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -1071,7 +1332,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>16</v>
+        <v>148</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -1080,7 +1341,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -1089,7 +1350,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -1098,7 +1359,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -1107,7 +1368,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -1116,7 +1377,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -1125,7 +1386,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>22</v>
+        <v>154</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -1134,7 +1395,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -1143,7 +1404,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>24</v>
+        <v>156</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -1152,7 +1413,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>157</v>
       </c>
       <c r="C23" s="2"/>
     </row>
@@ -1161,7 +1422,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="C24" s="2"/>
     </row>
@@ -1170,7 +1431,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>27</v>
+        <v>159</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -1179,7 +1440,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>28</v>
+        <v>160</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -1188,7 +1449,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>29</v>
+        <v>161</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -1197,7 +1458,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>30</v>
+        <v>162</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -1206,7 +1467,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -1215,7 +1476,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>32</v>
+        <v>164</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -1224,7 +1485,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -1233,7 +1494,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="C32" s="2"/>
     </row>
@@ -1242,7 +1503,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>35</v>
+        <v>167</v>
       </c>
       <c r="C33" s="2"/>
     </row>
@@ -1251,7 +1512,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>36</v>
+        <v>168</v>
       </c>
       <c r="C34" s="2"/>
     </row>
@@ -1260,7 +1521,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>37</v>
+        <v>169</v>
       </c>
       <c r="C35" s="2"/>
     </row>
@@ -1269,7 +1530,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="C36" s="2"/>
     </row>
@@ -1278,7 +1539,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>39</v>
+        <v>171</v>
       </c>
       <c r="C37" s="2"/>
     </row>
@@ -1287,7 +1548,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="C38" s="2"/>
     </row>
@@ -1296,7 +1557,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>41</v>
+        <v>173</v>
       </c>
       <c r="C39" s="2"/>
     </row>
@@ -1305,7 +1566,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>42</v>
+        <v>174</v>
       </c>
       <c r="C40" s="2"/>
     </row>
@@ -1314,7 +1575,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>43</v>
+        <v>175</v>
       </c>
       <c r="C41" s="2"/>
     </row>
@@ -1323,7 +1584,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="C42" s="2"/>
     </row>
@@ -1332,7 +1593,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>45</v>
+        <v>177</v>
       </c>
       <c r="C43" s="2"/>
     </row>
@@ -1341,7 +1602,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>46</v>
+        <v>178</v>
       </c>
       <c r="C44" s="2"/>
     </row>
@@ -1350,7 +1611,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>47</v>
+        <v>179</v>
       </c>
       <c r="C45" s="2"/>
     </row>
@@ -1359,7 +1620,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="C46" s="2"/>
     </row>
@@ -1368,7 +1629,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>49</v>
+        <v>181</v>
       </c>
       <c r="C47" s="2"/>
     </row>
@@ -1377,7 +1638,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>50</v>
+        <v>182</v>
       </c>
       <c r="C48" s="2"/>
     </row>
@@ -1386,7 +1647,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>51</v>
+        <v>183</v>
       </c>
       <c r="C49" s="2"/>
     </row>
@@ -1395,7 +1656,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="C50" s="2"/>
     </row>
@@ -1404,7 +1665,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>53</v>
+        <v>185</v>
       </c>
       <c r="C51" s="2"/>
     </row>
@@ -1413,7 +1674,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>54</v>
+        <v>186</v>
       </c>
       <c r="C52" s="2"/>
     </row>
@@ -1422,7 +1683,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>55</v>
+        <v>187</v>
       </c>
       <c r="C53" s="2"/>
     </row>
@@ -1431,7 +1692,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>56</v>
+        <v>188</v>
       </c>
       <c r="C54" s="2"/>
     </row>
@@ -1440,7 +1701,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>57</v>
+        <v>189</v>
       </c>
       <c r="C55" s="2"/>
     </row>
@@ -1449,7 +1710,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="C56" s="2"/>
     </row>
@@ -1458,7 +1719,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>59</v>
+        <v>191</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -1467,7 +1728,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>60</v>
+        <v>192</v>
       </c>
       <c r="C58" s="2"/>
     </row>
@@ -1476,7 +1737,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>61</v>
+        <v>193</v>
       </c>
       <c r="C59" s="2"/>
     </row>
@@ -1485,7 +1746,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="C60" s="2"/>
     </row>
@@ -1494,7 +1755,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>63</v>
+        <v>195</v>
       </c>
       <c r="C61" s="2"/>
     </row>
@@ -1502,71 +1763,62 @@
       <c r="A62" s="1">
         <v>61</v>
       </c>
-      <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65" s="2"/>
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
-      <c r="B67" s="2"/>
       <c r="C67" s="2"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B68" s="2"/>
       <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="B69" s="2"/>
       <c r="C69" s="2"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70" s="2"/>
       <c r="C70" s="2"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>64</v>
+      <c r="B71" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="C71" s="2"/>
     </row>
@@ -1574,8 +1826,8 @@
       <c r="A72" s="1">
         <v>71</v>
       </c>
-      <c r="B72" s="6" t="s">
-        <v>65</v>
+      <c r="B72" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="C72" s="2"/>
     </row>
@@ -1583,8 +1835,8 @@
       <c r="A73" s="1">
         <v>72</v>
       </c>
-      <c r="B73" s="6" t="s">
-        <v>66</v>
+      <c r="B73" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="C73" s="2"/>
     </row>
@@ -1592,8 +1844,8 @@
       <c r="A74" s="1">
         <v>73</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>67</v>
+      <c r="B74" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="C74" s="2"/>
     </row>
@@ -1601,8 +1853,8 @@
       <c r="A75" s="1">
         <v>74</v>
       </c>
-      <c r="B75" s="6" t="s">
-        <v>68</v>
+      <c r="B75" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="C75" s="2"/>
     </row>
@@ -1610,8 +1862,8 @@
       <c r="A76" s="1">
         <v>75</v>
       </c>
-      <c r="B76" s="6" t="s">
-        <v>69</v>
+      <c r="B76" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="C76" s="2"/>
     </row>
@@ -1619,8 +1871,8 @@
       <c r="A77" s="1">
         <v>76</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>70</v>
+      <c r="B77" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="C77" s="2"/>
     </row>
@@ -1628,8 +1880,8 @@
       <c r="A78" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="6" t="s">
-        <v>71</v>
+      <c r="B78" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="C78" s="2"/>
     </row>
@@ -1637,8 +1889,8 @@
       <c r="A79" s="1">
         <v>78</v>
       </c>
-      <c r="B79" s="6" t="s">
-        <v>72</v>
+      <c r="B79" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="C79" s="2"/>
     </row>
@@ -1647,7 +1899,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>73</v>
+        <v>205</v>
       </c>
       <c r="C80" s="2"/>
     </row>
@@ -1656,7 +1908,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>74</v>
+        <v>206</v>
       </c>
       <c r="C81" s="2"/>
     </row>
@@ -1665,7 +1917,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>75</v>
+        <v>207</v>
       </c>
       <c r="C82" s="2"/>
     </row>
@@ -1674,7 +1926,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>76</v>
+        <v>208</v>
       </c>
       <c r="C83" s="2"/>
     </row>
@@ -1683,7 +1935,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>77</v>
+        <v>209</v>
       </c>
       <c r="C84" s="2"/>
     </row>
@@ -1692,7 +1944,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>78</v>
+        <v>210</v>
       </c>
       <c r="C85" s="2"/>
     </row>
@@ -1701,7 +1953,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>79</v>
+        <v>211</v>
       </c>
       <c r="C86" s="2"/>
     </row>
@@ -1710,7 +1962,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>80</v>
+        <v>212</v>
       </c>
       <c r="C87" s="2"/>
     </row>
@@ -1719,7 +1971,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>81</v>
+        <v>213</v>
       </c>
       <c r="C88" s="2"/>
     </row>
@@ -1728,7 +1980,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>82</v>
+        <v>214</v>
       </c>
       <c r="C89" s="2"/>
     </row>
@@ -1737,7 +1989,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>83</v>
+        <v>215</v>
       </c>
       <c r="C90" s="2"/>
     </row>
@@ -1746,7 +1998,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>84</v>
+        <v>216</v>
       </c>
       <c r="C91" s="2"/>
     </row>
@@ -1755,7 +2007,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>85</v>
+        <v>217</v>
       </c>
       <c r="C92" s="2"/>
     </row>
@@ -1764,7 +2016,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>86</v>
+        <v>218</v>
       </c>
       <c r="C93" s="2"/>
     </row>
@@ -1773,7 +2025,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>87</v>
+        <v>219</v>
       </c>
       <c r="C94" s="2"/>
     </row>
@@ -1782,7 +2034,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>88</v>
+        <v>220</v>
       </c>
       <c r="C95" s="2"/>
     </row>
@@ -1791,7 +2043,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>89</v>
+        <v>221</v>
       </c>
       <c r="C96" s="2"/>
     </row>
@@ -1800,7 +2052,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="C97" s="2"/>
     </row>
@@ -1809,7 +2061,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>91</v>
+        <v>223</v>
       </c>
       <c r="C98" s="2"/>
     </row>
@@ -1818,7 +2070,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>92</v>
+        <v>224</v>
       </c>
       <c r="C99" s="2"/>
     </row>
@@ -1827,7 +2079,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>93</v>
+        <v>225</v>
       </c>
       <c r="C100" s="2"/>
     </row>
@@ -1836,7 +2088,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>94</v>
+        <v>226</v>
       </c>
       <c r="C101" s="2"/>
     </row>
@@ -1845,7 +2097,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>95</v>
+        <v>227</v>
       </c>
       <c r="C102" s="2"/>
     </row>
@@ -1854,7 +2106,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>96</v>
+        <v>228</v>
       </c>
       <c r="C103" s="2"/>
     </row>
@@ -1863,7 +2115,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>97</v>
+        <v>229</v>
       </c>
       <c r="C104" s="2"/>
     </row>
@@ -1872,7 +2124,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>98</v>
+        <v>230</v>
       </c>
       <c r="C105" s="2"/>
     </row>
@@ -1881,7 +2133,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>99</v>
+        <v>231</v>
       </c>
       <c r="C106" s="2"/>
     </row>
@@ -1890,7 +2142,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>100</v>
+        <v>232</v>
       </c>
       <c r="C107" s="2"/>
     </row>
@@ -1899,7 +2151,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>101</v>
+        <v>233</v>
       </c>
       <c r="C108" s="2"/>
     </row>
@@ -1908,7 +2160,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>102</v>
+        <v>234</v>
       </c>
       <c r="C109" s="2"/>
     </row>
@@ -1917,7 +2169,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>103</v>
+        <v>235</v>
       </c>
       <c r="C110" s="2"/>
     </row>
@@ -1926,7 +2178,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>104</v>
+        <v>236</v>
       </c>
       <c r="C111" s="2"/>
     </row>
@@ -1935,7 +2187,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>105</v>
+        <v>237</v>
       </c>
       <c r="C112" s="2"/>
     </row>
@@ -1944,7 +2196,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>106</v>
+        <v>238</v>
       </c>
       <c r="C113" s="2"/>
     </row>
@@ -1953,7 +2205,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>107</v>
+        <v>239</v>
       </c>
       <c r="C114" s="2"/>
     </row>
@@ -1962,7 +2214,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>108</v>
+        <v>240</v>
       </c>
       <c r="C115" s="2"/>
     </row>
@@ -1971,7 +2223,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>109</v>
+        <v>4</v>
       </c>
       <c r="C116" s="2"/>
     </row>
@@ -1980,7 +2232,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>110</v>
+        <v>241</v>
       </c>
       <c r="C117" s="2"/>
     </row>
@@ -1989,7 +2241,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>111</v>
+        <v>242</v>
       </c>
       <c r="C118" s="2"/>
     </row>
@@ -1998,7 +2250,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>112</v>
+        <v>243</v>
       </c>
       <c r="C119" s="2"/>
     </row>
@@ -2007,7 +2259,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>113</v>
+        <v>244</v>
       </c>
       <c r="C120" s="2"/>
     </row>
@@ -2016,7 +2268,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="C121" s="2"/>
     </row>
@@ -2025,7 +2277,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C122" s="2"/>
     </row>
@@ -2034,7 +2286,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="C123" s="2"/>
     </row>
@@ -2043,7 +2295,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="C124" s="2"/>
     </row>
@@ -2052,7 +2304,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="C125" s="2"/>
     </row>
@@ -2061,7 +2313,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
       <c r="C126" s="2"/>
     </row>
@@ -2070,7 +2322,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="C127" s="2"/>
     </row>
@@ -2079,7 +2331,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>121</v>
+        <v>12</v>
       </c>
       <c r="C128" s="2"/>
     </row>
@@ -2088,7 +2340,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="C129" s="2"/>
     </row>
@@ -2097,7 +2349,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="C130" s="2"/>
     </row>
@@ -2106,7 +2358,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="C131" s="2"/>
     </row>
@@ -2115,7 +2367,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="C132" s="2"/>
     </row>
@@ -2124,7 +2376,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>126</v>
+        <v>17</v>
       </c>
       <c r="C133" s="2"/>
     </row>
@@ -2133,7 +2385,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="C134" s="2"/>
     </row>
@@ -2142,7 +2394,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="C135" s="2"/>
     </row>
@@ -2151,7 +2403,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="C136" s="2"/>
     </row>
@@ -2160,7 +2412,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>130</v>
+        <v>21</v>
       </c>
       <c r="C137" s="2"/>
     </row>
@@ -2169,7 +2421,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="C138" s="2"/>
     </row>
@@ -2178,7 +2430,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="C139" s="2"/>
     </row>
@@ -2187,7 +2439,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="C140" s="2"/>
     </row>
@@ -2196,7 +2448,7 @@
         <v>140</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="C141" s="2"/>
     </row>
@@ -2205,7 +2457,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
       <c r="C142" s="2"/>
     </row>
@@ -2214,7 +2466,7 @@
         <v>142</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C143" s="2"/>
     </row>
@@ -2223,7 +2475,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
       <c r="C144" s="2"/>
     </row>
@@ -2232,7 +2484,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>138</v>
+        <v>29</v>
       </c>
       <c r="C145" s="2"/>
     </row>
@@ -2241,7 +2493,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="C146" s="2"/>
     </row>
@@ -2250,7 +2502,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
       <c r="C147" s="2"/>
     </row>
@@ -2259,7 +2511,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="C148" s="2"/>
     </row>
@@ -2268,7 +2520,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
       <c r="C149" s="2"/>
     </row>
@@ -2277,7 +2529,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>143</v>
+        <v>34</v>
       </c>
       <c r="C150" s="2"/>
     </row>
@@ -2286,7 +2538,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>144</v>
+        <v>35</v>
       </c>
       <c r="C151" s="2"/>
     </row>
@@ -2295,7 +2547,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="C152" s="2"/>
     </row>
@@ -2304,7 +2556,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>146</v>
+        <v>37</v>
       </c>
       <c r="C153" s="2"/>
     </row>
@@ -2313,7 +2565,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="C154" s="2"/>
     </row>
@@ -2322,7 +2574,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="C155" s="2"/>
     </row>
@@ -2331,7 +2583,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>149</v>
+        <v>40</v>
       </c>
       <c r="C156" s="2"/>
     </row>
@@ -2340,7 +2592,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="6" t="s">
-        <v>150</v>
+        <v>41</v>
       </c>
       <c r="C157" s="2"/>
     </row>
@@ -2349,7 +2601,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>151</v>
+        <v>42</v>
       </c>
       <c r="C158" s="2"/>
     </row>
@@ -2358,7 +2610,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="6" t="s">
-        <v>152</v>
+        <v>43</v>
       </c>
       <c r="C159" s="2"/>
     </row>
@@ -2367,7 +2619,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>153</v>
+        <v>44</v>
       </c>
       <c r="C160" s="2"/>
     </row>
@@ -2376,7 +2628,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="C161" s="2"/>
     </row>
@@ -2385,7 +2637,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>155</v>
+        <v>46</v>
       </c>
       <c r="C162" s="2"/>
     </row>
@@ -2394,7 +2646,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>156</v>
+        <v>47</v>
       </c>
       <c r="C163" s="2"/>
     </row>
@@ -2403,7 +2655,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>157</v>
+        <v>48</v>
       </c>
       <c r="C164" s="2"/>
     </row>
@@ -2411,609 +2663,783 @@
       <c r="A165" s="1">
         <v>164</v>
       </c>
-      <c r="B165" s="6"/>
+      <c r="B165" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="C165" s="2"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
-      <c r="B166" s="6"/>
+      <c r="B166" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="C166" s="2"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
-      <c r="B167" s="6"/>
+      <c r="B167" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="C167" s="2"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
-      <c r="B168" s="6"/>
+      <c r="B168" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="C168" s="2"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
-      <c r="B169" s="6"/>
+      <c r="B169" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="C169" s="2"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
-      <c r="B170" s="6"/>
+      <c r="B170" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="C170" s="2"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
-      <c r="B171" s="6"/>
+      <c r="B171" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="C171" s="2"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
-      <c r="B172" s="6"/>
+      <c r="B172" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="C172" s="2"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
-      <c r="B173" s="6"/>
+      <c r="B173" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="C173" s="2"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
-      <c r="B174" s="6"/>
+      <c r="B174" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="C174" s="2"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
-      <c r="B175" s="6"/>
+      <c r="B175" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="C175" s="2"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
-      <c r="B176" s="6"/>
+      <c r="B176" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="C176" s="2"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
-      <c r="B177" s="6"/>
+      <c r="B177" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="C177" s="2"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
-      <c r="B178" s="6"/>
+      <c r="B178" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="C178" s="2"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
-      <c r="B179" s="6"/>
+      <c r="B179" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="C179" s="2"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
-      <c r="B180" s="6"/>
+      <c r="B180" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="C180" s="2"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
-      <c r="B181" s="6"/>
+      <c r="B181" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="C181" s="2"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
-      <c r="B182" s="6"/>
+      <c r="B182" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="C182" s="2"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
-      <c r="B183" s="6"/>
+      <c r="B183" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="C183" s="2"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
-      <c r="B184" s="6"/>
+      <c r="B184" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="C184" s="2"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
-      <c r="B185" s="6"/>
+      <c r="B185" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="C185" s="2"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
-      <c r="B186" s="6"/>
+      <c r="B186" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="C186" s="2"/>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
-      <c r="B187" s="6"/>
+      <c r="B187" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="C187" s="2"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
-      <c r="B188" s="6"/>
+      <c r="B188" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="C188" s="2"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
-      <c r="B189" s="6"/>
+      <c r="B189" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="C189" s="2"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
-      <c r="B190" s="6"/>
+      <c r="B190" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="C190" s="2"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
-      <c r="B191" s="6"/>
+      <c r="B191" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="C191" s="2"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
-      <c r="B192" s="6"/>
+      <c r="B192" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="C192" s="2"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
-      <c r="B193" s="6"/>
+      <c r="B193" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="C193" s="2"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
-      <c r="B194" s="6"/>
+      <c r="B194" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="C194" s="2"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
-      <c r="B195" s="6"/>
+      <c r="B195" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="C195" s="2"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
-      <c r="B196" s="6"/>
+      <c r="B196" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="C196" s="2"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
-      <c r="B197" s="6"/>
+      <c r="B197" s="6" t="s">
+        <v>80</v>
+      </c>
       <c r="C197" s="2"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
-      <c r="B198" s="6"/>
+      <c r="B198" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="C198" s="2"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
-      <c r="B199" s="6"/>
+      <c r="B199" s="6" t="s">
+        <v>82</v>
+      </c>
       <c r="C199" s="2"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
-      <c r="B200" s="6"/>
+      <c r="B200" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="C200" s="2"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
-      <c r="B201" s="6"/>
+      <c r="B201" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="C201" s="2"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
-      <c r="B202" s="6"/>
+      <c r="B202" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="C202" s="2"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
-      <c r="B203" s="6"/>
+      <c r="B203" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="C203" s="2"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
-      <c r="B204" s="6"/>
+      <c r="B204" s="6" t="s">
+        <v>87</v>
+      </c>
       <c r="C204" s="2"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
-      <c r="B205" s="6"/>
+      <c r="B205" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="C205" s="2"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
-      <c r="B206" s="6"/>
+      <c r="B206" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="C206" s="2"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
-      <c r="B207" s="6"/>
+      <c r="B207" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="C207" s="2"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
-      <c r="B208" s="6"/>
+      <c r="B208" s="6" t="s">
+        <v>91</v>
+      </c>
       <c r="C208" s="2"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
-      <c r="B209" s="6"/>
+      <c r="B209" s="6" t="s">
+        <v>92</v>
+      </c>
       <c r="C209" s="2"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
-      <c r="B210" s="6"/>
+      <c r="B210" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="C210" s="2"/>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
-      <c r="B211" s="6"/>
+      <c r="B211" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C211" s="2"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
-      <c r="B212" s="6"/>
+      <c r="B212" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="C212" s="2"/>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
-      <c r="B213" s="6"/>
+      <c r="B213" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="C213" s="2"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
-      <c r="B214" s="6"/>
+      <c r="B214" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="C214" s="2"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
-      <c r="B215" s="6"/>
+      <c r="B215" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="C215" s="2"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
-      <c r="B216" s="6"/>
+      <c r="B216" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="C216" s="2"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
-      <c r="B217" s="6"/>
+      <c r="B217" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="C217" s="2"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
-      <c r="B218" s="6"/>
+      <c r="B218" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="C218" s="2"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
-      <c r="B219" s="6"/>
+      <c r="B219" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="C219" s="2"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
-      <c r="B220" s="6"/>
+      <c r="B220" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="C220" s="2"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
-      <c r="B221" s="6"/>
+      <c r="B221" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="C221" s="2"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
-      <c r="B222" s="6"/>
+      <c r="B222" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="C222" s="2"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
-      <c r="B223" s="6"/>
+      <c r="B223" s="6" t="s">
+        <v>106</v>
+      </c>
       <c r="C223" s="2"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
-      <c r="B224" s="6"/>
+      <c r="B224" s="6" t="s">
+        <v>107</v>
+      </c>
       <c r="C224" s="2"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
-      <c r="B225" s="6"/>
+      <c r="B225" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="C225" s="2"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
-      <c r="B226" s="6"/>
+      <c r="B226" s="6" t="s">
+        <v>109</v>
+      </c>
       <c r="C226" s="2"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
-      <c r="B227" s="6"/>
+      <c r="B227" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="C227" s="2"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
-      <c r="B228" s="6"/>
+      <c r="B228" s="6" t="s">
+        <v>111</v>
+      </c>
       <c r="C228" s="2"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>228</v>
       </c>
-      <c r="B229" s="6"/>
+      <c r="B229" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="C229" s="2"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
-      <c r="B230" s="6"/>
+      <c r="B230" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="C230" s="2"/>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>230</v>
       </c>
-      <c r="B231" s="6"/>
+      <c r="B231" s="6" t="s">
+        <v>114</v>
+      </c>
       <c r="C231" s="2"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>231</v>
       </c>
-      <c r="B232" s="6"/>
+      <c r="B232" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="C232" s="2"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>232</v>
       </c>
-      <c r="B233" s="6"/>
+      <c r="B233" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="C233" s="2"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>233</v>
       </c>
-      <c r="B234" s="6"/>
+      <c r="B234" s="6" t="s">
+        <v>117</v>
+      </c>
       <c r="C234" s="2"/>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>234</v>
       </c>
-      <c r="B235" s="6"/>
+      <c r="B235" s="6" t="s">
+        <v>118</v>
+      </c>
       <c r="C235" s="2"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>235</v>
       </c>
-      <c r="B236" s="6"/>
+      <c r="B236" s="6" t="s">
+        <v>119</v>
+      </c>
       <c r="C236" s="2"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>236</v>
       </c>
-      <c r="B237" s="6"/>
+      <c r="B237" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="C237" s="2"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>237</v>
       </c>
-      <c r="B238" s="6"/>
+      <c r="B238" s="6" t="s">
+        <v>121</v>
+      </c>
       <c r="C238" s="2"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>238</v>
       </c>
-      <c r="B239" s="6"/>
+      <c r="B239" s="6" t="s">
+        <v>122</v>
+      </c>
       <c r="C239" s="2"/>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>239</v>
       </c>
-      <c r="B240" s="6"/>
+      <c r="B240" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="C240" s="2"/>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>240</v>
       </c>
-      <c r="B241" s="6"/>
+      <c r="B241" s="6" t="s">
+        <v>124</v>
+      </c>
       <c r="C241" s="2"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>241</v>
       </c>
-      <c r="B242" s="6"/>
+      <c r="B242" s="6" t="s">
+        <v>125</v>
+      </c>
       <c r="C242" s="2"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>242</v>
       </c>
-      <c r="B243" s="6"/>
+      <c r="B243" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="C243" s="2"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>243</v>
       </c>
-      <c r="B244" s="6"/>
+      <c r="B244" s="6" t="s">
+        <v>127</v>
+      </c>
       <c r="C244" s="2"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>244</v>
       </c>
-      <c r="B245" s="6"/>
+      <c r="B245" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="C245" s="2"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>245</v>
       </c>
-      <c r="B246" s="6"/>
+      <c r="B246" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="C246" s="2"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>246</v>
       </c>
-      <c r="B247" s="6"/>
+      <c r="B247" s="6" t="s">
+        <v>130</v>
+      </c>
       <c r="C247" s="2"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>247</v>
       </c>
-      <c r="B248" s="6"/>
+      <c r="B248" s="6" t="s">
+        <v>131</v>
+      </c>
       <c r="C248" s="2"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>248</v>
       </c>
-      <c r="B249" s="6"/>
+      <c r="B249" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="C249" s="2"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>249</v>
       </c>
-      <c r="B250" s="6"/>
+      <c r="B250" s="6" t="s">
+        <v>133</v>
+      </c>
       <c r="C250" s="2"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>250</v>
       </c>
-      <c r="B251" s="6"/>
+      <c r="B251" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="C251" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificação da planilha - todos as imagens registradas
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.macedo\OneDrive - Sinergy RH\Desktop\Coding\Anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E91470-C176-459E-9A46-6D9F2261B864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB020935-AEEF-460C-823F-37C66D06CF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="497">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -74,90 +74,18 @@
     <t>VENTILADORES</t>
   </si>
   <si>
-    <t>cozinha infantil classica paris</t>
-  </si>
-  <si>
     <t>Cone</t>
   </si>
   <si>
-    <t>Piso molhado</t>
-  </si>
-  <si>
-    <t>Dispenser para copo de água e café</t>
-  </si>
-  <si>
     <t>Dispensers1</t>
   </si>
   <si>
     <t>Dispensers2</t>
   </si>
   <si>
-    <t>Fita demarcação</t>
-  </si>
-  <si>
-    <t>Canecas Personalizadas</t>
-  </si>
-  <si>
-    <t>Garrafa Personalizada</t>
-  </si>
-  <si>
     <t>Necessaires</t>
   </si>
   <si>
-    <t>Tacas Personalizadas</t>
-  </si>
-  <si>
-    <t>Pedestal unitario e em corrente plastica</t>
-  </si>
-  <si>
-    <t>Suporte para copos de água e café</t>
-  </si>
-  <si>
-    <t>Tapete Sanitizante</t>
-  </si>
-  <si>
-    <t>Totens para alcool em gel</t>
-  </si>
-  <si>
-    <t>Totem dispenser de alcool em gel e termometro por sensor</t>
-  </si>
-  <si>
-    <t>boneca 1</t>
-  </si>
-  <si>
-    <t>boneca 2</t>
-  </si>
-  <si>
-    <t>boneca 3</t>
-  </si>
-  <si>
-    <t>boneca 4</t>
-  </si>
-  <si>
-    <t>boneca 5</t>
-  </si>
-  <si>
-    <t>boneca 6</t>
-  </si>
-  <si>
-    <t>boneca 7</t>
-  </si>
-  <si>
-    <t>cozinha infantil retro branca</t>
-  </si>
-  <si>
-    <t>cozinha infantil retro noruega</t>
-  </si>
-  <si>
-    <t>cozinha infantil retro verde agua</t>
-  </si>
-  <si>
-    <t>cozinha infantil retro vermelha</t>
-  </si>
-  <si>
-    <t>cozinha infantil retro vintage</t>
-  </si>
-  <si>
     <t>Balanço-infantil-Mickey-Mouse-Xalingo-19798-cor-vermelho-e-preto</t>
   </si>
   <si>
@@ -1518,6 +1446,90 @@
   </si>
   <si>
     <t>183 - Piso molhado.png</t>
+  </si>
+  <si>
+    <t>61 - Caixa de caneta com 50 unidades.jpeg</t>
+  </si>
+  <si>
+    <t>182 - Cone.png</t>
+  </si>
+  <si>
+    <t>184 - Dispenser para copo de água e café.png</t>
+  </si>
+  <si>
+    <t>185 - Dispensers1.png</t>
+  </si>
+  <si>
+    <t>186 - Dispensers2.png</t>
+  </si>
+  <si>
+    <t>187 - Fita demarcação.png</t>
+  </si>
+  <si>
+    <t>188 - Canecas Personalizadas.png</t>
+  </si>
+  <si>
+    <t>189 - Garrafa Personalizada.jpg</t>
+  </si>
+  <si>
+    <t>190 - Necessaires.jpg</t>
+  </si>
+  <si>
+    <t>191 - Tacas Personalizadas.png</t>
+  </si>
+  <si>
+    <t>192 - Pedestal unitario e em corrente plastica.png</t>
+  </si>
+  <si>
+    <t>193 - Suporte para copos de água e café.png</t>
+  </si>
+  <si>
+    <t>194 - Tapete Sanitizante.png</t>
+  </si>
+  <si>
+    <t>195 - Totens para alcool em gel.png</t>
+  </si>
+  <si>
+    <t>196 - Totem dispenser de alcool em gel e termometro por sensor.png</t>
+  </si>
+  <si>
+    <t>232 - boneca 1.png</t>
+  </si>
+  <si>
+    <t>233 - boneca 2.png</t>
+  </si>
+  <si>
+    <t>234 - boneca 3.png</t>
+  </si>
+  <si>
+    <t>235 - boneca 4.png</t>
+  </si>
+  <si>
+    <t>236 - boneca 5.png</t>
+  </si>
+  <si>
+    <t>237 - boneca 6.png</t>
+  </si>
+  <si>
+    <t>238 - boneca 7.png</t>
+  </si>
+  <si>
+    <t>177 - cozinha infantil classica paris.png</t>
+  </si>
+  <si>
+    <t>239 - cozinha infantil retro branca.png</t>
+  </si>
+  <si>
+    <t>240 - cozinha infantil retro noruega.png</t>
+  </si>
+  <si>
+    <t>241 - cozinha infantil retro verde agua.png</t>
+  </si>
+  <si>
+    <t>242 - cozinha infantil retro vermelha.png</t>
+  </si>
+  <si>
+    <t>243 - cozinha infantil retro vintage.png</t>
   </si>
 </sst>
 </file>
@@ -1975,17 +1987,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:XFD252"/>
+  <dimension ref="A1:D252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66" style="2" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="60" style="2" customWidth="1"/>
     <col min="4" max="4" width="24.140625" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="2" hidden="1"/>
@@ -1993,853 +2004,853 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>4</v>
@@ -2850,14 +2861,14 @@
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
       <c r="C62" s="9"/>
       <c r="D62" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -2865,7 +2876,7 @@
       <c r="C63" s="9"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -2873,7 +2884,7 @@
       <c r="C64" s="9"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -2881,7 +2892,7 @@
       <c r="C65" s="9"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -2889,7 +2900,7 @@
       <c r="C66" s="9"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -2897,7 +2908,7 @@
       <c r="C67" s="9"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -2905,7 +2916,7 @@
       <c r="C68" s="9"/>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -2913,7 +2924,7 @@
       <c r="C69" s="9"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -2921,1569 +2932,1569 @@
       <c r="C70" s="9"/>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>116</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>117</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>118</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>119</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>120</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>121</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>122</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>123</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>124</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>125</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>126</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>127</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>128</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>402</v>
+        <v>378</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>129</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>130</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>131</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>132</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>133</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>134</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>135</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>136</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>137</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>138</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>139</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>140</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>141</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>142</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>143</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>144</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>145</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>146</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>147</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>148</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>459</v>
+        <v>435</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>149</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>460</v>
+        <v>436</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>150</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>151</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>152</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>153</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>154</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>155</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>156</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>157</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>158</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>159</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>160</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>161</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>162</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>163</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>164</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>165</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>166</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>167</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>168</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>169</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>170</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>171</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>154</v>
+        <v>130</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>172</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>155</v>
+        <v>131</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>173</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>174</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>485</v>
+        <v>461</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>175</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>486</v>
+        <v>462</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>176</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>487</v>
+        <v>463</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>177</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>11</v>
+        <v>491</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>178</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>488</v>
+        <v>464</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>179</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>489</v>
+        <v>465</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>180</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>490</v>
+        <v>466</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>181</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>491</v>
+        <v>467</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>3</v>
@@ -4494,10 +4505,10 @@
         <v>182</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>492</v>
+        <v>470</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>2</v>
@@ -4508,10 +4519,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>13</v>
+        <v>468</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>165</v>
+        <v>141</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>2</v>
@@ -4522,10 +4533,10 @@
         <v>184</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>14</v>
+        <v>471</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="D185" s="3" t="s">
         <v>2</v>
@@ -4536,10 +4547,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>15</v>
+        <v>472</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>2</v>
@@ -4550,10 +4561,10 @@
         <v>186</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>16</v>
+        <v>473</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D187" s="3" t="s">
         <v>2</v>
@@ -4564,10 +4575,10 @@
         <v>187</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>17</v>
+        <v>474</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>2</v>
@@ -4578,10 +4589,10 @@
         <v>188</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>18</v>
+        <v>475</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>2</v>
@@ -4592,10 +4603,10 @@
         <v>189</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>19</v>
+        <v>476</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>2</v>
@@ -4606,10 +4617,10 @@
         <v>190</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>20</v>
+        <v>477</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>2</v>
@@ -4620,10 +4631,10 @@
         <v>191</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>21</v>
+        <v>478</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>2</v>
@@ -4634,10 +4645,10 @@
         <v>192</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>22</v>
+        <v>479</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>2</v>
@@ -4648,10 +4659,10 @@
         <v>193</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>23</v>
+        <v>480</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="D194" s="3" t="s">
         <v>2</v>
@@ -4662,10 +4673,10 @@
         <v>194</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>24</v>
+        <v>481</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>2</v>
@@ -4676,10 +4687,10 @@
         <v>195</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>25</v>
+        <v>482</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>2</v>
@@ -4690,778 +4701,778 @@
         <v>196</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>26</v>
+        <v>483</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>197</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>198</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>199</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>200</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>201</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
       <c r="C202" s="8" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>202</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
       <c r="C203" s="8" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>203</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
       <c r="C204" s="8" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="D204" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>204</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>205</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="C206" s="8" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>206</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>207</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>208</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
       <c r="C209" s="8" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>209</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>210</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>211</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
       <c r="C212" s="8" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>212</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>213</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
       <c r="C214" s="8" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>214</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
       <c r="C215" s="8" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>215</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
       <c r="C216" s="8" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>216</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>217</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>218</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
       <c r="C219" s="8" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>219</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
       <c r="C220" s="8" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>220</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>221</v>
       </c>
       <c r="B222" s="8" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
       <c r="C222" s="8" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>222</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
       <c r="C223" s="8" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>223</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
       <c r="C224" s="8" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>224</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
       <c r="C225" s="8" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>225</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>453</v>
+        <v>429</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="5">
         <v>226</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="D227" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="5">
         <v>227</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="5">
         <v>228</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="5">
         <v>229</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="D230" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="5">
         <v>230</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="D231" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="5">
         <v>231</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="D232" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
         <v>232</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>27</v>
+        <v>484</v>
       </c>
       <c r="C233" s="8" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="D233" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>233</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>28</v>
+        <v>485</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>234</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>29</v>
+        <v>486</v>
       </c>
       <c r="C235" s="8" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>235</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>30</v>
+        <v>487</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="D236" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>236</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>31</v>
+        <v>488</v>
       </c>
       <c r="C237" s="8" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="D237" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>237</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>32</v>
+        <v>489</v>
       </c>
       <c r="C238" s="8" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="D238" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="3">
         <v>238</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>33</v>
+        <v>490</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D239" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>239</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>34</v>
+        <v>492</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="D240" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="3">
         <v>240</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>35</v>
+        <v>493</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="D241" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="3">
         <v>241</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>36</v>
+        <v>494</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="D242" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
         <v>242</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>37</v>
+        <v>495</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="D243" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="3">
         <v>243</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>38</v>
+        <v>496</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="D244" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
         <v>244</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="D245" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="3">
         <v>245</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
       <c r="C246" s="8" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="D246" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>246</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
       <c r="C247" s="8" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="D247" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>247</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D248" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="3">
         <v>248</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
       <c r="C249" s="8" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="D249" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="3">
         <v>248</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="C250" s="8" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="D250" s="3"/>
     </row>
-    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="3">
         <v>249</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="D251" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
         <v>250</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="D252" s="3" t="s">
         <v>1</v>
@@ -5469,11 +5480,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D252" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="VARIEDADES"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D252">
       <sortCondition ref="A1:A252"/>
     </sortState>

</xml_diff>

<commit_message>
mais alterações na planilha.. Criação de novos produtos em banners educativos
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.macedo\OneDrive - Sinergy RH\Desktop\Coding\Anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D34F06-7041-434A-82F3-C8C606FB7C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85294CD9-206B-4C00-9735-303D2A1B45DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="496">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -74,123 +74,6 @@
     <t>VENTILADORES</t>
   </si>
   <si>
-    <t>banner-aniversariante-do-mes-site</t>
-  </si>
-  <si>
-    <t>banner-aprenda-a-lavar-a-mao-corretamente</t>
-  </si>
-  <si>
-    <t>banner-bioma-do-brasil-site</t>
-  </si>
-  <si>
-    <t>banner-boa-convivencia-site</t>
-  </si>
-  <si>
-    <t>banner-calendario-site</t>
-  </si>
-  <si>
-    <t>banner-cantinho-da-leitura-site</t>
-  </si>
-  <si>
-    <t>banner-chamadinha-site</t>
-  </si>
-  <si>
-    <t>banner-ciclo-da-agua</t>
-  </si>
-  <si>
-    <t>banner-clima-do-brasil</t>
-  </si>
-  <si>
-    <t>banner-clima-site</t>
-  </si>
-  <si>
-    <t>banner-combinados-da-turma</t>
-  </si>
-  <si>
-    <t>banner-diga-nao-ao-bulling-site</t>
-  </si>
-  <si>
-    <t>BANNER-ESQUELETO-HUMANO</t>
-  </si>
-  <si>
-    <t>banner-formas-geometricas-completa</t>
-  </si>
-  <si>
-    <t>banner-fraçao-site</t>
-  </si>
-  <si>
-    <t>banner-generos-textuais-site</t>
-  </si>
-  <si>
-    <t>banner-geografia</t>
-  </si>
-  <si>
-    <t>banner-hino-nacional-brasileiro-site</t>
-  </si>
-  <si>
-    <t>banner-mapa-do-brasil</t>
-  </si>
-  <si>
-    <t>banner-mapa-economico-brasileiro-site</t>
-  </si>
-  <si>
-    <t>banner-mapa-mundi-site</t>
-  </si>
-  <si>
-    <t>banner-mapa-municipal-de-sao-paulo-site</t>
-  </si>
-  <si>
-    <t>banner-numerais-de-0-a-100-site</t>
-  </si>
-  <si>
-    <t>banner-numerais-e-escritas</t>
-  </si>
-  <si>
-    <t>banner-numeros-romanos-site</t>
-  </si>
-  <si>
-    <t>Banner-ou-painel-corpo-humano-material-gratuito</t>
-  </si>
-  <si>
-    <t>banner-palavrinhas-magicas-site</t>
-  </si>
-  <si>
-    <t>banner-presidentes-do-brasil-site</t>
-  </si>
-  <si>
-    <t>banner-regras-do-porque-site</t>
-  </si>
-  <si>
-    <t>banner-regras-matematica</t>
-  </si>
-  <si>
-    <t>banner-silabario-simples-site</t>
-  </si>
-  <si>
-    <t>banner-sinais-de-pontuacao-site</t>
-  </si>
-  <si>
-    <t>banner-sistema-muscular-site</t>
-  </si>
-  <si>
-    <t>banner-subtracao-site</t>
-  </si>
-  <si>
-    <t>banner-tabela-periodica</t>
-  </si>
-  <si>
-    <t>banner-tabuada-site</t>
-  </si>
-  <si>
-    <t>banner-texto-narrativo-site</t>
-  </si>
-  <si>
-    <t>banner-vogais-e-consuantes</t>
-  </si>
-  <si>
-    <t>banner-vogais-site</t>
-  </si>
-  <si>
     <t>Tabela-Basquete-Mdf-9mm-Aro-36-Cm-Basketball-Master-Xalingo-SITE</t>
   </si>
   <si>
@@ -200,51 +83,12 @@
     <t>Xalingo-tabela-cesta-de-basquete-com-bola-SITE</t>
   </si>
   <si>
-    <t>banner-ajudante-do-dia</t>
-  </si>
-  <si>
-    <t>banner-aniversariante-do-mes</t>
-  </si>
-  <si>
-    <t>banner-chamadinha</t>
-  </si>
-  <si>
-    <t>boas-maneiras,-regrinhas-de-convivencia</t>
-  </si>
-  <si>
-    <t>emborrachado-de-calendario-personalizavel</t>
-  </si>
-  <si>
-    <t>defina-seu-cardapio-da-semana</t>
-  </si>
-  <si>
-    <t>Banner-Meses-do-Ano-80-x-120-cm-(L-x-A)</t>
-  </si>
-  <si>
     <t>Jogo-De-Ping-Pong-Simples-Xalingo-SITE</t>
   </si>
   <si>
-    <t>banner-formas-geometricas</t>
-  </si>
-  <si>
-    <t>banner-montagem-silabica-site</t>
-  </si>
-  <si>
     <t>Mesa-de-pebolim-Xalingo-Super-copa-cor-verde-SITE</t>
   </si>
   <si>
-    <t>banner-pedagogico-animais-vertebrados-repteis-site</t>
-  </si>
-  <si>
-    <t>banner-divisao-site</t>
-  </si>
-  <si>
-    <t>banner-mapa-de-sao-paulo-site</t>
-  </si>
-  <si>
-    <t>banner-personalizado-conforme-a-solicitaçao-do-cliente-site</t>
-  </si>
-  <si>
     <t>Jogo-De-Botao-Brasileirao-Xalingo-SITE</t>
   </si>
   <si>
@@ -1524,6 +1368,165 @@
   </si>
   <si>
     <t>167-ventilador-ventisilva-coluna-mesa-2-em-1.html</t>
+  </si>
+  <si>
+    <t>22-banner-aniversariante-do-mes-site.html</t>
+  </si>
+  <si>
+    <t>23-banner-aprenda-a-lavar-a-mao-corretamente.html</t>
+  </si>
+  <si>
+    <t>24-banner-bioma-do-brasil-site.html</t>
+  </si>
+  <si>
+    <t>25-banner-boa-convivencia-site.html</t>
+  </si>
+  <si>
+    <t>26-banner-calendario-site.html</t>
+  </si>
+  <si>
+    <t>27-banner-cantinho-da-leitura-site.html</t>
+  </si>
+  <si>
+    <t>28-banner-chamadinha-site.html</t>
+  </si>
+  <si>
+    <t>29-banner-ciclo-da-agua.html</t>
+  </si>
+  <si>
+    <t>30-banner-clima-do-brasil.html</t>
+  </si>
+  <si>
+    <t>31-banner-clima-site.html</t>
+  </si>
+  <si>
+    <t>32-banner-combinados-da-turma.html</t>
+  </si>
+  <si>
+    <t>33-banner-diga-nao-ao-bulling-site.html</t>
+  </si>
+  <si>
+    <t>34-banner-divisao-site.html</t>
+  </si>
+  <si>
+    <t>35-BANNER-ESQUELETO-HUMANO.html</t>
+  </si>
+  <si>
+    <t>36-banner-formas-geometricas.html</t>
+  </si>
+  <si>
+    <t>37-banner-formas-geometricas-completa.html</t>
+  </si>
+  <si>
+    <t>38-banner-fraçao-site.html</t>
+  </si>
+  <si>
+    <t>39-banner-generos-textuais-site.html</t>
+  </si>
+  <si>
+    <t>40-banner-geografia.html</t>
+  </si>
+  <si>
+    <t>41-banner-hino-nacional-brasileiro-site.html</t>
+  </si>
+  <si>
+    <t>42-banner-mapa-de-sao-paulo-site.html</t>
+  </si>
+  <si>
+    <t>43-banner-mapa-do-brasil.html</t>
+  </si>
+  <si>
+    <t>44-banner-mapa-economico-brasileiro-site.html</t>
+  </si>
+  <si>
+    <t>45-banner-mapa-mundi-site.html</t>
+  </si>
+  <si>
+    <t>46-banner-mapa-municipal-de-sao-paulo-site.html</t>
+  </si>
+  <si>
+    <t>47-Banner-Meses-do-Ano-80-x-120-cm-(L-x-A).html</t>
+  </si>
+  <si>
+    <t>48-banner-montagem-silabica-site.html</t>
+  </si>
+  <si>
+    <t>49-banner-numerais-de-0-a-100-site.html</t>
+  </si>
+  <si>
+    <t>50-banner-numerais-e-escritas.html</t>
+  </si>
+  <si>
+    <t>51-banner-numeros-romanos-site.html</t>
+  </si>
+  <si>
+    <t>52-Banner-ou-painel-corpo-humano-material-gratuito.html</t>
+  </si>
+  <si>
+    <t>53-banner-palavrinhas-magicas-site.html</t>
+  </si>
+  <si>
+    <t>54-banner-pedagogico-animais-vertebrados-repteis-site.html</t>
+  </si>
+  <si>
+    <t>55-banner-personalizado-conforme-a-solicitaçao-do-cliente-site.html</t>
+  </si>
+  <si>
+    <t>56-banner-presidentes-do-brasil-site.html</t>
+  </si>
+  <si>
+    <t>57-banner-regras-do-porque-site.html</t>
+  </si>
+  <si>
+    <t>58-banner-regras-matematica.html</t>
+  </si>
+  <si>
+    <t>59-banner-silabario-simples-site.html</t>
+  </si>
+  <si>
+    <t>60-banner-sinais-de-pontuacao-site.html</t>
+  </si>
+  <si>
+    <t>61-Caixa de caneta com 50 unidades.html</t>
+  </si>
+  <si>
+    <t>70-banner-sistema-muscular-site.html</t>
+  </si>
+  <si>
+    <t>71-banner-subtracao-site.html</t>
+  </si>
+  <si>
+    <t>72-banner-tabela-periodica.html</t>
+  </si>
+  <si>
+    <t>73-banner-tabuada-site.html</t>
+  </si>
+  <si>
+    <t>74-banner-texto-narrativo-site.html</t>
+  </si>
+  <si>
+    <t>76-banner-vogais-site.html</t>
+  </si>
+  <si>
+    <t>75-banner-vogais-e-consoantes.html</t>
+  </si>
+  <si>
+    <t>226-banner-ajudante-do-dia.html</t>
+  </si>
+  <si>
+    <t>227-banner-aniversariante-do-mes.html</t>
+  </si>
+  <si>
+    <t>228-banner-chamadinha.html</t>
+  </si>
+  <si>
+    <t>229-boas-maneiras-regrinhas-de-convivencia.html</t>
+  </si>
+  <si>
+    <t>230-emborrachado-personalizavel.html</t>
+  </si>
+  <si>
+    <t>231-defina-seu-cardapio-da-semana.html</t>
   </si>
 </sst>
 </file>
@@ -1981,10 +1984,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,153 +2002,153 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>233</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>329</v>
+        <v>277</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>330</v>
+        <v>278</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>331</v>
+        <v>279</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>152</v>
+        <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>332</v>
+        <v>280</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>153</v>
+        <v>101</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>333</v>
+        <v>281</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>154</v>
+        <v>102</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>334</v>
+        <v>282</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>155</v>
+        <v>103</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>335</v>
+        <v>283</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>336</v>
+        <v>284</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>337</v>
+        <v>285</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>158</v>
+        <v>106</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>338</v>
+        <v>286</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>1</v>
@@ -2155,10 +2159,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>4</v>
@@ -2169,10 +2173,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>4</v>
@@ -2183,10 +2187,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>4</v>
@@ -2197,10 +2201,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>4</v>
@@ -2211,10 +2215,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>90</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>4</v>
@@ -2225,10 +2229,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>4</v>
@@ -2239,10 +2243,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>4</v>
@@ -2253,10 +2257,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>4</v>
@@ -2267,10 +2271,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>4</v>
@@ -2281,10 +2285,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>4</v>
@@ -2295,10 +2299,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>4</v>
@@ -2309,10 +2313,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>11</v>
+        <v>443</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>4</v>
@@ -2323,10 +2327,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>12</v>
+        <v>444</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>4</v>
@@ -2337,10 +2341,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>99</v>
+        <v>47</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>13</v>
+        <v>445</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
@@ -2351,10 +2355,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>14</v>
+        <v>446</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>4</v>
@@ -2365,10 +2369,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>15</v>
+        <v>447</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>4</v>
@@ -2379,10 +2383,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>16</v>
+        <v>448</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>4</v>
@@ -2393,10 +2397,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>17</v>
+        <v>449</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>4</v>
@@ -2407,10 +2411,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>18</v>
+        <v>450</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
@@ -2421,10 +2425,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>19</v>
+        <v>451</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>4</v>
@@ -2435,10 +2439,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>20</v>
+        <v>452</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>4</v>
@@ -2449,10 +2453,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>21</v>
+        <v>453</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>4</v>
@@ -2463,10 +2467,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>108</v>
+        <v>56</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>22</v>
+        <v>454</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>4</v>
@@ -2477,10 +2481,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>65</v>
+        <v>455</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>4</v>
@@ -2491,10 +2495,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>110</v>
+        <v>58</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>23</v>
+        <v>456</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>4</v>
@@ -2505,10 +2509,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>61</v>
+        <v>457</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>4</v>
@@ -2519,10 +2523,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>24</v>
+        <v>458</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>4</v>
@@ -2533,10 +2537,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>113</v>
+        <v>61</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>25</v>
+        <v>459</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>4</v>
@@ -2547,10 +2551,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>26</v>
+        <v>460</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>4</v>
@@ -2561,10 +2565,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>27</v>
+        <v>461</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>4</v>
@@ -2575,10 +2579,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>28</v>
+        <v>462</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>4</v>
@@ -2589,10 +2593,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>66</v>
+        <v>463</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>4</v>
@@ -2603,10 +2607,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>29</v>
+        <v>464</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>4</v>
@@ -2617,10 +2621,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>30</v>
+        <v>465</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>4</v>
@@ -2631,10 +2635,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>31</v>
+        <v>466</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>4</v>
@@ -2645,10 +2649,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>32</v>
+        <v>467</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>4</v>
@@ -2659,10 +2663,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>59</v>
+        <v>468</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>4</v>
@@ -2673,10 +2677,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>123</v>
+        <v>71</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>62</v>
+        <v>469</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>4</v>
@@ -2687,10 +2691,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>33</v>
+        <v>470</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>4</v>
@@ -2701,10 +2705,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>34</v>
+        <v>471</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>4</v>
@@ -2715,10 +2719,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>126</v>
+        <v>74</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>35</v>
+        <v>472</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>4</v>
@@ -2729,10 +2733,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>127</v>
+        <v>75</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>36</v>
+        <v>473</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>4</v>
@@ -2743,10 +2747,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>37</v>
+        <v>474</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>4</v>
@@ -2757,10 +2761,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>64</v>
+        <v>475</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>4</v>
@@ -2771,10 +2775,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>67</v>
+        <v>476</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>4</v>
@@ -2785,10 +2789,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>38</v>
+        <v>477</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>4</v>
@@ -2799,10 +2803,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>39</v>
+        <v>478</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>4</v>
@@ -2813,10 +2817,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>40</v>
+        <v>479</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>4</v>
@@ -2827,10 +2831,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>41</v>
+        <v>480</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>4</v>
@@ -2841,28 +2845,30 @@
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>42</v>
+        <v>481</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="C62" s="9"/>
+        <v>249</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>482</v>
+      </c>
       <c r="D62" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -2870,7 +2876,7 @@
       <c r="C63" s="9"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -2878,7 +2884,7 @@
       <c r="C64" s="9"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -2886,7 +2892,7 @@
       <c r="C65" s="9"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -2894,7 +2900,7 @@
       <c r="C66" s="9"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -2902,7 +2908,7 @@
       <c r="C67" s="9"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -2910,7 +2916,7 @@
       <c r="C68" s="9"/>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -2918,7 +2924,7 @@
       <c r="C69" s="9"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -2931,10 +2937,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>43</v>
+        <v>483</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>4</v>
@@ -2945,10 +2951,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>44</v>
+        <v>484</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>4</v>
@@ -2959,10 +2965,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>45</v>
+        <v>485</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>4</v>
@@ -2973,10 +2979,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>46</v>
+        <v>486</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>4</v>
@@ -2987,10 +2993,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>47</v>
+        <v>487</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>4</v>
@@ -3001,10 +3007,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>48</v>
+        <v>489</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>4</v>
@@ -3015,2090 +3021,2090 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>142</v>
+        <v>90</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>49</v>
+        <v>488</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>339</v>
+        <v>287</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>160</v>
+        <v>108</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>340</v>
+        <v>288</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>161</v>
+        <v>109</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>341</v>
+        <v>289</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>162</v>
+        <v>110</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>342</v>
+        <v>290</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>343</v>
+        <v>291</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>344</v>
+        <v>292</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>165</v>
+        <v>113</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>345</v>
+        <v>293</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>346</v>
+        <v>294</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>167</v>
+        <v>115</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>347</v>
+        <v>295</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>168</v>
+        <v>116</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>348</v>
+        <v>296</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>349</v>
+        <v>297</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>350</v>
+        <v>298</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>351</v>
+        <v>299</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>352</v>
+        <v>300</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>173</v>
+        <v>121</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>353</v>
+        <v>301</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>354</v>
+        <v>302</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>355</v>
+        <v>303</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>356</v>
+        <v>304</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>177</v>
+        <v>125</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>357</v>
+        <v>305</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>178</v>
+        <v>126</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>358</v>
+        <v>306</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>359</v>
+        <v>307</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>180</v>
+        <v>128</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>360</v>
+        <v>308</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>361</v>
+        <v>309</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>182</v>
+        <v>130</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>362</v>
+        <v>310</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>363</v>
+        <v>311</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>184</v>
+        <v>132</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>364</v>
+        <v>312</v>
       </c>
       <c r="D103" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>365</v>
+        <v>313</v>
       </c>
       <c r="D104" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>186</v>
+        <v>134</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>366</v>
+        <v>314</v>
       </c>
       <c r="D105" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>187</v>
+        <v>135</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>367</v>
+        <v>315</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>188</v>
+        <v>136</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>368</v>
+        <v>316</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>189</v>
+        <v>137</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>369</v>
+        <v>317</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>190</v>
+        <v>138</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>370</v>
+        <v>318</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>191</v>
+        <v>139</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>371</v>
+        <v>319</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>192</v>
+        <v>140</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>372</v>
+        <v>320</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>193</v>
+        <v>141</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>373</v>
+        <v>321</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>194</v>
+        <v>142</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>374</v>
+        <v>322</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>375</v>
+        <v>323</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>376</v>
+        <v>324</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>197</v>
+        <v>145</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>377</v>
+        <v>325</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>116</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>198</v>
+        <v>146</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>378</v>
+        <v>326</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>117</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>199</v>
+        <v>147</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>379</v>
+        <v>327</v>
       </c>
       <c r="D118" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>118</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>380</v>
+        <v>328</v>
       </c>
       <c r="D119" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>119</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>201</v>
+        <v>149</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>381</v>
+        <v>329</v>
       </c>
       <c r="D120" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>120</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>382</v>
+        <v>330</v>
       </c>
       <c r="D121" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>121</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>203</v>
+        <v>151</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>383</v>
+        <v>331</v>
       </c>
       <c r="D122" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>122</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>204</v>
+        <v>152</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>384</v>
+        <v>332</v>
       </c>
       <c r="D123" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>123</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>385</v>
+        <v>333</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>124</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>206</v>
+        <v>154</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>386</v>
+        <v>334</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>125</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>207</v>
+        <v>155</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>387</v>
+        <v>335</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>126</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>388</v>
+        <v>336</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>127</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>209</v>
+        <v>157</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>389</v>
+        <v>337</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>128</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>210</v>
+        <v>158</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>390</v>
+        <v>338</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>129</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>211</v>
+        <v>159</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>391</v>
+        <v>339</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>130</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>212</v>
+        <v>160</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>392</v>
+        <v>340</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>131</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>393</v>
+        <v>341</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>132</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>394</v>
+        <v>342</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>133</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>395</v>
+        <v>343</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>134</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>135</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>217</v>
+        <v>165</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>397</v>
+        <v>345</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>136</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>218</v>
+        <v>166</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>398</v>
+        <v>346</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>137</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>219</v>
+        <v>167</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>399</v>
+        <v>347</v>
       </c>
       <c r="D138" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>138</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>220</v>
+        <v>168</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>400</v>
+        <v>348</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>139</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>221</v>
+        <v>169</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>401</v>
+        <v>349</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>140</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>222</v>
+        <v>170</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>402</v>
+        <v>350</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>141</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>223</v>
+        <v>171</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>403</v>
+        <v>351</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>142</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>224</v>
+        <v>172</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>404</v>
+        <v>352</v>
       </c>
       <c r="D143" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>143</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>470</v>
+        <v>418</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>144</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>263</v>
+        <v>211</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>471</v>
+        <v>419</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>145</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>264</v>
+        <v>212</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>472</v>
+        <v>420</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>146</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>265</v>
+        <v>213</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>473</v>
+        <v>421</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>147</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>474</v>
+        <v>422</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>148</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>267</v>
+        <v>215</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>475</v>
+        <v>423</v>
       </c>
       <c r="D149" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>149</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>268</v>
+        <v>216</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>476</v>
+        <v>424</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>150</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>269</v>
+        <v>217</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>477</v>
+        <v>425</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>151</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>270</v>
+        <v>218</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>478</v>
+        <v>426</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>152</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>479</v>
+        <v>427</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>153</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>272</v>
+        <v>220</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>480</v>
+        <v>428</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>154</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>273</v>
+        <v>221</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>481</v>
+        <v>429</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>155</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>274</v>
+        <v>222</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>482</v>
+        <v>430</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>156</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>275</v>
+        <v>223</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>483</v>
+        <v>431</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>157</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>276</v>
+        <v>224</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>484</v>
+        <v>432</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>158</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>277</v>
+        <v>225</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>485</v>
+        <v>433</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>159</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>486</v>
+        <v>434</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>160</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>279</v>
+        <v>227</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>487</v>
+        <v>435</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>161</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>280</v>
+        <v>228</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>488</v>
+        <v>436</v>
       </c>
       <c r="D162" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>162</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>281</v>
+        <v>229</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>489</v>
+        <v>437</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>163</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>282</v>
+        <v>230</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>490</v>
+        <v>438</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>164</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>283</v>
+        <v>231</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>491</v>
+        <v>439</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>165</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>284</v>
+        <v>232</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>492</v>
+        <v>440</v>
       </c>
       <c r="D166" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>166</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>285</v>
+        <v>233</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>493</v>
+        <v>441</v>
       </c>
       <c r="D167" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>167</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>286</v>
+        <v>234</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>494</v>
+        <v>442</v>
       </c>
       <c r="D168" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>168</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>287</v>
+        <v>235</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>445</v>
+        <v>393</v>
       </c>
       <c r="D169" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>169</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>288</v>
+        <v>236</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>446</v>
+        <v>394</v>
       </c>
       <c r="D170" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>170</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>289</v>
+        <v>237</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>447</v>
+        <v>395</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>171</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>290</v>
+        <v>238</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>448</v>
+        <v>396</v>
       </c>
       <c r="D172" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>172</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>449</v>
+        <v>397</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>173</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>292</v>
+        <v>240</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>450</v>
+        <v>398</v>
       </c>
       <c r="D174" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>174</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>293</v>
+        <v>241</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>451</v>
+        <v>399</v>
       </c>
       <c r="D175" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>175</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>294</v>
+        <v>242</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>452</v>
+        <v>400</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>176</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>295</v>
+        <v>243</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>453</v>
+        <v>401</v>
       </c>
       <c r="D177" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>177</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>323</v>
+        <v>271</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>419</v>
+        <v>367</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>178</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>296</v>
+        <v>244</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>454</v>
+        <v>402</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>179</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>297</v>
+        <v>245</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>455</v>
+        <v>403</v>
       </c>
       <c r="D180" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>180</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>298</v>
+        <v>246</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>456</v>
+        <v>404</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>181</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>299</v>
+        <v>247</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>457</v>
+        <v>405</v>
       </c>
       <c r="D182" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>182</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>302</v>
+        <v>250</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>458</v>
+        <v>406</v>
       </c>
       <c r="D183" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>183</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>300</v>
+        <v>248</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>459</v>
+        <v>407</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>184</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>303</v>
+        <v>251</v>
       </c>
       <c r="C185" s="9"/>
       <c r="D185" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>185</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>304</v>
+        <v>252</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>460</v>
+        <v>408</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>186</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>305</v>
+        <v>253</v>
       </c>
       <c r="C187" s="9"/>
       <c r="D187" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>187</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>306</v>
+        <v>254</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>461</v>
+        <v>409</v>
       </c>
       <c r="D188" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>188</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>307</v>
+        <v>255</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>462</v>
+        <v>410</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>189</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>308</v>
+        <v>256</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>463</v>
+        <v>411</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>190</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>309</v>
+        <v>257</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>464</v>
+        <v>412</v>
       </c>
       <c r="D191" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>191</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>310</v>
+        <v>258</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>465</v>
+        <v>413</v>
       </c>
       <c r="D192" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>192</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>311</v>
+        <v>259</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>466</v>
+        <v>414</v>
       </c>
       <c r="D193" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>193</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>312</v>
+        <v>260</v>
       </c>
       <c r="C194" s="9"/>
       <c r="D194" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>194</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>313</v>
+        <v>261</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>467</v>
+        <v>415</v>
       </c>
       <c r="D195" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>195</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>314</v>
+        <v>262</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>468</v>
+        <v>416</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>196</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>315</v>
+        <v>263</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>469</v>
+        <v>417</v>
       </c>
       <c r="D197" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>197</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>234</v>
+        <v>182</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="D198" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>198</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>235</v>
+        <v>183</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D199" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>199</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>236</v>
+        <v>184</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="D200" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>200</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>237</v>
+        <v>185</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D201" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>201</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>238</v>
+        <v>186</v>
       </c>
       <c r="C202" s="8" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="D202" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>202</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>239</v>
+        <v>187</v>
       </c>
       <c r="C203" s="8" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="D203" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>203</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>240</v>
+        <v>188</v>
       </c>
       <c r="C204" s="8" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D204" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>204</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>241</v>
+        <v>189</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="D205" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>205</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>242</v>
+        <v>190</v>
       </c>
       <c r="C206" s="8" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>206</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>243</v>
+        <v>191</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>425</v>
+        <v>373</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>207</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>426</v>
+        <v>374</v>
       </c>
       <c r="D208" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>208</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>245</v>
+        <v>193</v>
       </c>
       <c r="C209" s="8" t="s">
-        <v>427</v>
+        <v>375</v>
       </c>
       <c r="D209" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>209</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>246</v>
+        <v>194</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>428</v>
+        <v>376</v>
       </c>
       <c r="D210" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>210</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>429</v>
+        <v>377</v>
       </c>
       <c r="D211" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>211</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>247</v>
+        <v>195</v>
       </c>
       <c r="C212" s="8" t="s">
-        <v>430</v>
+        <v>378</v>
       </c>
       <c r="D212" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>212</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>248</v>
+        <v>196</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>431</v>
+        <v>379</v>
       </c>
       <c r="D213" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>213</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>249</v>
+        <v>197</v>
       </c>
       <c r="C214" s="8" t="s">
-        <v>432</v>
+        <v>380</v>
       </c>
       <c r="D214" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>214</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="C215" s="8" t="s">
-        <v>433</v>
+        <v>381</v>
       </c>
       <c r="D215" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>215</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="C216" s="8" t="s">
-        <v>434</v>
+        <v>382</v>
       </c>
       <c r="D216" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>216</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>435</v>
+        <v>383</v>
       </c>
       <c r="D217" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>217</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>253</v>
+        <v>201</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>436</v>
+        <v>384</v>
       </c>
       <c r="D218" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>218</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="C219" s="8" t="s">
-        <v>437</v>
+        <v>385</v>
       </c>
       <c r="D219" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>219</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="C220" s="8" t="s">
-        <v>438</v>
+        <v>386</v>
       </c>
       <c r="D220" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>220</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>439</v>
+        <v>387</v>
       </c>
       <c r="D221" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>221</v>
       </c>
       <c r="B222" s="8" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
       <c r="C222" s="8" t="s">
-        <v>440</v>
+        <v>388</v>
       </c>
       <c r="D222" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>222</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>258</v>
+        <v>206</v>
       </c>
       <c r="C223" s="8" t="s">
-        <v>441</v>
+        <v>389</v>
       </c>
       <c r="D223" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>223</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>259</v>
+        <v>207</v>
       </c>
       <c r="C224" s="8" t="s">
-        <v>442</v>
+        <v>390</v>
       </c>
       <c r="D224" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>224</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>260</v>
+        <v>208</v>
       </c>
       <c r="C225" s="8" t="s">
-        <v>443</v>
+        <v>391</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>225</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>261</v>
+        <v>209</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>444</v>
+        <v>392</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>9</v>
@@ -5109,10 +5115,10 @@
         <v>226</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>53</v>
+        <v>490</v>
       </c>
       <c r="D227" s="5" t="s">
         <v>4</v>
@@ -5123,10 +5129,10 @@
         <v>227</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>54</v>
+        <v>491</v>
       </c>
       <c r="D228" s="5" t="s">
         <v>4</v>
@@ -5137,10 +5143,10 @@
         <v>228</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>55</v>
+        <v>492</v>
       </c>
       <c r="D229" s="5" t="s">
         <v>4</v>
@@ -5151,10 +5157,10 @@
         <v>229</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>56</v>
+        <v>493</v>
       </c>
       <c r="D230" s="5" t="s">
         <v>4</v>
@@ -5165,10 +5171,10 @@
         <v>230</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>57</v>
+        <v>494</v>
       </c>
       <c r="D231" s="5" t="s">
         <v>4</v>
@@ -5179,288 +5185,288 @@
         <v>231</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>148</v>
+        <v>96</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>58</v>
+        <v>495</v>
       </c>
       <c r="D232" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
         <v>232</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>316</v>
+        <v>264</v>
       </c>
       <c r="C233" s="8" t="s">
-        <v>412</v>
+        <v>360</v>
       </c>
       <c r="D233" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>233</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>317</v>
+        <v>265</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>413</v>
+        <v>361</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>234</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>318</v>
+        <v>266</v>
       </c>
       <c r="C235" s="8" t="s">
-        <v>414</v>
+        <v>362</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>235</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>319</v>
+        <v>267</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>415</v>
+        <v>363</v>
       </c>
       <c r="D236" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>236</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>320</v>
+        <v>268</v>
       </c>
       <c r="C237" s="8" t="s">
-        <v>416</v>
+        <v>364</v>
       </c>
       <c r="D237" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>237</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>321</v>
+        <v>269</v>
       </c>
       <c r="C238" s="8" t="s">
-        <v>417</v>
+        <v>365</v>
       </c>
       <c r="D238" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="3">
         <v>238</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>322</v>
+        <v>270</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>418</v>
+        <v>366</v>
       </c>
       <c r="D239" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>239</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>420</v>
+        <v>368</v>
       </c>
       <c r="D240" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="3">
         <v>240</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>325</v>
+        <v>273</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>421</v>
+        <v>369</v>
       </c>
       <c r="D241" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3">
         <v>241</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>326</v>
+        <v>274</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>422</v>
+        <v>370</v>
       </c>
       <c r="D242" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
         <v>242</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>327</v>
+        <v>275</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>423</v>
+        <v>371</v>
       </c>
       <c r="D243" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="3">
         <v>243</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>328</v>
+        <v>276</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>424</v>
+        <v>372</v>
       </c>
       <c r="D244" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
         <v>244</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>225</v>
+        <v>173</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>405</v>
+        <v>353</v>
       </c>
       <c r="D245" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="3">
         <v>245</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>226</v>
+        <v>174</v>
       </c>
       <c r="C246" s="8" t="s">
-        <v>406</v>
+        <v>354</v>
       </c>
       <c r="D246" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>246</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>227</v>
+        <v>175</v>
       </c>
       <c r="C247" s="8" t="s">
-        <v>407</v>
+        <v>355</v>
       </c>
       <c r="D247" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>247</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>228</v>
+        <v>176</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>408</v>
+        <v>356</v>
       </c>
       <c r="D248" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="3">
         <v>248</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>229</v>
+        <v>177</v>
       </c>
       <c r="C249" s="8" t="s">
-        <v>409</v>
+        <v>357</v>
       </c>
       <c r="D249" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="3">
         <v>248</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>230</v>
+        <v>178</v>
       </c>
       <c r="C250" s="8" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="D250" s="3"/>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="3">
         <v>249</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>231</v>
+        <v>179</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>410</v>
+        <v>358</v>
       </c>
       <c r="D251" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
         <v>250</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>232</v>
+        <v>180</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>411</v>
+        <v>359</v>
       </c>
       <c r="D252" s="3" t="s">
         <v>1</v>
@@ -5468,6 +5474,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D252" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="BANNERS EDUCATIVOS"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D252">
       <sortCondition ref="A1:A252"/>
     </sortState>

</xml_diff>

<commit_message>
criação de alguns arquivos python - teste 1
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.macedo\OneDrive - Sinergy RH\Desktop\Coding\Anil-clean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85294CD9-206B-4C00-9735-303D2A1B45DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866B2BA7-2105-4BEE-8768-EEBC98002C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$D$252</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$E$252</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="566">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -1527,6 +1527,216 @@
   </si>
   <si>
     <t>231-defina-seu-cardapio-da-semana.html</t>
+  </si>
+  <si>
+    <t>NOME DO PRODUTO</t>
+  </si>
+  <si>
+    <t>Banner ou painel corpo humano material gratuito</t>
+  </si>
+  <si>
+    <t>banner texto narrativo site</t>
+  </si>
+  <si>
+    <t>banner vogais e consuantes</t>
+  </si>
+  <si>
+    <t>banner vogais site</t>
+  </si>
+  <si>
+    <t>banner ajudante do dia</t>
+  </si>
+  <si>
+    <t>banner aniversariante do mes</t>
+  </si>
+  <si>
+    <t>banner chamadinha</t>
+  </si>
+  <si>
+    <t>boas maneiras, regrinhas de convivencia</t>
+  </si>
+  <si>
+    <t>emborrachado de calendario personalizavel</t>
+  </si>
+  <si>
+    <t>defina seu cardapio da semana</t>
+  </si>
+  <si>
+    <t>Banner árvore da vida</t>
+  </si>
+  <si>
+    <t>Banner cardápio da semana</t>
+  </si>
+  <si>
+    <t>Banner célula vegetal e animal</t>
+  </si>
+  <si>
+    <t>Banner plantas</t>
+  </si>
+  <si>
+    <t>Banner tabuada adição</t>
+  </si>
+  <si>
+    <t>Banner ajudante do dia</t>
+  </si>
+  <si>
+    <t>Banner alfabeto</t>
+  </si>
+  <si>
+    <t>Banner animais vertebrados aves</t>
+  </si>
+  <si>
+    <t>Banner animais vertebrados anfíbios</t>
+  </si>
+  <si>
+    <t>Banner animais vertebrados mamíferos</t>
+  </si>
+  <si>
+    <t>Banner animais vertebrados peixes</t>
+  </si>
+  <si>
+    <t>Banner aniversariante do mês</t>
+  </si>
+  <si>
+    <t>Banner aprenda a lavar a mão corretamente</t>
+  </si>
+  <si>
+    <t>Banner bioma do Brasil</t>
+  </si>
+  <si>
+    <t>Banner boa convivência</t>
+  </si>
+  <si>
+    <t>Banner calendário</t>
+  </si>
+  <si>
+    <t>Banner cantinho da leitura</t>
+  </si>
+  <si>
+    <t>Banner chamadinha</t>
+  </si>
+  <si>
+    <t>Banner ciclo da água</t>
+  </si>
+  <si>
+    <t>Banner clima do Brasil</t>
+  </si>
+  <si>
+    <t>Banner clima</t>
+  </si>
+  <si>
+    <t>Banner combinados da turma</t>
+  </si>
+  <si>
+    <t>Banner diga não ao bullying</t>
+  </si>
+  <si>
+    <t>Banner divisão</t>
+  </si>
+  <si>
+    <t>Banner esqueleto humano</t>
+  </si>
+  <si>
+    <t>Banner formas geométricas</t>
+  </si>
+  <si>
+    <t>Banner formas geométricas completa</t>
+  </si>
+  <si>
+    <t>Banner fração</t>
+  </si>
+  <si>
+    <t>Banner gêneros textuais</t>
+  </si>
+  <si>
+    <t>Banner geografia</t>
+  </si>
+  <si>
+    <t>Banner hino nacional brasileiro</t>
+  </si>
+  <si>
+    <t>Banner mapa de São Paulo</t>
+  </si>
+  <si>
+    <t>Banner mapa do Brasil</t>
+  </si>
+  <si>
+    <t>Banner mapa econômico brasileiro</t>
+  </si>
+  <si>
+    <t>Banner mapa mundi</t>
+  </si>
+  <si>
+    <t>Banner mapa municipal de São Paulo</t>
+  </si>
+  <si>
+    <t>Banner meses do ano - 80 x 120 cm (L x A)</t>
+  </si>
+  <si>
+    <t>Banner montagem silábica</t>
+  </si>
+  <si>
+    <t>Banner numerais de 0 a 100</t>
+  </si>
+  <si>
+    <t>Banner numerais e escritas</t>
+  </si>
+  <si>
+    <t>Banner números romanos</t>
+  </si>
+  <si>
+    <t>Banner palavrinhas mágicas</t>
+  </si>
+  <si>
+    <t>Banner pedagógico animais vertebrados répteis</t>
+  </si>
+  <si>
+    <t>Banner personalizado conforme a solicitação do cliente</t>
+  </si>
+  <si>
+    <t>Banner presidentes do Brasil</t>
+  </si>
+  <si>
+    <t>Banner regras do porquê</t>
+  </si>
+  <si>
+    <t>Banner regras matemática</t>
+  </si>
+  <si>
+    <t>Banner silabário simples</t>
+  </si>
+  <si>
+    <t>Banner sinais de pontuação</t>
+  </si>
+  <si>
+    <t>Banner sistema muscular</t>
+  </si>
+  <si>
+    <t>Banner subtração</t>
+  </si>
+  <si>
+    <t>Banner tabela periódica</t>
+  </si>
+  <si>
+    <t>Banner tabuada</t>
+  </si>
+  <si>
+    <t>Banner texto narrativo</t>
+  </si>
+  <si>
+    <t>Banner vogais e consoantes</t>
+  </si>
+  <si>
+    <t>Banner vogais</t>
+  </si>
+  <si>
+    <t>Boas maneiras, regrinhas de convivência</t>
+  </si>
+  <si>
+    <t>Emborrachado de calendário personalizável</t>
+  </si>
+  <si>
+    <t>Defina seu cardápio da semana</t>
   </si>
 </sst>
 </file>
@@ -1557,7 +1767,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1579,6 +1789,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1610,7 +1826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1639,6 +1855,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1985,10 +2204,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D252"/>
+  <dimension ref="A1:F252"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,11 +2215,13 @@
     <col min="1" max="1" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="74.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="73.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2" hidden="1"/>
+    <col min="4" max="4" width="46.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="0" style="2" hidden="1"/>
+    <col min="7" max="16384" width="9.140625" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>181</v>
       </c>
@@ -2011,10 +2232,13 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2024,11 +2248,12 @@
       <c r="C2" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="4"/>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2038,11 +2263,12 @@
       <c r="C3" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="4"/>
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2052,11 +2278,12 @@
       <c r="C4" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="4"/>
+      <c r="E4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2066,11 +2293,12 @@
       <c r="C5" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2080,11 +2308,12 @@
       <c r="C6" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
+      <c r="E6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2094,11 +2323,12 @@
       <c r="C7" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="4"/>
+      <c r="E7" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2108,11 +2338,12 @@
       <c r="C8" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="4"/>
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2122,11 +2353,12 @@
       <c r="C9" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="4"/>
+      <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2136,11 +2368,12 @@
       <c r="C10" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+      <c r="E10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2150,11 +2383,12 @@
       <c r="C11" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="4"/>
+      <c r="E11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2164,11 +2398,14 @@
       <c r="C12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2178,11 +2415,14 @@
       <c r="C13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2192,11 +2432,14 @@
       <c r="C14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2206,11 +2449,14 @@
       <c r="C15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2220,11 +2466,14 @@
       <c r="C16" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2234,11 +2483,14 @@
       <c r="C17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2248,11 +2500,14 @@
       <c r="C18" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2262,11 +2517,14 @@
       <c r="C19" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2276,11 +2534,14 @@
       <c r="C20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2290,11 +2551,14 @@
       <c r="C21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2304,25 +2568,31 @@
       <c r="C22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="8" t="s">
+        <v>518</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2332,11 +2602,14 @@
       <c r="C24" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2346,11 +2619,14 @@
       <c r="C25" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2360,11 +2636,14 @@
       <c r="C26" s="10" t="s">
         <v>446</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2374,11 +2653,14 @@
       <c r="C27" s="10" t="s">
         <v>447</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2388,11 +2670,14 @@
       <c r="C28" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2402,11 +2687,14 @@
       <c r="C29" s="10" t="s">
         <v>449</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2416,11 +2704,14 @@
       <c r="C30" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2430,11 +2721,14 @@
       <c r="C31" s="10" t="s">
         <v>451</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2444,11 +2738,14 @@
       <c r="C32" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2458,11 +2755,14 @@
       <c r="C33" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2472,11 +2772,14 @@
       <c r="C34" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2486,11 +2789,14 @@
       <c r="C35" s="10" t="s">
         <v>455</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2500,11 +2806,14 @@
       <c r="C36" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2514,11 +2823,14 @@
       <c r="C37" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2528,11 +2840,14 @@
       <c r="C38" s="10" t="s">
         <v>458</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2542,11 +2857,14 @@
       <c r="C39" s="10" t="s">
         <v>459</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2556,11 +2874,14 @@
       <c r="C40" s="10" t="s">
         <v>460</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2570,11 +2891,14 @@
       <c r="C41" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2584,11 +2908,14 @@
       <c r="C42" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2598,11 +2925,14 @@
       <c r="C43" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2612,11 +2942,14 @@
       <c r="C44" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2626,11 +2959,14 @@
       <c r="C45" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2640,11 +2976,14 @@
       <c r="C46" s="10" t="s">
         <v>466</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2654,11 +2993,14 @@
       <c r="C47" s="10" t="s">
         <v>467</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2668,11 +3010,14 @@
       <c r="C48" s="10" t="s">
         <v>468</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2682,11 +3027,14 @@
       <c r="C49" s="10" t="s">
         <v>469</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2696,11 +3044,14 @@
       <c r="C50" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2710,11 +3061,14 @@
       <c r="C51" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -2724,11 +3078,14 @@
       <c r="C52" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="8" t="s">
+        <v>547</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -2738,11 +3095,14 @@
       <c r="C53" s="10" t="s">
         <v>473</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -2752,11 +3112,14 @@
       <c r="C54" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="8" t="s">
+        <v>548</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -2766,11 +3129,14 @@
       <c r="C55" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -2780,11 +3146,14 @@
       <c r="C56" s="10" t="s">
         <v>476</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -2794,11 +3163,14 @@
       <c r="C57" s="10" t="s">
         <v>477</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="8" t="s">
+        <v>551</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -2808,11 +3180,14 @@
       <c r="C58" s="10" t="s">
         <v>478</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="8" t="s">
+        <v>552</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -2822,11 +3197,14 @@
       <c r="C59" s="10" t="s">
         <v>479</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="8" t="s">
+        <v>553</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -2836,11 +3214,14 @@
       <c r="C60" s="10" t="s">
         <v>480</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -2850,11 +3231,14 @@
       <c r="C61" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="8" t="s">
+        <v>555</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -2864,75 +3248,102 @@
       <c r="C62" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D64" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D65" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D66" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D67" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D68" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>68</v>
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>69</v>
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -2942,11 +3353,14 @@
       <c r="C71" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -2956,11 +3370,14 @@
       <c r="C72" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -2970,11 +3387,14 @@
       <c r="C73" s="11" t="s">
         <v>485</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -2984,11 +3404,14 @@
       <c r="C74" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -2998,11 +3421,14 @@
       <c r="C75" s="11" t="s">
         <v>487</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -3012,11 +3438,14 @@
       <c r="C76" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -3026,11 +3455,14 @@
       <c r="C77" s="11" t="s">
         <v>488</v>
       </c>
-      <c r="D77" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D77" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -3040,11 +3472,14 @@
       <c r="C78" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="D78" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D78" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -3054,11 +3489,14 @@
       <c r="C79" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="D79" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D79" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -3068,11 +3506,14 @@
       <c r="C80" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D80" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -3082,11 +3523,14 @@
       <c r="C81" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D81" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -3096,11 +3540,14 @@
       <c r="C82" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D82" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -3110,11 +3557,14 @@
       <c r="C83" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D83" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -3124,11 +3574,12 @@
       <c r="C84" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D84" s="8"/>
+      <c r="E84" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -3138,11 +3589,12 @@
       <c r="C85" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D85" s="8"/>
+      <c r="E85" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -3152,11 +3604,12 @@
       <c r="C86" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="D86" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D86" s="8"/>
+      <c r="E86" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -3166,11 +3619,12 @@
       <c r="C87" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="D87" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D87" s="8"/>
+      <c r="E87" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -3180,11 +3634,12 @@
       <c r="C88" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="D88" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D88" s="8"/>
+      <c r="E88" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -3194,11 +3649,12 @@
       <c r="C89" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D89" s="8"/>
+      <c r="E89" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -3208,11 +3664,12 @@
       <c r="C90" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D90" s="8"/>
+      <c r="E90" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -3222,11 +3679,12 @@
       <c r="C91" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D91" s="8"/>
+      <c r="E91" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -3236,11 +3694,12 @@
       <c r="C92" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D92" s="8"/>
+      <c r="E92" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -3250,11 +3709,12 @@
       <c r="C93" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D93" s="8"/>
+      <c r="E93" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -3264,11 +3724,12 @@
       <c r="C94" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D94" s="8"/>
+      <c r="E94" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -3278,11 +3739,12 @@
       <c r="C95" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D95" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D95" s="8"/>
+      <c r="E95" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -3292,11 +3754,12 @@
       <c r="C96" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="D96" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D96" s="8"/>
+      <c r="E96" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -3306,11 +3769,12 @@
       <c r="C97" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D97" s="8"/>
+      <c r="E97" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -3320,11 +3784,12 @@
       <c r="C98" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D98" s="8"/>
+      <c r="E98" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -3334,11 +3799,12 @@
       <c r="C99" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D99" s="8"/>
+      <c r="E99" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -3348,11 +3814,12 @@
       <c r="C100" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D100" s="8"/>
+      <c r="E100" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -3362,11 +3829,12 @@
       <c r="C101" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="D101" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D101" s="8"/>
+      <c r="E101" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -3376,11 +3844,12 @@
       <c r="C102" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D102" s="8"/>
+      <c r="E102" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -3390,11 +3859,12 @@
       <c r="C103" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="D103" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D103" s="8"/>
+      <c r="E103" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -3404,11 +3874,12 @@
       <c r="C104" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="D104" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D104" s="8"/>
+      <c r="E104" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -3418,11 +3889,12 @@
       <c r="C105" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D105" s="8"/>
+      <c r="E105" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -3432,11 +3904,12 @@
       <c r="C106" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D106" s="8"/>
+      <c r="E106" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -3446,11 +3919,12 @@
       <c r="C107" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D107" s="8"/>
+      <c r="E107" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -3460,11 +3934,12 @@
       <c r="C108" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D108" s="8"/>
+      <c r="E108" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -3474,11 +3949,12 @@
       <c r="C109" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D109" s="8"/>
+      <c r="E109" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -3488,11 +3964,12 @@
       <c r="C110" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D110" s="8"/>
+      <c r="E110" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -3502,11 +3979,12 @@
       <c r="C111" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D111" s="8"/>
+      <c r="E111" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -3516,11 +3994,12 @@
       <c r="C112" s="8" t="s">
         <v>321</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D112" s="8"/>
+      <c r="E112" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -3530,11 +4009,12 @@
       <c r="C113" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D113" s="8"/>
+      <c r="E113" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -3544,11 +4024,12 @@
       <c r="C114" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D114" s="8"/>
+      <c r="E114" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -3558,11 +4039,12 @@
       <c r="C115" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D115" s="8"/>
+      <c r="E115" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -3572,11 +4054,12 @@
       <c r="C116" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D116" s="8"/>
+      <c r="E116" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -3586,11 +4069,12 @@
       <c r="C117" s="8" t="s">
         <v>326</v>
       </c>
-      <c r="D117" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D117" s="8"/>
+      <c r="E117" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -3600,11 +4084,12 @@
       <c r="C118" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="D118" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D118" s="8"/>
+      <c r="E118" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -3614,11 +4099,12 @@
       <c r="C119" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="D119" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D119" s="8"/>
+      <c r="E119" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -3628,11 +4114,12 @@
       <c r="C120" s="8" t="s">
         <v>329</v>
       </c>
-      <c r="D120" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D120" s="8"/>
+      <c r="E120" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -3642,11 +4129,12 @@
       <c r="C121" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D121" s="8"/>
+      <c r="E121" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -3656,11 +4144,12 @@
       <c r="C122" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D122" s="8"/>
+      <c r="E122" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -3670,11 +4159,12 @@
       <c r="C123" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D123" s="8"/>
+      <c r="E123" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -3684,11 +4174,12 @@
       <c r="C124" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="D124" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D124" s="8"/>
+      <c r="E124" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -3698,11 +4189,12 @@
       <c r="C125" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="D125" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D125" s="8"/>
+      <c r="E125" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -3712,11 +4204,12 @@
       <c r="C126" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="D126" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D126" s="8"/>
+      <c r="E126" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -3726,11 +4219,12 @@
       <c r="C127" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="D127" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D127" s="8"/>
+      <c r="E127" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -3740,11 +4234,12 @@
       <c r="C128" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="D128" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D128" s="8"/>
+      <c r="E128" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -3754,11 +4249,12 @@
       <c r="C129" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D129" s="8"/>
+      <c r="E129" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -3768,11 +4264,12 @@
       <c r="C130" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="D130" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D130" s="8"/>
+      <c r="E130" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -3782,11 +4279,12 @@
       <c r="C131" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="D131" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D131" s="8"/>
+      <c r="E131" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -3796,11 +4294,12 @@
       <c r="C132" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D132" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D132" s="8"/>
+      <c r="E132" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -3810,11 +4309,12 @@
       <c r="C133" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="D133" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D133" s="8"/>
+      <c r="E133" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -3824,11 +4324,12 @@
       <c r="C134" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="D134" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D134" s="8"/>
+      <c r="E134" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -3838,11 +4339,12 @@
       <c r="C135" s="8" t="s">
         <v>344</v>
       </c>
-      <c r="D135" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D135" s="8"/>
+      <c r="E135" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -3852,11 +4354,12 @@
       <c r="C136" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="D136" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D136" s="8"/>
+      <c r="E136" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -3866,11 +4369,12 @@
       <c r="C137" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="D137" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D137" s="8"/>
+      <c r="E137" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -3880,11 +4384,12 @@
       <c r="C138" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="D138" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D138" s="8"/>
+      <c r="E138" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -3894,11 +4399,12 @@
       <c r="C139" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="D139" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D139" s="8"/>
+      <c r="E139" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -3908,11 +4414,12 @@
       <c r="C140" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="D140" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D140" s="8"/>
+      <c r="E140" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -3922,11 +4429,12 @@
       <c r="C141" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="D141" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D141" s="8"/>
+      <c r="E141" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -3936,11 +4444,12 @@
       <c r="C142" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="D142" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D142" s="8"/>
+      <c r="E142" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -3950,11 +4459,12 @@
       <c r="C143" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="D143" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D143" s="8"/>
+      <c r="E143" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -3964,11 +4474,12 @@
       <c r="C144" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D144" s="8"/>
+      <c r="E144" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -3978,11 +4489,12 @@
       <c r="C145" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="D145" s="3" t="s">
+      <c r="D145" s="8"/>
+      <c r="E145" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -3992,11 +4504,12 @@
       <c r="C146" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="D146" s="3" t="s">
+      <c r="D146" s="8"/>
+      <c r="E146" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -4006,11 +4519,12 @@
       <c r="C147" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D147" s="8"/>
+      <c r="E147" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -4020,11 +4534,12 @@
       <c r="C148" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="D148" s="3" t="s">
+      <c r="D148" s="8"/>
+      <c r="E148" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -4034,11 +4549,12 @@
       <c r="C149" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D149" s="8"/>
+      <c r="E149" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -4048,11 +4564,12 @@
       <c r="C150" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="D150" s="8"/>
+      <c r="E150" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -4062,11 +4579,12 @@
       <c r="C151" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="D151" s="8"/>
+      <c r="E151" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -4076,11 +4594,12 @@
       <c r="C152" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="D152" s="3" t="s">
+      <c r="D152" s="8"/>
+      <c r="E152" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -4090,11 +4609,12 @@
       <c r="C153" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="D153" s="3" t="s">
+      <c r="D153" s="8"/>
+      <c r="E153" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -4104,11 +4624,12 @@
       <c r="C154" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D154" s="8"/>
+      <c r="E154" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -4118,11 +4639,12 @@
       <c r="C155" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D155" s="8"/>
+      <c r="E155" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -4132,11 +4654,12 @@
       <c r="C156" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="D156" s="3" t="s">
+      <c r="D156" s="8"/>
+      <c r="E156" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -4146,11 +4669,12 @@
       <c r="C157" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="D157" s="3" t="s">
+      <c r="D157" s="8"/>
+      <c r="E157" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -4160,11 +4684,12 @@
       <c r="C158" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="D158" s="8"/>
+      <c r="E158" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -4174,11 +4699,12 @@
       <c r="C159" s="8" t="s">
         <v>433</v>
       </c>
-      <c r="D159" s="3" t="s">
+      <c r="D159" s="8"/>
+      <c r="E159" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -4188,11 +4714,12 @@
       <c r="C160" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="D160" s="8"/>
+      <c r="E160" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -4202,11 +4729,12 @@
       <c r="C161" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D161" s="8"/>
+      <c r="E161" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -4216,11 +4744,12 @@
       <c r="C162" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="D162" s="3" t="s">
+      <c r="D162" s="8"/>
+      <c r="E162" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -4230,11 +4759,12 @@
       <c r="C163" s="8" t="s">
         <v>437</v>
       </c>
-      <c r="D163" s="3" t="s">
+      <c r="D163" s="8"/>
+      <c r="E163" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -4244,11 +4774,12 @@
       <c r="C164" s="8" t="s">
         <v>438</v>
       </c>
-      <c r="D164" s="3" t="s">
+      <c r="D164" s="8"/>
+      <c r="E164" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -4258,11 +4789,12 @@
       <c r="C165" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="D165" s="3" t="s">
+      <c r="D165" s="8"/>
+      <c r="E165" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -4272,11 +4804,12 @@
       <c r="C166" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="D166" s="3" t="s">
+      <c r="D166" s="8"/>
+      <c r="E166" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -4286,11 +4819,12 @@
       <c r="C167" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="D167" s="3" t="s">
+      <c r="D167" s="8"/>
+      <c r="E167" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -4300,11 +4834,12 @@
       <c r="C168" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="D168" s="8"/>
+      <c r="E168" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -4314,11 +4849,12 @@
       <c r="C169" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="D169" s="3" t="s">
+      <c r="D169" s="8"/>
+      <c r="E169" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -4328,11 +4864,12 @@
       <c r="C170" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="D170" s="3" t="s">
+      <c r="D170" s="8"/>
+      <c r="E170" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>170</v>
       </c>
@@ -4342,11 +4879,12 @@
       <c r="C171" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="D171" s="3" t="s">
+      <c r="D171" s="8"/>
+      <c r="E171" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>171</v>
       </c>
@@ -4356,11 +4894,12 @@
       <c r="C172" s="8" t="s">
         <v>396</v>
       </c>
-      <c r="D172" s="3" t="s">
+      <c r="D172" s="8"/>
+      <c r="E172" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>172</v>
       </c>
@@ -4370,11 +4909,12 @@
       <c r="C173" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="D173" s="3" t="s">
+      <c r="D173" s="8"/>
+      <c r="E173" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>173</v>
       </c>
@@ -4384,11 +4924,12 @@
       <c r="C174" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="D174" s="3" t="s">
+      <c r="D174" s="8"/>
+      <c r="E174" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>174</v>
       </c>
@@ -4398,11 +4939,12 @@
       <c r="C175" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="D175" s="3" t="s">
+      <c r="D175" s="8"/>
+      <c r="E175" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>175</v>
       </c>
@@ -4412,11 +4954,12 @@
       <c r="C176" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="D176" s="3" t="s">
+      <c r="D176" s="8"/>
+      <c r="E176" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>176</v>
       </c>
@@ -4426,11 +4969,12 @@
       <c r="C177" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="D177" s="3" t="s">
+      <c r="D177" s="8"/>
+      <c r="E177" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>177</v>
       </c>
@@ -4440,11 +4984,12 @@
       <c r="C178" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="D178" s="3" t="s">
+      <c r="D178" s="8"/>
+      <c r="E178" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>178</v>
       </c>
@@ -4454,11 +4999,12 @@
       <c r="C179" s="8" t="s">
         <v>402</v>
       </c>
-      <c r="D179" s="3" t="s">
+      <c r="D179" s="8"/>
+      <c r="E179" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>179</v>
       </c>
@@ -4468,11 +5014,12 @@
       <c r="C180" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="D180" s="3" t="s">
+      <c r="D180" s="8"/>
+      <c r="E180" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>180</v>
       </c>
@@ -4482,11 +5029,12 @@
       <c r="C181" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="D181" s="3" t="s">
+      <c r="D181" s="8"/>
+      <c r="E181" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>181</v>
       </c>
@@ -4496,11 +5044,12 @@
       <c r="C182" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="D182" s="3" t="s">
+      <c r="D182" s="8"/>
+      <c r="E182" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>182</v>
       </c>
@@ -4510,11 +5059,12 @@
       <c r="C183" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="D183" s="3" t="s">
+      <c r="D183" s="8"/>
+      <c r="E183" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>183</v>
       </c>
@@ -4524,11 +5074,12 @@
       <c r="C184" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="D184" s="3" t="s">
+      <c r="D184" s="8"/>
+      <c r="E184" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>184</v>
       </c>
@@ -4536,11 +5087,12 @@
         <v>251</v>
       </c>
       <c r="C185" s="9"/>
-      <c r="D185" s="3" t="s">
+      <c r="D185" s="9"/>
+      <c r="E185" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>185</v>
       </c>
@@ -4550,11 +5102,12 @@
       <c r="C186" s="8" t="s">
         <v>408</v>
       </c>
-      <c r="D186" s="3" t="s">
+      <c r="D186" s="8"/>
+      <c r="E186" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>186</v>
       </c>
@@ -4562,11 +5115,12 @@
         <v>253</v>
       </c>
       <c r="C187" s="9"/>
-      <c r="D187" s="3" t="s">
+      <c r="D187" s="9"/>
+      <c r="E187" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>187</v>
       </c>
@@ -4576,11 +5130,12 @@
       <c r="C188" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="D188" s="3" t="s">
+      <c r="D188" s="8"/>
+      <c r="E188" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>188</v>
       </c>
@@ -4590,11 +5145,12 @@
       <c r="C189" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="D189" s="3" t="s">
+      <c r="D189" s="8"/>
+      <c r="E189" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>189</v>
       </c>
@@ -4604,11 +5160,12 @@
       <c r="C190" s="8" t="s">
         <v>411</v>
       </c>
-      <c r="D190" s="3" t="s">
+      <c r="D190" s="8"/>
+      <c r="E190" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>190</v>
       </c>
@@ -4618,11 +5175,12 @@
       <c r="C191" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="D191" s="3" t="s">
+      <c r="D191" s="8"/>
+      <c r="E191" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>191</v>
       </c>
@@ -4632,11 +5190,12 @@
       <c r="C192" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="D192" s="3" t="s">
+      <c r="D192" s="8"/>
+      <c r="E192" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>192</v>
       </c>
@@ -4646,11 +5205,12 @@
       <c r="C193" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="D193" s="3" t="s">
+      <c r="D193" s="8"/>
+      <c r="E193" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>193</v>
       </c>
@@ -4658,11 +5218,12 @@
         <v>260</v>
       </c>
       <c r="C194" s="9"/>
-      <c r="D194" s="3" t="s">
+      <c r="D194" s="9"/>
+      <c r="E194" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>194</v>
       </c>
@@ -4672,11 +5233,12 @@
       <c r="C195" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="D195" s="3" t="s">
+      <c r="D195" s="8"/>
+      <c r="E195" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>195</v>
       </c>
@@ -4686,11 +5248,12 @@
       <c r="C196" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="D196" s="3" t="s">
+      <c r="D196" s="8"/>
+      <c r="E196" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>196</v>
       </c>
@@ -4700,11 +5263,12 @@
       <c r="C197" s="8" t="s">
         <v>417</v>
       </c>
-      <c r="D197" s="3" t="s">
+      <c r="D197" s="8"/>
+      <c r="E197" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>197</v>
       </c>
@@ -4714,11 +5278,12 @@
       <c r="C198" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D198" s="3" t="s">
+      <c r="D198" s="8"/>
+      <c r="E198" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>198</v>
       </c>
@@ -4728,11 +5293,12 @@
       <c r="C199" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D199" s="3" t="s">
+      <c r="D199" s="8"/>
+      <c r="E199" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>199</v>
       </c>
@@ -4742,11 +5308,12 @@
       <c r="C200" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D200" s="3" t="s">
+      <c r="D200" s="8"/>
+      <c r="E200" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>200</v>
       </c>
@@ -4756,11 +5323,12 @@
       <c r="C201" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D201" s="3" t="s">
+      <c r="D201" s="8"/>
+      <c r="E201" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>201</v>
       </c>
@@ -4770,11 +5338,12 @@
       <c r="C202" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D202" s="3" t="s">
+      <c r="D202" s="8"/>
+      <c r="E202" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>202</v>
       </c>
@@ -4784,11 +5353,12 @@
       <c r="C203" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D203" s="3" t="s">
+      <c r="D203" s="8"/>
+      <c r="E203" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>203</v>
       </c>
@@ -4798,11 +5368,12 @@
       <c r="C204" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D204" s="3" t="s">
+      <c r="D204" s="8"/>
+      <c r="E204" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>204</v>
       </c>
@@ -4812,11 +5383,12 @@
       <c r="C205" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D205" s="3" t="s">
+      <c r="D205" s="8"/>
+      <c r="E205" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>205</v>
       </c>
@@ -4826,11 +5398,12 @@
       <c r="C206" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D206" s="3" t="s">
+      <c r="D206" s="8"/>
+      <c r="E206" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>206</v>
       </c>
@@ -4840,11 +5413,12 @@
       <c r="C207" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="D207" s="3" t="s">
+      <c r="D207" s="8"/>
+      <c r="E207" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>207</v>
       </c>
@@ -4854,11 +5428,12 @@
       <c r="C208" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="D208" s="3" t="s">
+      <c r="D208" s="8"/>
+      <c r="E208" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>208</v>
       </c>
@@ -4868,11 +5443,12 @@
       <c r="C209" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="D209" s="3" t="s">
+      <c r="D209" s="8"/>
+      <c r="E209" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>209</v>
       </c>
@@ -4882,11 +5458,12 @@
       <c r="C210" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="D210" s="3" t="s">
+      <c r="D210" s="8"/>
+      <c r="E210" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>210</v>
       </c>
@@ -4896,11 +5473,12 @@
       <c r="C211" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="D211" s="3" t="s">
+      <c r="D211" s="8"/>
+      <c r="E211" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>211</v>
       </c>
@@ -4910,11 +5488,12 @@
       <c r="C212" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="D212" s="3" t="s">
+      <c r="D212" s="8"/>
+      <c r="E212" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>212</v>
       </c>
@@ -4924,11 +5503,12 @@
       <c r="C213" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="D213" s="3" t="s">
+      <c r="D213" s="8"/>
+      <c r="E213" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>213</v>
       </c>
@@ -4938,11 +5518,12 @@
       <c r="C214" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="D214" s="3" t="s">
+      <c r="D214" s="8"/>
+      <c r="E214" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>214</v>
       </c>
@@ -4952,11 +5533,12 @@
       <c r="C215" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="D215" s="3" t="s">
+      <c r="D215" s="8"/>
+      <c r="E215" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>215</v>
       </c>
@@ -4966,11 +5548,12 @@
       <c r="C216" s="8" t="s">
         <v>382</v>
       </c>
-      <c r="D216" s="3" t="s">
+      <c r="D216" s="8"/>
+      <c r="E216" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>216</v>
       </c>
@@ -4980,11 +5563,12 @@
       <c r="C217" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="D217" s="3" t="s">
+      <c r="D217" s="8"/>
+      <c r="E217" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>217</v>
       </c>
@@ -4994,11 +5578,12 @@
       <c r="C218" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="D218" s="3" t="s">
+      <c r="D218" s="8"/>
+      <c r="E218" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>218</v>
       </c>
@@ -5008,11 +5593,12 @@
       <c r="C219" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="D219" s="3" t="s">
+      <c r="D219" s="8"/>
+      <c r="E219" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>219</v>
       </c>
@@ -5022,11 +5608,12 @@
       <c r="C220" s="8" t="s">
         <v>386</v>
       </c>
-      <c r="D220" s="3" t="s">
+      <c r="D220" s="8"/>
+      <c r="E220" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>220</v>
       </c>
@@ -5036,11 +5623,12 @@
       <c r="C221" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="D221" s="3" t="s">
+      <c r="D221" s="8"/>
+      <c r="E221" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>221</v>
       </c>
@@ -5050,11 +5638,12 @@
       <c r="C222" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="D222" s="3" t="s">
+      <c r="D222" s="8"/>
+      <c r="E222" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>222</v>
       </c>
@@ -5064,11 +5653,12 @@
       <c r="C223" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="D223" s="3" t="s">
+      <c r="D223" s="8"/>
+      <c r="E223" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>223</v>
       </c>
@@ -5078,11 +5668,12 @@
       <c r="C224" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="D224" s="3" t="s">
+      <c r="D224" s="8"/>
+      <c r="E224" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>224</v>
       </c>
@@ -5092,11 +5683,12 @@
       <c r="C225" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="D225" s="3" t="s">
+      <c r="D225" s="8"/>
+      <c r="E225" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="226" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>225</v>
       </c>
@@ -5106,11 +5698,12 @@
       <c r="C226" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="D226" s="3" t="s">
+      <c r="D226" s="8"/>
+      <c r="E226" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" s="5">
         <v>226</v>
       </c>
@@ -5120,11 +5713,14 @@
       <c r="C227" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="D227" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D227" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="E227" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" s="5">
         <v>227</v>
       </c>
@@ -5134,11 +5730,14 @@
       <c r="C228" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="D228" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D228" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="E228" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" s="5">
         <v>228</v>
       </c>
@@ -5148,11 +5747,14 @@
       <c r="C229" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="D229" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D229" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="E229" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" s="5">
         <v>229</v>
       </c>
@@ -5162,11 +5764,14 @@
       <c r="C230" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="D230" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D230" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="E230" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="5">
         <v>230</v>
       </c>
@@ -5176,11 +5781,14 @@
       <c r="C231" s="7" t="s">
         <v>494</v>
       </c>
-      <c r="D231" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D231" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="E231" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" s="5">
         <v>231</v>
       </c>
@@ -5190,11 +5798,14 @@
       <c r="C232" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="D232" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D232" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="E232" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
         <v>232</v>
       </c>
@@ -5204,11 +5815,12 @@
       <c r="C233" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="D233" s="3" t="s">
+      <c r="D233" s="8"/>
+      <c r="E233" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>233</v>
       </c>
@@ -5218,11 +5830,12 @@
       <c r="C234" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="D234" s="3" t="s">
+      <c r="D234" s="8"/>
+      <c r="E234" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>234</v>
       </c>
@@ -5232,11 +5845,12 @@
       <c r="C235" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="D235" s="3" t="s">
+      <c r="D235" s="8"/>
+      <c r="E235" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>235</v>
       </c>
@@ -5246,11 +5860,12 @@
       <c r="C236" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="D236" s="3" t="s">
+      <c r="D236" s="8"/>
+      <c r="E236" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>236</v>
       </c>
@@ -5260,11 +5875,12 @@
       <c r="C237" s="8" t="s">
         <v>364</v>
       </c>
-      <c r="D237" s="3" t="s">
+      <c r="D237" s="8"/>
+      <c r="E237" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="238" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="3">
         <v>237</v>
       </c>
@@ -5274,11 +5890,12 @@
       <c r="C238" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="D238" s="3" t="s">
+      <c r="D238" s="8"/>
+      <c r="E238" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="3">
         <v>238</v>
       </c>
@@ -5288,11 +5905,12 @@
       <c r="C239" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="D239" s="3" t="s">
+      <c r="D239" s="8"/>
+      <c r="E239" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>239</v>
       </c>
@@ -5302,11 +5920,12 @@
       <c r="C240" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="D240" s="3" t="s">
+      <c r="D240" s="8"/>
+      <c r="E240" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="3">
         <v>240</v>
       </c>
@@ -5316,11 +5935,12 @@
       <c r="C241" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="D241" s="3" t="s">
+      <c r="D241" s="8"/>
+      <c r="E241" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="3">
         <v>241</v>
       </c>
@@ -5330,11 +5950,12 @@
       <c r="C242" s="8" t="s">
         <v>370</v>
       </c>
-      <c r="D242" s="3" t="s">
+      <c r="D242" s="8"/>
+      <c r="E242" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="3">
         <v>242</v>
       </c>
@@ -5344,11 +5965,12 @@
       <c r="C243" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="D243" s="3" t="s">
+      <c r="D243" s="8"/>
+      <c r="E243" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="3">
         <v>243</v>
       </c>
@@ -5358,11 +5980,12 @@
       <c r="C244" s="8" t="s">
         <v>372</v>
       </c>
-      <c r="D244" s="3" t="s">
+      <c r="D244" s="8"/>
+      <c r="E244" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="3">
         <v>244</v>
       </c>
@@ -5372,11 +5995,12 @@
       <c r="C245" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="D245" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D245" s="8"/>
+      <c r="E245" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="3">
         <v>245</v>
       </c>
@@ -5386,11 +6010,12 @@
       <c r="C246" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="D246" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D246" s="8"/>
+      <c r="E246" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="3">
         <v>246</v>
       </c>
@@ -5400,11 +6025,12 @@
       <c r="C247" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="D247" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D247" s="8"/>
+      <c r="E247" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="3">
         <v>247</v>
       </c>
@@ -5414,11 +6040,12 @@
       <c r="C248" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="D248" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D248" s="8"/>
+      <c r="E248" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="3">
         <v>248</v>
       </c>
@@ -5428,11 +6055,12 @@
       <c r="C249" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="D249" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D249" s="8"/>
+      <c r="E249" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="3">
         <v>248</v>
       </c>
@@ -5442,9 +6070,10 @@
       <c r="C250" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D250" s="3"/>
-    </row>
-    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D250" s="8"/>
+      <c r="E250" s="3"/>
+    </row>
+    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="3">
         <v>249</v>
       </c>
@@ -5454,11 +6083,12 @@
       <c r="C251" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="D251" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D251" s="8"/>
+      <c r="E251" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="3">
         <v>250</v>
       </c>
@@ -5468,23 +6098,24 @@
       <c r="C252" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="D252" s="3" t="s">
+      <c r="D252" s="9"/>
+      <c r="E252" s="3" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D252" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
-    <filterColumn colId="3">
+  <autoFilter ref="A1:E252" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
+    <filterColumn colId="4">
       <filters>
         <filter val="BANNERS EDUCATIVOS"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D252">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E252">
       <sortCondition ref="A1:A252"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C2:C3">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C2:D3">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
teste 5 - finalizado, 100% funcional com os banners
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28503F27-A153-423C-BF83-4AC4BE1C7FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4618250D-76D0-46BB-93BE-50C9B0220A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
@@ -2179,8 +2179,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,7 +2572,7 @@
       <c r="B24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="12" t="s">
         <v>444</v>
       </c>
       <c r="D24" s="8" t="s">

</xml_diff>

<commit_message>
finalizei de  adicionar todos os produtos de banners
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4618250D-76D0-46BB-93BE-50C9B0220A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFAE606-3029-41CC-9754-BAFD76D57D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
@@ -2179,8 +2179,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,7 +2589,7 @@
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="12" t="s">
         <v>445</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -2606,7 +2606,7 @@
       <c r="B26" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="12" t="s">
         <v>446</v>
       </c>
       <c r="D26" s="8" t="s">
@@ -2623,7 +2623,7 @@
       <c r="B27" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="12" t="s">
         <v>447</v>
       </c>
       <c r="D27" s="8" t="s">
@@ -2640,7 +2640,7 @@
       <c r="B28" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="12" t="s">
         <v>448</v>
       </c>
       <c r="D28" s="8" t="s">
@@ -2657,7 +2657,7 @@
       <c r="B29" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="12" t="s">
         <v>449</v>
       </c>
       <c r="D29" s="8" t="s">

</xml_diff>

<commit_message>
finalizei a adiçãõ dos produtos de materiais esportivos
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFAE606-3029-41CC-9754-BAFD76D57D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BCDF14-D63C-4ED6-9D20-50FFEE3D4B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="557">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -185,9 +185,6 @@
     <t>024 - banner bioma do brasil site.jpg</t>
   </si>
   <si>
-    <t>025 - banner boa convivencia site.webp</t>
-  </si>
-  <si>
     <t>026 - banner calendario site.webp</t>
   </si>
   <si>
@@ -1379,9 +1376,6 @@
     <t>24-banner-bioma-do-brasil-site.html</t>
   </si>
   <si>
-    <t>25-banner-boa-convivencia-site.html</t>
-  </si>
-  <si>
     <t>26-banner-calendario-site.html</t>
   </si>
   <si>
@@ -1577,9 +1571,6 @@
     <t>Banner bioma do Brasil</t>
   </si>
   <si>
-    <t>Banner boa convivência</t>
-  </si>
-  <si>
     <t>Banner calendário</t>
   </si>
   <si>
@@ -1682,27 +1673,6 @@
     <t>Banner sinais de pontuação</t>
   </si>
   <si>
-    <t>Banner sistema muscular</t>
-  </si>
-  <si>
-    <t>Banner subtração</t>
-  </si>
-  <si>
-    <t>Banner tabela periódica</t>
-  </si>
-  <si>
-    <t>Banner tabuada</t>
-  </si>
-  <si>
-    <t>Banner texto narrativo</t>
-  </si>
-  <si>
-    <t>Banner vogais e consoantes</t>
-  </si>
-  <si>
-    <t>Banner vogais</t>
-  </si>
-  <si>
     <t>Boas maneiras, regrinhas de convivência</t>
   </si>
   <si>
@@ -1710,6 +1680,36 @@
   </si>
   <si>
     <t>Defina seu cardápio da semana</t>
+  </si>
+  <si>
+    <t>Caixa de caneta com 50 unidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jogo De Botão Brasileirão Xalingo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jogo De Ping Pong Simples - Xalingo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesa de pebolim Xalingo Super copa cor verde  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesa E Jogo De Futebol De Botão com 2 Marcadores Xalingo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesa Para Ping Pong  Tênis De Mesa Azul com Pés Dobráveis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabela Basquete Mdf 9mm Aro 36 Cm Basketball Master Xalingo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabela De Basquete infantil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xalingo tabela cesta de basquete com bola </t>
+  </si>
+  <si>
+    <t>Conjunto Completo - Tênis De Mesa - Ping Pong - Rede e Raquete</t>
   </si>
 </sst>
 </file>
@@ -1740,7 +1740,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1761,13 +1761,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1799,7 +1793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1828,9 +1822,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2179,24 +2170,24 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D254" sqref="D254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="73.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="57.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="73.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
@@ -2205,7 +2196,7 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -2216,10 +2207,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
@@ -2231,10 +2222,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="3" t="s">
@@ -2246,10 +2237,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3" t="s">
@@ -2261,10 +2252,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
@@ -2276,10 +2267,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
@@ -2291,10 +2282,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
@@ -2306,10 +2297,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
@@ -2321,10 +2312,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
@@ -2336,10 +2327,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
@@ -2351,17 +2342,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2372,13 +2363,13 @@
         <v>23</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2389,13 +2380,13 @@
         <v>24</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2406,13 +2397,13 @@
         <v>25</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2423,13 +2414,13 @@
         <v>26</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2440,13 +2431,13 @@
         <v>27</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2457,13 +2448,13 @@
         <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -2474,13 +2465,13 @@
         <v>29</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2491,13 +2482,13 @@
         <v>30</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2508,13 +2499,13 @@
         <v>31</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2525,13 +2516,13 @@
         <v>32</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2542,670 +2533,662 @@
         <v>33</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>443</v>
+      <c r="C23" s="10" t="s">
+        <v>442</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>444</v>
+      <c r="C24" s="10" t="s">
+        <v>443</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>445</v>
+      <c r="C25" s="10" t="s">
+        <v>444</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>446</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>512</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>447</v>
+        <v>48</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>445</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>448</v>
+        <v>49</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>446</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>449</v>
+        <v>50</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>447</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>4</v>
@@ -3216,10 +3199,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D62" s="9" t="s">
         <v>547</v>
@@ -3234,9 +3217,7 @@
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
-      <c r="D63" s="9" t="s">
-        <v>548</v>
-      </c>
+      <c r="D63" s="9"/>
       <c r="E63" s="3"/>
     </row>
     <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3245,9 +3226,7 @@
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
-      <c r="D64" s="9" t="s">
-        <v>549</v>
-      </c>
+      <c r="D64" s="9"/>
       <c r="E64" s="3"/>
     </row>
     <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3256,9 +3235,7 @@
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
-      <c r="D65" s="9" t="s">
-        <v>550</v>
-      </c>
+      <c r="D65" s="9"/>
       <c r="E65" s="3"/>
     </row>
     <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3267,9 +3244,7 @@
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
-      <c r="D66" s="9" t="s">
-        <v>551</v>
-      </c>
+      <c r="D66" s="9"/>
       <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3278,9 +3253,7 @@
       </c>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
-      <c r="D67" s="9" t="s">
-        <v>552</v>
-      </c>
+      <c r="D67" s="9"/>
       <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3289,9 +3262,7 @@
       </c>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
-      <c r="D68" s="9" t="s">
-        <v>553</v>
-      </c>
+      <c r="D68" s="9"/>
       <c r="E68" s="3"/>
     </row>
     <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3300,9 +3271,7 @@
       </c>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
-      <c r="D69" s="9" t="s">
-        <v>503</v>
-      </c>
+      <c r="D69" s="9"/>
       <c r="E69" s="3"/>
     </row>
     <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -3311,126 +3280,110 @@
       </c>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
-      <c r="D70" s="9" t="s">
-        <v>509</v>
-      </c>
+      <c r="D70" s="9"/>
       <c r="E70" s="3"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>483</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>515</v>
-      </c>
+        <v>481</v>
+      </c>
+      <c r="D71" s="9"/>
       <c r="E71" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>484</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>554</v>
-      </c>
+        <v>482</v>
+      </c>
+      <c r="D72" s="9"/>
       <c r="E72" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>485</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>555</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="D73" s="9"/>
       <c r="E73" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>486</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>556</v>
-      </c>
+        <v>484</v>
+      </c>
+      <c r="D74" s="9"/>
       <c r="E74" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>487</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>551</v>
-      </c>
+        <v>485</v>
+      </c>
+      <c r="D75" s="9"/>
       <c r="E75" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="D76" s="9" t="s">
-        <v>552</v>
-      </c>
+        <v>487</v>
+      </c>
+      <c r="D76" s="9"/>
       <c r="E76" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>488</v>
-      </c>
-      <c r="D77" s="9" t="s">
-        <v>553</v>
-      </c>
+        <v>486</v>
+      </c>
+      <c r="D77" s="9"/>
       <c r="E77" s="3" t="s">
         <v>4</v>
       </c>
@@ -3440,14 +3393,12 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>503</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="D78" s="7"/>
       <c r="E78" s="3" t="s">
         <v>1</v>
       </c>
@@ -3457,14 +3408,12 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>509</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="D79" s="7"/>
       <c r="E79" s="3" t="s">
         <v>1</v>
       </c>
@@ -3474,14 +3423,12 @@
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>515</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D80" s="7"/>
       <c r="E80" s="3" t="s">
         <v>1</v>
       </c>
@@ -3491,14 +3438,12 @@
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>554</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="D81" s="7"/>
       <c r="E81" s="3" t="s">
         <v>1</v>
       </c>
@@ -3508,14 +3453,12 @@
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>555</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="D82" s="7"/>
       <c r="E82" s="3" t="s">
         <v>1</v>
       </c>
@@ -3525,14 +3468,12 @@
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>556</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="D83" s="7"/>
       <c r="E83" s="3" t="s">
         <v>1</v>
       </c>
@@ -3542,10 +3483,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="3" t="s">
@@ -3557,10 +3498,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="3" t="s">
@@ -3572,10 +3513,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="3" t="s">
@@ -3587,10 +3528,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D87" s="8"/>
       <c r="E87" s="3" t="s">
@@ -3602,10 +3543,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="3" t="s">
@@ -3617,10 +3558,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="3" t="s">
@@ -3632,10 +3573,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="3" t="s">
@@ -3647,10 +3588,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="3" t="s">
@@ -3662,10 +3603,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D92" s="8"/>
       <c r="E92" s="3" t="s">
@@ -3677,10 +3618,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="3" t="s">
@@ -3692,10 +3633,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="3" t="s">
@@ -3707,10 +3648,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D95" s="8"/>
       <c r="E95" s="3" t="s">
@@ -3722,10 +3663,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D96" s="8"/>
       <c r="E96" s="3" t="s">
@@ -3737,10 +3678,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="3" t="s">
@@ -3752,10 +3693,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="3" t="s">
@@ -3767,10 +3708,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="3" t="s">
@@ -3782,10 +3723,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="3" t="s">
@@ -3797,10 +3738,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D101" s="8"/>
       <c r="E101" s="3" t="s">
@@ -3812,10 +3753,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D102" s="8"/>
       <c r="E102" s="3" t="s">
@@ -3827,10 +3768,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D103" s="8"/>
       <c r="E103" s="3" t="s">
@@ -3842,10 +3783,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D104" s="8"/>
       <c r="E104" s="3" t="s">
@@ -3857,10 +3798,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="3" t="s">
@@ -3872,10 +3813,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D106" s="8"/>
       <c r="E106" s="3" t="s">
@@ -3887,10 +3828,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D107" s="8"/>
       <c r="E107" s="3" t="s">
@@ -3902,10 +3843,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D108" s="8"/>
       <c r="E108" s="3" t="s">
@@ -3917,10 +3858,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D109" s="8"/>
       <c r="E109" s="3" t="s">
@@ -3932,10 +3873,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D110" s="8"/>
       <c r="E110" s="3" t="s">
@@ -3947,10 +3888,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D111" s="8"/>
       <c r="E111" s="3" t="s">
@@ -3962,10 +3903,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="3" t="s">
@@ -3977,10 +3918,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D113" s="8"/>
       <c r="E113" s="3" t="s">
@@ -3992,10 +3933,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D114" s="8"/>
       <c r="E114" s="3" t="s">
@@ -4007,10 +3948,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D115" s="8"/>
       <c r="E115" s="3" t="s">
@@ -4022,10 +3963,10 @@
         <v>115</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D116" s="8"/>
       <c r="E116" s="3" t="s">
@@ -4037,10 +3978,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="3" t="s">
@@ -4052,10 +3993,10 @@
         <v>117</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D118" s="8"/>
       <c r="E118" s="3" t="s">
@@ -4067,10 +4008,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="3" t="s">
@@ -4082,10 +4023,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D120" s="8"/>
       <c r="E120" s="3" t="s">
@@ -4097,10 +4038,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D121" s="8"/>
       <c r="E121" s="3" t="s">
@@ -4112,10 +4053,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D122" s="8"/>
       <c r="E122" s="3" t="s">
@@ -4127,10 +4068,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D123" s="8"/>
       <c r="E123" s="3" t="s">
@@ -4142,10 +4083,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D124" s="8"/>
       <c r="E124" s="3" t="s">
@@ -4157,10 +4098,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D125" s="8"/>
       <c r="E125" s="3" t="s">
@@ -4172,10 +4113,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="3" t="s">
@@ -4187,10 +4128,10 @@
         <v>126</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D127" s="8"/>
       <c r="E127" s="3" t="s">
@@ -4202,10 +4143,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="3" t="s">
@@ -4217,10 +4158,10 @@
         <v>128</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="3" t="s">
@@ -4232,10 +4173,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="3" t="s">
@@ -4247,10 +4188,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D131" s="8"/>
       <c r="E131" s="3" t="s">
@@ -4262,10 +4203,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D132" s="8"/>
       <c r="E132" s="3" t="s">
@@ -4277,10 +4218,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D133" s="8"/>
       <c r="E133" s="3" t="s">
@@ -4292,10 +4233,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D134" s="8"/>
       <c r="E134" s="3" t="s">
@@ -4307,10 +4248,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D135" s="8"/>
       <c r="E135" s="3" t="s">
@@ -4322,10 +4263,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D136" s="8"/>
       <c r="E136" s="3" t="s">
@@ -4337,10 +4278,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D137" s="8"/>
       <c r="E137" s="3" t="s">
@@ -4352,10 +4293,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D138" s="8"/>
       <c r="E138" s="3" t="s">
@@ -4367,10 +4308,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D139" s="8"/>
       <c r="E139" s="3" t="s">
@@ -4382,10 +4323,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="3" t="s">
@@ -4397,10 +4338,10 @@
         <v>140</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D141" s="8"/>
       <c r="E141" s="3" t="s">
@@ -4412,10 +4353,10 @@
         <v>141</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D142" s="8"/>
       <c r="E142" s="3" t="s">
@@ -4427,10 +4368,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D143" s="8"/>
       <c r="E143" s="3" t="s">
@@ -4442,10 +4383,10 @@
         <v>143</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D144" s="8"/>
       <c r="E144" s="3" t="s">
@@ -4457,10 +4398,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D145" s="8"/>
       <c r="E145" s="3" t="s">
@@ -4472,10 +4413,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D146" s="8"/>
       <c r="E146" s="3" t="s">
@@ -4487,10 +4428,10 @@
         <v>146</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D147" s="8"/>
       <c r="E147" s="3" t="s">
@@ -4502,10 +4443,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D148" s="8"/>
       <c r="E148" s="3" t="s">
@@ -4517,10 +4458,10 @@
         <v>148</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D149" s="8"/>
       <c r="E149" s="3" t="s">
@@ -4532,10 +4473,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D150" s="8"/>
       <c r="E150" s="3" t="s">
@@ -4547,10 +4488,10 @@
         <v>150</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D151" s="8"/>
       <c r="E151" s="3" t="s">
@@ -4562,10 +4503,10 @@
         <v>151</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D152" s="8"/>
       <c r="E152" s="3" t="s">
@@ -4577,10 +4518,10 @@
         <v>152</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D153" s="8"/>
       <c r="E153" s="3" t="s">
@@ -4592,10 +4533,10 @@
         <v>153</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D154" s="8"/>
       <c r="E154" s="3" t="s">
@@ -4607,10 +4548,10 @@
         <v>154</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D155" s="8"/>
       <c r="E155" s="3" t="s">
@@ -4622,10 +4563,10 @@
         <v>155</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D156" s="8"/>
       <c r="E156" s="3" t="s">
@@ -4637,10 +4578,10 @@
         <v>156</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D157" s="8"/>
       <c r="E157" s="3" t="s">
@@ -4652,10 +4593,10 @@
         <v>157</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D158" s="8"/>
       <c r="E158" s="3" t="s">
@@ -4667,10 +4608,10 @@
         <v>158</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D159" s="8"/>
       <c r="E159" s="3" t="s">
@@ -4682,10 +4623,10 @@
         <v>159</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D160" s="8"/>
       <c r="E160" s="3" t="s">
@@ -4697,10 +4638,10 @@
         <v>160</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D161" s="8"/>
       <c r="E161" s="3" t="s">
@@ -4712,10 +4653,10 @@
         <v>161</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D162" s="8"/>
       <c r="E162" s="3" t="s">
@@ -4727,10 +4668,10 @@
         <v>162</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D163" s="8"/>
       <c r="E163" s="3" t="s">
@@ -4742,10 +4683,10 @@
         <v>163</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D164" s="8"/>
       <c r="E164" s="3" t="s">
@@ -4757,10 +4698,10 @@
         <v>164</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D165" s="8"/>
       <c r="E165" s="3" t="s">
@@ -4772,10 +4713,10 @@
         <v>165</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D166" s="8"/>
       <c r="E166" s="3" t="s">
@@ -4787,10 +4728,10 @@
         <v>166</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D167" s="8"/>
       <c r="E167" s="3" t="s">
@@ -4802,10 +4743,10 @@
         <v>167</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D168" s="8"/>
       <c r="E168" s="3" t="s">
@@ -4817,10 +4758,10 @@
         <v>168</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D169" s="8"/>
       <c r="E169" s="3" t="s">
@@ -4832,10 +4773,10 @@
         <v>169</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D170" s="8"/>
       <c r="E170" s="3" t="s">
@@ -4847,10 +4788,10 @@
         <v>170</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D171" s="8"/>
       <c r="E171" s="3" t="s">
@@ -4862,10 +4803,10 @@
         <v>171</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D172" s="8"/>
       <c r="E172" s="3" t="s">
@@ -4877,10 +4818,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D173" s="8"/>
       <c r="E173" s="3" t="s">
@@ -4892,10 +4833,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D174" s="8"/>
       <c r="E174" s="3" t="s">
@@ -4907,10 +4848,10 @@
         <v>174</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D175" s="8"/>
       <c r="E175" s="3" t="s">
@@ -4922,10 +4863,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D176" s="8"/>
       <c r="E176" s="3" t="s">
@@ -4937,10 +4878,10 @@
         <v>176</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D177" s="8"/>
       <c r="E177" s="3" t="s">
@@ -4952,10 +4893,10 @@
         <v>177</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D178" s="8"/>
       <c r="E178" s="3" t="s">
@@ -4967,10 +4908,10 @@
         <v>178</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D179" s="8"/>
       <c r="E179" s="3" t="s">
@@ -4982,10 +4923,10 @@
         <v>179</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D180" s="8"/>
       <c r="E180" s="3" t="s">
@@ -4997,10 +4938,10 @@
         <v>180</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D181" s="8"/>
       <c r="E181" s="3" t="s">
@@ -5012,10 +4953,10 @@
         <v>181</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D182" s="8"/>
       <c r="E182" s="3" t="s">
@@ -5027,10 +4968,10 @@
         <v>182</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D183" s="8"/>
       <c r="E183" s="3" t="s">
@@ -5042,10 +4983,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D184" s="8"/>
       <c r="E184" s="3" t="s">
@@ -5057,7 +4998,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C185" s="9"/>
       <c r="D185" s="9"/>
@@ -5070,10 +5011,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D186" s="8"/>
       <c r="E186" s="3" t="s">
@@ -5085,7 +5026,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C187" s="9"/>
       <c r="D187" s="9"/>
@@ -5098,10 +5039,10 @@
         <v>187</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D188" s="8"/>
       <c r="E188" s="3" t="s">
@@ -5113,10 +5054,10 @@
         <v>188</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D189" s="8"/>
       <c r="E189" s="3" t="s">
@@ -5128,10 +5069,10 @@
         <v>189</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D190" s="8"/>
       <c r="E190" s="3" t="s">
@@ -5143,10 +5084,10 @@
         <v>190</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D191" s="8"/>
       <c r="E191" s="3" t="s">
@@ -5158,10 +5099,10 @@
         <v>191</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D192" s="8"/>
       <c r="E192" s="3" t="s">
@@ -5173,10 +5114,10 @@
         <v>192</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D193" s="8"/>
       <c r="E193" s="3" t="s">
@@ -5188,7 +5129,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C194" s="9"/>
       <c r="D194" s="9"/>
@@ -5201,10 +5142,10 @@
         <v>194</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D195" s="8"/>
       <c r="E195" s="3" t="s">
@@ -5216,10 +5157,10 @@
         <v>195</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D196" s="8"/>
       <c r="E196" s="3" t="s">
@@ -5231,147 +5172,165 @@
         <v>196</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D197" s="8"/>
       <c r="E197" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>197</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C198" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D198" s="8"/>
+      <c r="D198" s="8" t="s">
+        <v>556</v>
+      </c>
       <c r="E198" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>198</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C199" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D199" s="8"/>
+      <c r="D199" s="8" t="s">
+        <v>548</v>
+      </c>
       <c r="E199" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>199</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C200" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D200" s="8"/>
+      <c r="D200" s="8" t="s">
+        <v>549</v>
+      </c>
       <c r="E200" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>200</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C201" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D201" s="8"/>
+      <c r="D201" s="8" t="s">
+        <v>550</v>
+      </c>
       <c r="E201" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>201</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C202" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D202" s="8"/>
+      <c r="D202" s="8" t="s">
+        <v>551</v>
+      </c>
       <c r="E202" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>202</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C203" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D203" s="8"/>
+      <c r="D203" s="8" t="s">
+        <v>552</v>
+      </c>
       <c r="E203" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>203</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C204" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D204" s="8"/>
+      <c r="D204" s="8" t="s">
+        <v>553</v>
+      </c>
       <c r="E204" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>204</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C205" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D205" s="8"/>
+      <c r="D205" s="8" t="s">
+        <v>554</v>
+      </c>
       <c r="E205" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>205</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C206" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D206" s="8"/>
+      <c r="D206" s="8" t="s">
+        <v>555</v>
+      </c>
       <c r="E206" s="3" t="s">
         <v>7</v>
       </c>
@@ -5381,10 +5340,10 @@
         <v>206</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D207" s="8"/>
       <c r="E207" s="3" t="s">
@@ -5396,10 +5355,10 @@
         <v>207</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D208" s="8"/>
       <c r="E208" s="3" t="s">
@@ -5411,10 +5370,10 @@
         <v>208</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C209" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D209" s="8"/>
       <c r="E209" s="3" t="s">
@@ -5426,10 +5385,10 @@
         <v>209</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D210" s="8"/>
       <c r="E210" s="3" t="s">
@@ -5441,10 +5400,10 @@
         <v>210</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D211" s="8"/>
       <c r="E211" s="3" t="s">
@@ -5456,10 +5415,10 @@
         <v>211</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C212" s="8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D212" s="8"/>
       <c r="E212" s="3" t="s">
@@ -5471,10 +5430,10 @@
         <v>212</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D213" s="8"/>
       <c r="E213" s="3" t="s">
@@ -5486,10 +5445,10 @@
         <v>213</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C214" s="8" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D214" s="8"/>
       <c r="E214" s="3" t="s">
@@ -5501,10 +5460,10 @@
         <v>214</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C215" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D215" s="8"/>
       <c r="E215" s="3" t="s">
@@ -5516,10 +5475,10 @@
         <v>215</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C216" s="8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D216" s="8"/>
       <c r="E216" s="3" t="s">
@@ -5531,10 +5490,10 @@
         <v>216</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D217" s="8"/>
       <c r="E217" s="3" t="s">
@@ -5546,10 +5505,10 @@
         <v>217</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D218" s="8"/>
       <c r="E218" s="3" t="s">
@@ -5561,10 +5520,10 @@
         <v>218</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C219" s="8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D219" s="8"/>
       <c r="E219" s="3" t="s">
@@ -5576,10 +5535,10 @@
         <v>219</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C220" s="8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D220" s="8"/>
       <c r="E220" s="3" t="s">
@@ -5591,10 +5550,10 @@
         <v>220</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D221" s="8"/>
       <c r="E221" s="3" t="s">
@@ -5606,10 +5565,10 @@
         <v>221</v>
       </c>
       <c r="B222" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C222" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D222" s="8"/>
       <c r="E222" s="3" t="s">
@@ -5621,10 +5580,10 @@
         <v>222</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C223" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D223" s="8"/>
       <c r="E223" s="3" t="s">
@@ -5636,10 +5595,10 @@
         <v>223</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C224" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D224" s="8"/>
       <c r="E224" s="3" t="s">
@@ -5651,10 +5610,10 @@
         <v>224</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C225" s="8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D225" s="8"/>
       <c r="E225" s="3" t="s">
@@ -5666,113 +5625,113 @@
         <v>225</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D226" s="8"/>
       <c r="E226" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="5">
         <v>226</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D227" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E227" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="5">
         <v>227</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D228" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E228" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="5">
         <v>228</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D229" s="7" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="E229" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="5">
         <v>229</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D230" s="7" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="E230" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="5">
         <v>230</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D231" s="7" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="E231" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="5">
         <v>231</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D232" s="7" t="s">
-        <v>556</v>
+        <v>546</v>
       </c>
       <c r="E232" s="5" t="s">
         <v>4</v>
@@ -5783,10 +5742,10 @@
         <v>232</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C233" s="8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D233" s="8"/>
       <c r="E233" s="3" t="s">
@@ -5798,10 +5757,10 @@
         <v>233</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D234" s="8"/>
       <c r="E234" s="3" t="s">
@@ -5813,10 +5772,10 @@
         <v>234</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C235" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D235" s="8"/>
       <c r="E235" s="3" t="s">
@@ -5828,10 +5787,10 @@
         <v>235</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D236" s="8"/>
       <c r="E236" s="3" t="s">
@@ -5843,10 +5802,10 @@
         <v>236</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C237" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D237" s="8"/>
       <c r="E237" s="3" t="s">
@@ -5858,10 +5817,10 @@
         <v>237</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C238" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D238" s="8"/>
       <c r="E238" s="3" t="s">
@@ -5873,10 +5832,10 @@
         <v>238</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D239" s="8"/>
       <c r="E239" s="3" t="s">
@@ -5888,10 +5847,10 @@
         <v>239</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D240" s="8"/>
       <c r="E240" s="3" t="s">
@@ -5903,10 +5862,10 @@
         <v>240</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D241" s="8"/>
       <c r="E241" s="3" t="s">
@@ -5918,10 +5877,10 @@
         <v>241</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D242" s="8"/>
       <c r="E242" s="3" t="s">
@@ -5933,10 +5892,10 @@
         <v>242</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D243" s="8"/>
       <c r="E243" s="3" t="s">
@@ -5948,10 +5907,10 @@
         <v>243</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D244" s="8"/>
       <c r="E244" s="3" t="s">
@@ -5963,10 +5922,10 @@
         <v>244</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D245" s="8"/>
       <c r="E245" s="3" t="s">
@@ -5978,10 +5937,10 @@
         <v>245</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C246" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D246" s="8"/>
       <c r="E246" s="3" t="s">
@@ -5993,10 +5952,10 @@
         <v>246</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C247" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D247" s="8"/>
       <c r="E247" s="3" t="s">
@@ -6008,10 +5967,10 @@
         <v>247</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D248" s="8"/>
       <c r="E248" s="3" t="s">
@@ -6023,10 +5982,10 @@
         <v>248</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C249" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D249" s="8"/>
       <c r="E249" s="3" t="s">
@@ -6038,7 +5997,7 @@
         <v>248</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C250" s="8" t="s">
         <v>18</v>
@@ -6051,10 +6010,10 @@
         <v>249</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D251" s="8"/>
       <c r="E251" s="3" t="s">
@@ -6066,10 +6025,10 @@
         <v>250</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D252" s="9"/>
       <c r="E252" s="3" t="s">
@@ -6080,7 +6039,7 @@
   <autoFilter ref="A1:E252" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
     <filterColumn colId="4">
       <filters>
-        <filter val="BANNERS EDUCATIVOS"/>
+        <filter val="MATERIAIS ESPORTIVOS"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E252">

</xml_diff>

<commit_message>
adicionei os dois arquivos txt que são para base do código de criar a página do produto
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BCDF14-D63C-4ED6-9D20-50FFEE3D4B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA5D4D6-1514-4949-9628-BD4C88143D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
@@ -74,39 +74,12 @@
     <t>VENTILADORES</t>
   </si>
   <si>
-    <t>Tabela-Basquete-Mdf-9mm-Aro-36-Cm-Basketball-Master-Xalingo-SITE</t>
-  </si>
-  <si>
-    <t>Tabela-De-Basquete-infantil-SITE</t>
-  </si>
-  <si>
-    <t>Xalingo-tabela-cesta-de-basquete-com-bola-SITE</t>
-  </si>
-  <si>
-    <t>Jogo-De-Ping-Pong-Simples-Xalingo-SITE</t>
-  </si>
-  <si>
-    <t>Mesa-de-pebolim-Xalingo-Super-copa-cor-verde-SITE</t>
-  </si>
-  <si>
-    <t>Jogo-De-Botao-Brasileirao-Xalingo-SITE</t>
-  </si>
-  <si>
-    <t>Mesa-E-Jogo-De-Futebol-De-Botao-Com-2-Marcadores-Xalingo-SITE</t>
-  </si>
-  <si>
     <t>Brinquedo-de-Borracha-Mamae-pata-e-seus-patinhos</t>
   </si>
   <si>
     <t>NOME DO ARQUIVO .HTML</t>
   </si>
   <si>
-    <t>Conjunto-Completo-Tenis-De-Mesa-Ping-Pong-Rede-E-Raquete-STE</t>
-  </si>
-  <si>
-    <t>Mesa-Para-Ping-Pong-Tenis-De-Mesa-Azul-COM-Pes-Dobráveis-SITE</t>
-  </si>
-  <si>
     <t>NOME DA IMAGEM</t>
   </si>
   <si>
@@ -1685,31 +1658,58 @@
     <t>Caixa de caneta com 50 unidades</t>
   </si>
   <si>
-    <t xml:space="preserve">Jogo De Botão Brasileirão Xalingo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jogo De Ping Pong Simples - Xalingo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesa de pebolim Xalingo Super copa cor verde  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesa E Jogo De Futebol De Botão com 2 Marcadores Xalingo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mesa Para Ping Pong  Tênis De Mesa Azul com Pés Dobráveis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabela Basquete Mdf 9mm Aro 36 Cm Basketball Master Xalingo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabela De Basquete infantil </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xalingo tabela cesta de basquete com bola </t>
-  </si>
-  <si>
-    <t>Conjunto Completo - Tênis De Mesa - Ping Pong - Rede e Raquete</t>
+    <t>Cesta de basquete Xalingo, com bola inclusa</t>
+  </si>
+  <si>
+    <t>197-conjunto-completo-tenis-de-mesa-ping-pong-rede-e-raquete.html</t>
+  </si>
+  <si>
+    <t>198-jogo-de-botao-brasileirao-xalingo.html</t>
+  </si>
+  <si>
+    <t>199-jogo-de-ping-pong-simples-xalingo.html</t>
+  </si>
+  <si>
+    <t>200-mesa-de-pebolim-xalingo-super-copa-verde.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201-mesa-e-jogo-de-futebol-de-botao-com-dois-marcadores-xalingo.html </t>
+  </si>
+  <si>
+    <t>202-mesa-para-ping-pong-tenis-de-mesa-azul-com-pes-dobraveis.html</t>
+  </si>
+  <si>
+    <t>203-tabela-basquete-mdf-9mm-aro-36cm-basketball-master-xalingo.html</t>
+  </si>
+  <si>
+    <t>204-tabela-de-basquete-infantil.html</t>
+  </si>
+  <si>
+    <t>205-cesta-de-basquete-com-bola-xalingo.html</t>
+  </si>
+  <si>
+    <t>Conjunto completo - tênis de mesa - ping pong - rede e raquete</t>
+  </si>
+  <si>
+    <t>Jogo de botão Brasileirão Xalingo</t>
+  </si>
+  <si>
+    <t>Jogo de ping pong simples - Xalingo</t>
+  </si>
+  <si>
+    <t>Mesa e jogo de futebol de botão com 2 marcadores Xalingo</t>
+  </si>
+  <si>
+    <t>Mesa para ping pong - tênis de mesa azul com pés dobráveis</t>
+  </si>
+  <si>
+    <t>Tabela basquete MDF 9mm aro 36 cm Basketball Master Xalingo</t>
+  </si>
+  <si>
+    <t>Tabela de basquete infantil</t>
+  </si>
+  <si>
+    <t>Mesa de Pebolim Super Copa - Xalingo</t>
   </si>
 </sst>
 </file>
@@ -2171,14 +2171,14 @@
   <dimension ref="A1:F252"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D254" sqref="D254"/>
+      <selection activeCell="C206" sqref="C206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="57.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="73.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="0" style="2" hidden="1" customWidth="1"/>
@@ -2187,16 +2187,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -2207,10 +2207,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3" t="s">
@@ -2222,10 +2222,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="3" t="s">
@@ -2237,10 +2237,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="3" t="s">
@@ -2252,10 +2252,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="3" t="s">
@@ -2267,10 +2267,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
@@ -2282,10 +2282,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
@@ -2297,10 +2297,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
@@ -2312,10 +2312,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="3" t="s">
@@ -2327,10 +2327,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="3" t="s">
@@ -2342,10 +2342,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="3" t="s">
@@ -2357,13 +2357,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>4</v>
@@ -2374,13 +2374,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>4</v>
@@ -2391,13 +2391,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>4</v>
@@ -2408,13 +2408,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>4</v>
@@ -2425,13 +2425,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>4</v>
@@ -2442,13 +2442,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>4</v>
@@ -2459,13 +2459,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>4</v>
@@ -2476,13 +2476,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>4</v>
@@ -2493,13 +2493,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>4</v>
@@ -2510,13 +2510,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>4</v>
@@ -2527,13 +2527,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>4</v>
@@ -2544,13 +2544,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>4</v>
@@ -2561,13 +2561,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>4</v>
@@ -2578,13 +2578,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>4</v>
@@ -2604,13 +2604,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>4</v>
@@ -2621,13 +2621,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>4</v>
@@ -2638,13 +2638,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>4</v>
@@ -2655,13 +2655,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>4</v>
@@ -2672,13 +2672,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>4</v>
@@ -2689,13 +2689,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>4</v>
@@ -2706,13 +2706,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>4</v>
@@ -2723,13 +2723,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>4</v>
@@ -2740,13 +2740,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>4</v>
@@ -2757,13 +2757,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>4</v>
@@ -2774,13 +2774,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>4</v>
@@ -2791,13 +2791,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>4</v>
@@ -2808,13 +2808,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>4</v>
@@ -2825,13 +2825,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>4</v>
@@ -2842,13 +2842,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>4</v>
@@ -2859,13 +2859,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>4</v>
@@ -2876,13 +2876,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>4</v>
@@ -2893,13 +2893,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>4</v>
@@ -2910,13 +2910,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>4</v>
@@ -2927,13 +2927,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>4</v>
@@ -2944,13 +2944,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>4</v>
@@ -2961,13 +2961,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>4</v>
@@ -2978,13 +2978,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>4</v>
@@ -2995,13 +2995,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>4</v>
@@ -3012,13 +3012,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>4</v>
@@ -3029,13 +3029,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>4</v>
@@ -3046,13 +3046,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>4</v>
@@ -3063,13 +3063,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>4</v>
@@ -3080,13 +3080,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>4</v>
@@ -3097,13 +3097,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>4</v>
@@ -3114,13 +3114,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>4</v>
@@ -3131,13 +3131,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>4</v>
@@ -3148,13 +3148,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>4</v>
@@ -3165,13 +3165,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>4</v>
@@ -3182,13 +3182,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>4</v>
@@ -3199,13 +3199,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>2</v>
@@ -3288,10 +3288,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="3" t="s">
@@ -3303,10 +3303,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="3" t="s">
@@ -3318,10 +3318,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="3" t="s">
@@ -3333,10 +3333,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="3" t="s">
@@ -3348,10 +3348,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="3" t="s">
@@ -3363,10 +3363,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="D76" s="9"/>
       <c r="E76" s="3" t="s">
@@ -3378,10 +3378,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="3" t="s">
@@ -3393,10 +3393,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="3" t="s">
@@ -3408,10 +3408,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="3" t="s">
@@ -3423,10 +3423,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="3" t="s">
@@ -3438,10 +3438,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="3" t="s">
@@ -3453,10 +3453,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="3" t="s">
@@ -3468,10 +3468,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="3" t="s">
@@ -3483,10 +3483,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="3" t="s">
@@ -3498,10 +3498,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="3" t="s">
@@ -3513,10 +3513,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="3" t="s">
@@ -3528,10 +3528,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D87" s="8"/>
       <c r="E87" s="3" t="s">
@@ -3543,10 +3543,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="3" t="s">
@@ -3558,10 +3558,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="3" t="s">
@@ -3573,10 +3573,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="3" t="s">
@@ -3588,10 +3588,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="3" t="s">
@@ -3603,10 +3603,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D92" s="8"/>
       <c r="E92" s="3" t="s">
@@ -3618,10 +3618,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="3" t="s">
@@ -3633,10 +3633,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="3" t="s">
@@ -3648,10 +3648,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="D95" s="8"/>
       <c r="E95" s="3" t="s">
@@ -3663,10 +3663,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D96" s="8"/>
       <c r="E96" s="3" t="s">
@@ -3678,10 +3678,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="3" t="s">
@@ -3693,10 +3693,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="3" t="s">
@@ -3708,10 +3708,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="3" t="s">
@@ -3723,10 +3723,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="D100" s="8"/>
       <c r="E100" s="3" t="s">
@@ -3738,10 +3738,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D101" s="8"/>
       <c r="E101" s="3" t="s">
@@ -3753,10 +3753,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D102" s="8"/>
       <c r="E102" s="3" t="s">
@@ -3768,10 +3768,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D103" s="8"/>
       <c r="E103" s="3" t="s">
@@ -3783,10 +3783,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="D104" s="8"/>
       <c r="E104" s="3" t="s">
@@ -3798,10 +3798,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D105" s="8"/>
       <c r="E105" s="3" t="s">
@@ -3813,10 +3813,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="D106" s="8"/>
       <c r="E106" s="3" t="s">
@@ -3828,10 +3828,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="D107" s="8"/>
       <c r="E107" s="3" t="s">
@@ -3843,10 +3843,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D108" s="8"/>
       <c r="E108" s="3" t="s">
@@ -3858,10 +3858,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="D109" s="8"/>
       <c r="E109" s="3" t="s">
@@ -3873,10 +3873,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="D110" s="8"/>
       <c r="E110" s="3" t="s">
@@ -3888,10 +3888,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="D111" s="8"/>
       <c r="E111" s="3" t="s">
@@ -3903,10 +3903,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="3" t="s">
@@ -3918,10 +3918,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D113" s="8"/>
       <c r="E113" s="3" t="s">
@@ -3933,10 +3933,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="D114" s="8"/>
       <c r="E114" s="3" t="s">
@@ -3948,10 +3948,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D115" s="8"/>
       <c r="E115" s="3" t="s">
@@ -3963,10 +3963,10 @@
         <v>115</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="D116" s="8"/>
       <c r="E116" s="3" t="s">
@@ -3978,10 +3978,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="D117" s="8"/>
       <c r="E117" s="3" t="s">
@@ -3993,10 +3993,10 @@
         <v>117</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="D118" s="8"/>
       <c r="E118" s="3" t="s">
@@ -4008,10 +4008,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="3" t="s">
@@ -4023,10 +4023,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="D120" s="8"/>
       <c r="E120" s="3" t="s">
@@ -4038,10 +4038,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="D121" s="8"/>
       <c r="E121" s="3" t="s">
@@ -4053,10 +4053,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="D122" s="8"/>
       <c r="E122" s="3" t="s">
@@ -4068,10 +4068,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="D123" s="8"/>
       <c r="E123" s="3" t="s">
@@ -4083,10 +4083,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="D124" s="8"/>
       <c r="E124" s="3" t="s">
@@ -4098,10 +4098,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="D125" s="8"/>
       <c r="E125" s="3" t="s">
@@ -4113,10 +4113,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="3" t="s">
@@ -4128,10 +4128,10 @@
         <v>126</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="D127" s="8"/>
       <c r="E127" s="3" t="s">
@@ -4143,10 +4143,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="3" t="s">
@@ -4158,10 +4158,10 @@
         <v>128</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="3" t="s">
@@ -4173,10 +4173,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="D130" s="8"/>
       <c r="E130" s="3" t="s">
@@ -4188,10 +4188,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="D131" s="8"/>
       <c r="E131" s="3" t="s">
@@ -4203,10 +4203,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="D132" s="8"/>
       <c r="E132" s="3" t="s">
@@ -4218,10 +4218,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D133" s="8"/>
       <c r="E133" s="3" t="s">
@@ -4233,10 +4233,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="D134" s="8"/>
       <c r="E134" s="3" t="s">
@@ -4248,10 +4248,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="D135" s="8"/>
       <c r="E135" s="3" t="s">
@@ -4263,10 +4263,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D136" s="8"/>
       <c r="E136" s="3" t="s">
@@ -4278,10 +4278,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="D137" s="8"/>
       <c r="E137" s="3" t="s">
@@ -4293,10 +4293,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D138" s="8"/>
       <c r="E138" s="3" t="s">
@@ -4308,10 +4308,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="D139" s="8"/>
       <c r="E139" s="3" t="s">
@@ -4323,10 +4323,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="3" t="s">
@@ -4338,10 +4338,10 @@
         <v>140</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D141" s="8"/>
       <c r="E141" s="3" t="s">
@@ -4353,10 +4353,10 @@
         <v>141</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="D142" s="8"/>
       <c r="E142" s="3" t="s">
@@ -4368,10 +4368,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="D143" s="8"/>
       <c r="E143" s="3" t="s">
@@ -4383,10 +4383,10 @@
         <v>143</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="D144" s="8"/>
       <c r="E144" s="3" t="s">
@@ -4398,10 +4398,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="D145" s="8"/>
       <c r="E145" s="3" t="s">
@@ -4413,10 +4413,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D146" s="8"/>
       <c r="E146" s="3" t="s">
@@ -4428,10 +4428,10 @@
         <v>146</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="D147" s="8"/>
       <c r="E147" s="3" t="s">
@@ -4443,10 +4443,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="D148" s="8"/>
       <c r="E148" s="3" t="s">
@@ -4458,10 +4458,10 @@
         <v>148</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="D149" s="8"/>
       <c r="E149" s="3" t="s">
@@ -4473,10 +4473,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="D150" s="8"/>
       <c r="E150" s="3" t="s">
@@ -4488,10 +4488,10 @@
         <v>150</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="D151" s="8"/>
       <c r="E151" s="3" t="s">
@@ -4503,10 +4503,10 @@
         <v>151</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="D152" s="8"/>
       <c r="E152" s="3" t="s">
@@ -4518,10 +4518,10 @@
         <v>152</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="D153" s="8"/>
       <c r="E153" s="3" t="s">
@@ -4533,10 +4533,10 @@
         <v>153</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="D154" s="8"/>
       <c r="E154" s="3" t="s">
@@ -4548,10 +4548,10 @@
         <v>154</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="D155" s="8"/>
       <c r="E155" s="3" t="s">
@@ -4563,10 +4563,10 @@
         <v>155</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C156" s="8" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="D156" s="8"/>
       <c r="E156" s="3" t="s">
@@ -4578,10 +4578,10 @@
         <v>156</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="D157" s="8"/>
       <c r="E157" s="3" t="s">
@@ -4593,10 +4593,10 @@
         <v>157</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C158" s="8" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="D158" s="8"/>
       <c r="E158" s="3" t="s">
@@ -4608,10 +4608,10 @@
         <v>158</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="D159" s="8"/>
       <c r="E159" s="3" t="s">
@@ -4623,10 +4623,10 @@
         <v>159</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="D160" s="8"/>
       <c r="E160" s="3" t="s">
@@ -4638,10 +4638,10 @@
         <v>160</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="D161" s="8"/>
       <c r="E161" s="3" t="s">
@@ -4653,10 +4653,10 @@
         <v>161</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="D162" s="8"/>
       <c r="E162" s="3" t="s">
@@ -4668,10 +4668,10 @@
         <v>162</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="D163" s="8"/>
       <c r="E163" s="3" t="s">
@@ -4683,10 +4683,10 @@
         <v>163</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="D164" s="8"/>
       <c r="E164" s="3" t="s">
@@ -4698,10 +4698,10 @@
         <v>164</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="D165" s="8"/>
       <c r="E165" s="3" t="s">
@@ -4713,10 +4713,10 @@
         <v>165</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="D166" s="8"/>
       <c r="E166" s="3" t="s">
@@ -4728,10 +4728,10 @@
         <v>166</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="D167" s="8"/>
       <c r="E167" s="3" t="s">
@@ -4743,10 +4743,10 @@
         <v>167</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="D168" s="8"/>
       <c r="E168" s="3" t="s">
@@ -4758,10 +4758,10 @@
         <v>168</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="D169" s="8"/>
       <c r="E169" s="3" t="s">
@@ -4773,10 +4773,10 @@
         <v>169</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="D170" s="8"/>
       <c r="E170" s="3" t="s">
@@ -4788,10 +4788,10 @@
         <v>170</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="D171" s="8"/>
       <c r="E171" s="3" t="s">
@@ -4803,10 +4803,10 @@
         <v>171</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="D172" s="8"/>
       <c r="E172" s="3" t="s">
@@ -4818,10 +4818,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="D173" s="8"/>
       <c r="E173" s="3" t="s">
@@ -4833,10 +4833,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="D174" s="8"/>
       <c r="E174" s="3" t="s">
@@ -4848,10 +4848,10 @@
         <v>174</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="D175" s="8"/>
       <c r="E175" s="3" t="s">
@@ -4863,10 +4863,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="D176" s="8"/>
       <c r="E176" s="3" t="s">
@@ -4878,10 +4878,10 @@
         <v>176</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="D177" s="8"/>
       <c r="E177" s="3" t="s">
@@ -4893,10 +4893,10 @@
         <v>177</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="D178" s="8"/>
       <c r="E178" s="3" t="s">
@@ -4908,10 +4908,10 @@
         <v>178</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="D179" s="8"/>
       <c r="E179" s="3" t="s">
@@ -4923,10 +4923,10 @@
         <v>179</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C180" s="8" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="D180" s="8"/>
       <c r="E180" s="3" t="s">
@@ -4938,10 +4938,10 @@
         <v>180</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="D181" s="8"/>
       <c r="E181" s="3" t="s">
@@ -4953,10 +4953,10 @@
         <v>181</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="D182" s="8"/>
       <c r="E182" s="3" t="s">
@@ -4968,10 +4968,10 @@
         <v>182</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="D183" s="8"/>
       <c r="E183" s="3" t="s">
@@ -4983,10 +4983,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="D184" s="8"/>
       <c r="E184" s="3" t="s">
@@ -4998,7 +4998,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C185" s="9"/>
       <c r="D185" s="9"/>
@@ -5011,10 +5011,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="D186" s="8"/>
       <c r="E186" s="3" t="s">
@@ -5026,7 +5026,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C187" s="9"/>
       <c r="D187" s="9"/>
@@ -5039,10 +5039,10 @@
         <v>187</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="D188" s="8"/>
       <c r="E188" s="3" t="s">
@@ -5054,10 +5054,10 @@
         <v>188</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="D189" s="8"/>
       <c r="E189" s="3" t="s">
@@ -5069,10 +5069,10 @@
         <v>189</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="D190" s="8"/>
       <c r="E190" s="3" t="s">
@@ -5084,10 +5084,10 @@
         <v>190</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="D191" s="8"/>
       <c r="E191" s="3" t="s">
@@ -5099,10 +5099,10 @@
         <v>191</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
       <c r="D192" s="8"/>
       <c r="E192" s="3" t="s">
@@ -5114,10 +5114,10 @@
         <v>192</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="D193" s="8"/>
       <c r="E193" s="3" t="s">
@@ -5129,7 +5129,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C194" s="9"/>
       <c r="D194" s="9"/>
@@ -5142,10 +5142,10 @@
         <v>194</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="D195" s="8"/>
       <c r="E195" s="3" t="s">
@@ -5157,10 +5157,10 @@
         <v>195</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D196" s="8"/>
       <c r="E196" s="3" t="s">
@@ -5172,10 +5172,10 @@
         <v>196</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="D197" s="8"/>
       <c r="E197" s="3" t="s">
@@ -5187,13 +5187,13 @@
         <v>197</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>20</v>
+        <v>540</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="E198" s="3" t="s">
         <v>7</v>
@@ -5204,13 +5204,13 @@
         <v>198</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>16</v>
+        <v>541</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E199" s="3" t="s">
         <v>7</v>
@@ -5221,13 +5221,13 @@
         <v>199</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>14</v>
+        <v>542</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>7</v>
@@ -5238,13 +5238,13 @@
         <v>200</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>15</v>
+        <v>543</v>
       </c>
       <c r="D201" s="8" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>7</v>
@@ -5255,13 +5255,13 @@
         <v>201</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C202" s="8" t="s">
-        <v>17</v>
+        <v>544</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E202" s="3" t="s">
         <v>7</v>
@@ -5272,13 +5272,13 @@
         <v>202</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C203" s="8" t="s">
-        <v>21</v>
+        <v>545</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E203" s="3" t="s">
         <v>7</v>
@@ -5289,13 +5289,13 @@
         <v>203</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C204" s="8" t="s">
-        <v>11</v>
+        <v>546</v>
       </c>
       <c r="D204" s="8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E204" s="3" t="s">
         <v>7</v>
@@ -5306,13 +5306,13 @@
         <v>204</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>12</v>
+        <v>547</v>
       </c>
       <c r="D205" s="8" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>7</v>
@@ -5323,13 +5323,13 @@
         <v>205</v>
       </c>
       <c r="B206" s="8" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C206" s="8" t="s">
-        <v>13</v>
+        <v>548</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>555</v>
+        <v>539</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>7</v>
@@ -5340,10 +5340,10 @@
         <v>206</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="D207" s="8"/>
       <c r="E207" s="3" t="s">
@@ -5355,10 +5355,10 @@
         <v>207</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D208" s="8"/>
       <c r="E208" s="3" t="s">
@@ -5370,10 +5370,10 @@
         <v>208</v>
       </c>
       <c r="B209" s="8" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C209" s="8" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="D209" s="8"/>
       <c r="E209" s="3" t="s">
@@ -5385,10 +5385,10 @@
         <v>209</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D210" s="8"/>
       <c r="E210" s="3" t="s">
@@ -5400,10 +5400,10 @@
         <v>210</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="D211" s="8"/>
       <c r="E211" s="3" t="s">
@@ -5415,10 +5415,10 @@
         <v>211</v>
       </c>
       <c r="B212" s="8" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C212" s="8" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="D212" s="8"/>
       <c r="E212" s="3" t="s">
@@ -5430,10 +5430,10 @@
         <v>212</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="D213" s="8"/>
       <c r="E213" s="3" t="s">
@@ -5445,10 +5445,10 @@
         <v>213</v>
       </c>
       <c r="B214" s="8" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C214" s="8" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="D214" s="8"/>
       <c r="E214" s="3" t="s">
@@ -5460,10 +5460,10 @@
         <v>214</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C215" s="8" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="D215" s="8"/>
       <c r="E215" s="3" t="s">
@@ -5475,10 +5475,10 @@
         <v>215</v>
       </c>
       <c r="B216" s="8" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C216" s="8" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="D216" s="8"/>
       <c r="E216" s="3" t="s">
@@ -5490,10 +5490,10 @@
         <v>216</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D217" s="8"/>
       <c r="E217" s="3" t="s">
@@ -5505,10 +5505,10 @@
         <v>217</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
       <c r="D218" s="8"/>
       <c r="E218" s="3" t="s">
@@ -5520,10 +5520,10 @@
         <v>218</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C219" s="8" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D219" s="8"/>
       <c r="E219" s="3" t="s">
@@ -5535,10 +5535,10 @@
         <v>219</v>
       </c>
       <c r="B220" s="8" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C220" s="8" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="D220" s="8"/>
       <c r="E220" s="3" t="s">
@@ -5550,10 +5550,10 @@
         <v>220</v>
       </c>
       <c r="B221" s="8" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="D221" s="8"/>
       <c r="E221" s="3" t="s">
@@ -5565,10 +5565,10 @@
         <v>221</v>
       </c>
       <c r="B222" s="8" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C222" s="8" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="D222" s="8"/>
       <c r="E222" s="3" t="s">
@@ -5580,10 +5580,10 @@
         <v>222</v>
       </c>
       <c r="B223" s="8" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C223" s="8" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="D223" s="8"/>
       <c r="E223" s="3" t="s">
@@ -5595,10 +5595,10 @@
         <v>223</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C224" s="8" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="D224" s="8"/>
       <c r="E224" s="3" t="s">
@@ -5610,10 +5610,10 @@
         <v>224</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C225" s="8" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="D225" s="8"/>
       <c r="E225" s="3" t="s">
@@ -5625,10 +5625,10 @@
         <v>225</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="D226" s="8"/>
       <c r="E226" s="3" t="s">
@@ -5640,13 +5640,13 @@
         <v>226</v>
       </c>
       <c r="B227" s="7" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="D227" s="7" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="E227" s="5" t="s">
         <v>4</v>
@@ -5657,13 +5657,13 @@
         <v>227</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="D228" s="7" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="E228" s="5" t="s">
         <v>4</v>
@@ -5674,13 +5674,13 @@
         <v>228</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="D229" s="7" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="E229" s="5" t="s">
         <v>4</v>
@@ -5691,13 +5691,13 @@
         <v>229</v>
       </c>
       <c r="B230" s="7" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="D230" s="7" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
       <c r="E230" s="5" t="s">
         <v>4</v>
@@ -5708,13 +5708,13 @@
         <v>230</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="D231" s="7" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="E231" s="5" t="s">
         <v>4</v>
@@ -5725,13 +5725,13 @@
         <v>231</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="D232" s="7" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="E232" s="5" t="s">
         <v>4</v>
@@ -5742,10 +5742,10 @@
         <v>232</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C233" s="8" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D233" s="8"/>
       <c r="E233" s="3" t="s">
@@ -5757,10 +5757,10 @@
         <v>233</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="D234" s="8"/>
       <c r="E234" s="3" t="s">
@@ -5772,10 +5772,10 @@
         <v>234</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C235" s="8" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D235" s="8"/>
       <c r="E235" s="3" t="s">
@@ -5787,10 +5787,10 @@
         <v>235</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="D236" s="8"/>
       <c r="E236" s="3" t="s">
@@ -5802,10 +5802,10 @@
         <v>236</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C237" s="8" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D237" s="8"/>
       <c r="E237" s="3" t="s">
@@ -5817,10 +5817,10 @@
         <v>237</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C238" s="8" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="D238" s="8"/>
       <c r="E238" s="3" t="s">
@@ -5832,10 +5832,10 @@
         <v>238</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="D239" s="8"/>
       <c r="E239" s="3" t="s">
@@ -5847,10 +5847,10 @@
         <v>239</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C240" s="8" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="D240" s="8"/>
       <c r="E240" s="3" t="s">
@@ -5862,10 +5862,10 @@
         <v>240</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="D241" s="8"/>
       <c r="E241" s="3" t="s">
@@ -5877,10 +5877,10 @@
         <v>241</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="D242" s="8"/>
       <c r="E242" s="3" t="s">
@@ -5892,10 +5892,10 @@
         <v>242</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="D243" s="8"/>
       <c r="E243" s="3" t="s">
@@ -5907,10 +5907,10 @@
         <v>243</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="D244" s="8"/>
       <c r="E244" s="3" t="s">
@@ -5922,10 +5922,10 @@
         <v>244</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="D245" s="8"/>
       <c r="E245" s="3" t="s">
@@ -5937,10 +5937,10 @@
         <v>245</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C246" s="8" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D246" s="8"/>
       <c r="E246" s="3" t="s">
@@ -5952,10 +5952,10 @@
         <v>246</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C247" s="8" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="D247" s="8"/>
       <c r="E247" s="3" t="s">
@@ -5967,10 +5967,10 @@
         <v>247</v>
       </c>
       <c r="B248" s="8" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="D248" s="8"/>
       <c r="E248" s="3" t="s">
@@ -5982,10 +5982,10 @@
         <v>248</v>
       </c>
       <c r="B249" s="8" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C249" s="8" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="D249" s="8"/>
       <c r="E249" s="3" t="s">
@@ -5997,10 +5997,10 @@
         <v>248</v>
       </c>
       <c r="B250" s="8" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C250" s="8" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D250" s="8"/>
       <c r="E250" s="3"/>
@@ -6010,10 +6010,10 @@
         <v>249</v>
       </c>
       <c r="B251" s="8" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="D251" s="8"/>
       <c r="E251" s="3" t="s">
@@ -6025,10 +6025,10 @@
         <v>250</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="D252" s="9"/>
       <c r="E252" s="3" t="s">

</xml_diff>

<commit_message>
tinha esquecido de enviar a planilha com as atualizações
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.macedo\OneDrive - Sinergy RH\Desktop\Coding\Anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783CF4FA-0FD6-4DC4-B888-C3BB6B3E2103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBB2D06-B1AA-479D-8010-401CC45A4864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="823" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$D$1:$J$252</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$D$1:$K$252</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="564">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -1716,6 +1716,21 @@
   </si>
   <si>
     <t>NUMERAÇÃO ALEATÓRIA</t>
+  </si>
+  <si>
+    <t>banners-educativos</t>
+  </si>
+  <si>
+    <t>NOME DA PASTA</t>
+  </si>
+  <si>
+    <t>pedagogico</t>
+  </si>
+  <si>
+    <t>ventiladores</t>
+  </si>
+  <si>
+    <t>triciclos</t>
   </si>
 </sst>
 </file>
@@ -2192,10 +2207,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:K252"/>
+  <dimension ref="A1:L252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,13 +2221,13 @@
     <col min="6" max="6" width="53.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="36.42578125" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="0" style="2" hidden="1"/>
-    <col min="12" max="16384" width="10.85546875" style="2" hidden="1"/>
+    <col min="9" max="10" width="25.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="0" style="2" hidden="1"/>
+    <col min="13" max="16384" width="10.85546875" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>171</v>
       </c>
@@ -2232,10 +2247,13 @@
         <v>558</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D2" s="3">
         <v>99</v>
       </c>
@@ -2253,10 +2271,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D3" s="3">
         <v>55</v>
       </c>
@@ -2276,10 +2297,13 @@
         <v>2</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D4" s="3">
         <v>3</v>
       </c>
@@ -2297,10 +2321,13 @@
         <v>3</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D5" s="3">
         <v>130</v>
       </c>
@@ -2318,10 +2345,13 @@
         <v>4</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="3">
         <v>102</v>
       </c>
@@ -2339,10 +2369,13 @@
         <v>5</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="3">
         <v>72</v>
       </c>
@@ -2360,10 +2393,13 @@
         <v>6</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="3">
         <v>42</v>
       </c>
@@ -2383,10 +2419,13 @@
         <v>7</v>
       </c>
       <c r="J8" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="3">
         <v>91</v>
       </c>
@@ -2404,10 +2443,13 @@
         <v>8</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D10" s="3">
         <v>25</v>
       </c>
@@ -2420,9 +2462,12 @@
       <c r="I10" s="15">
         <v>27</v>
       </c>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D11" s="3">
         <v>34</v>
       </c>
@@ -2442,10 +2487,13 @@
         <v>9</v>
       </c>
       <c r="J11" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="3">
         <v>87</v>
       </c>
@@ -2463,10 +2511,13 @@
         <v>10</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="3">
         <v>110</v>
       </c>
@@ -2484,10 +2535,13 @@
         <v>11</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" s="3">
         <v>6</v>
       </c>
@@ -2505,10 +2559,13 @@
         <v>12</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="3">
         <v>134</v>
       </c>
@@ -2526,10 +2583,13 @@
         <v>13</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="3">
         <v>51</v>
       </c>
@@ -2549,10 +2609,13 @@
         <v>14</v>
       </c>
       <c r="J16" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="3">
         <v>114</v>
       </c>
@@ -2570,10 +2633,13 @@
         <v>15</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="3">
         <v>122</v>
       </c>
@@ -2591,10 +2657,13 @@
         <v>16</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="3">
         <v>142</v>
       </c>
@@ -2612,10 +2681,13 @@
         <v>17</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="3">
         <v>58</v>
       </c>
@@ -2635,10 +2707,13 @@
         <v>18</v>
       </c>
       <c r="J20" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3">
         <v>75</v>
       </c>
@@ -2656,10 +2731,13 @@
         <v>19</v>
       </c>
       <c r="J21" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="3">
         <v>106</v>
       </c>
@@ -2677,10 +2755,13 @@
         <v>20</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="3">
         <v>83</v>
       </c>
@@ -2698,10 +2779,13 @@
         <v>21</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="3">
         <v>138</v>
       </c>
@@ -2719,10 +2803,13 @@
         <v>22</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="3">
         <v>37</v>
       </c>
@@ -2742,10 +2829,13 @@
         <v>23</v>
       </c>
       <c r="J25" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" s="3">
         <v>157</v>
       </c>
@@ -2763,10 +2853,13 @@
         <v>24</v>
       </c>
       <c r="J26" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="3">
         <v>118</v>
       </c>
@@ -2784,10 +2877,13 @@
         <v>26</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28" s="3">
         <v>147</v>
       </c>
@@ -2805,10 +2901,13 @@
         <v>28</v>
       </c>
       <c r="J28" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K28" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29" s="3">
         <v>95</v>
       </c>
@@ -2826,10 +2925,13 @@
         <v>29</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D30" s="3">
         <v>126</v>
       </c>
@@ -2847,10 +2949,13 @@
         <v>30</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31" s="3">
         <v>45</v>
       </c>
@@ -2870,10 +2975,13 @@
         <v>31</v>
       </c>
       <c r="J31" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K31" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="3">
         <v>153</v>
       </c>
@@ -2891,10 +2999,13 @@
         <v>33</v>
       </c>
       <c r="J32" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K32" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="3">
         <v>8</v>
       </c>
@@ -2912,10 +3023,13 @@
         <v>34</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="3">
         <v>116</v>
       </c>
@@ -2933,10 +3047,13 @@
         <v>35</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="3">
         <v>79</v>
       </c>
@@ -2954,10 +3071,13 @@
         <v>36</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="3">
         <v>104</v>
       </c>
@@ -2975,10 +3095,13 @@
         <v>37</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="3">
         <v>145</v>
       </c>
@@ -2996,10 +3119,13 @@
         <v>38</v>
       </c>
       <c r="J37" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K37" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="3">
         <v>161</v>
       </c>
@@ -3017,10 +3143,13 @@
         <v>39</v>
       </c>
       <c r="J38" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K38" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="3">
         <v>93</v>
       </c>
@@ -3038,10 +3167,13 @@
         <v>40</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="3">
         <v>47</v>
       </c>
@@ -3061,10 +3193,13 @@
         <v>41</v>
       </c>
       <c r="J40" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K40" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="3">
         <v>165</v>
       </c>
@@ -3082,10 +3217,13 @@
         <v>42</v>
       </c>
       <c r="J41" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K41" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="3">
         <v>132</v>
       </c>
@@ -3103,10 +3241,13 @@
         <v>43</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="3">
         <v>85</v>
       </c>
@@ -3124,10 +3265,13 @@
         <v>44</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="3">
         <v>32</v>
       </c>
@@ -3147,10 +3291,13 @@
         <v>45</v>
       </c>
       <c r="J44" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K44" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="3">
         <v>171</v>
       </c>
@@ -3168,10 +3315,13 @@
         <v>47</v>
       </c>
       <c r="J45" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D46" s="3">
         <v>62</v>
       </c>
@@ -3184,9 +3334,10 @@
       <c r="I46" s="15">
         <v>84</v>
       </c>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="15"/>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D47" s="3">
         <v>63</v>
       </c>
@@ -3199,9 +3350,10 @@
       <c r="I47" s="15">
         <v>169</v>
       </c>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J47" s="15"/>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D48" s="3">
         <v>64</v>
       </c>
@@ -3214,9 +3366,10 @@
       <c r="I48" s="15">
         <v>25</v>
       </c>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J48" s="15"/>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D49" s="3">
         <v>65</v>
       </c>
@@ -3229,9 +3382,10 @@
       <c r="I49" s="15">
         <v>110</v>
       </c>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J49" s="15"/>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D50" s="3">
         <v>66</v>
       </c>
@@ -3244,9 +3398,10 @@
       <c r="I50" s="15">
         <v>46</v>
       </c>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J50" s="15"/>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D51" s="3">
         <v>67</v>
       </c>
@@ -3259,9 +3414,10 @@
       <c r="I51" s="15">
         <v>179</v>
       </c>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J51" s="15"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D52" s="3">
         <v>68</v>
       </c>
@@ -3274,9 +3430,10 @@
       <c r="I52" s="15">
         <v>32</v>
       </c>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J52" s="15"/>
+      <c r="K52" s="3"/>
+    </row>
+    <row r="53" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D53" s="3">
         <v>69</v>
       </c>
@@ -3289,9 +3446,10 @@
       <c r="I53" s="15">
         <v>139</v>
       </c>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J53" s="15"/>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54" s="3">
         <v>112</v>
       </c>
@@ -3309,10 +3467,13 @@
         <v>48</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D55" s="3">
         <v>53</v>
       </c>
@@ -3332,10 +3493,13 @@
         <v>49</v>
       </c>
       <c r="J55" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K55" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D56" s="3">
         <v>159</v>
       </c>
@@ -3353,10 +3517,13 @@
         <v>50</v>
       </c>
       <c r="J56" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K56" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D57" s="3">
         <v>175</v>
       </c>
@@ -3374,10 +3541,13 @@
         <v>51</v>
       </c>
       <c r="J57" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K57" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D58" s="3">
         <v>89</v>
       </c>
@@ -3395,10 +3565,13 @@
         <v>52</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D59" s="3">
         <v>73</v>
       </c>
@@ -3416,10 +3589,13 @@
         <v>53</v>
       </c>
       <c r="J59" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K59" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D60" s="3">
         <v>120</v>
       </c>
@@ -3437,10 +3613,13 @@
         <v>54</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D61" s="3">
         <v>40</v>
       </c>
@@ -3460,10 +3639,13 @@
         <v>55</v>
       </c>
       <c r="J61" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K61" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D62" s="3">
         <v>136</v>
       </c>
@@ -3481,10 +3663,13 @@
         <v>56</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D63" s="3">
         <v>2</v>
       </c>
@@ -3502,10 +3687,13 @@
         <v>57</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D64" s="3">
         <v>151</v>
       </c>
@@ -3523,10 +3711,13 @@
         <v>59</v>
       </c>
       <c r="J64" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K64" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D65" s="3">
         <v>124</v>
       </c>
@@ -3544,10 +3735,13 @@
         <v>60</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D66" s="3">
         <v>173</v>
       </c>
@@ -3565,10 +3759,13 @@
         <v>61</v>
       </c>
       <c r="J66" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K66" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D67" s="3">
         <v>188</v>
       </c>
@@ -3588,8 +3785,11 @@
       <c r="J67" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D68" s="3">
         <v>29</v>
       </c>
@@ -3609,10 +3809,13 @@
         <v>63</v>
       </c>
       <c r="J68" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K68" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D69" s="3">
         <v>81</v>
       </c>
@@ -3630,10 +3833,13 @@
         <v>64</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D70" s="3">
         <v>108</v>
       </c>
@@ -3651,10 +3857,13 @@
         <v>65</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D71" s="3">
         <v>49</v>
       </c>
@@ -3674,10 +3883,13 @@
         <v>66</v>
       </c>
       <c r="J71" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K71" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D72" s="3">
         <v>180</v>
       </c>
@@ -3695,10 +3907,13 @@
         <v>67</v>
       </c>
       <c r="J72" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K72" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D73" s="3">
         <v>140</v>
       </c>
@@ -3716,10 +3931,13 @@
         <v>68</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D74" s="3">
         <v>190</v>
       </c>
@@ -3739,8 +3957,11 @@
       <c r="J74" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K74" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D75" s="3">
         <v>77</v>
       </c>
@@ -3758,10 +3979,13 @@
         <v>71</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K75" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D76" s="3">
         <v>60</v>
       </c>
@@ -3781,10 +4005,13 @@
         <v>73</v>
       </c>
       <c r="J76" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K76" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D77" s="3">
         <v>36</v>
       </c>
@@ -3804,10 +4031,13 @@
         <v>74</v>
       </c>
       <c r="J77" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K77" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D78" s="3">
         <v>128</v>
       </c>
@@ -3825,10 +4055,13 @@
         <v>75</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D79" s="3">
         <v>155</v>
       </c>
@@ -3846,10 +4079,13 @@
         <v>76</v>
       </c>
       <c r="J79" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K79" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D80" s="3">
         <v>97</v>
       </c>
@@ -3867,10 +4103,13 @@
         <v>77</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K80" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D81" s="3">
         <v>163</v>
       </c>
@@ -3888,10 +4127,13 @@
         <v>78</v>
       </c>
       <c r="J81" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K81" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D82" s="3">
         <v>43</v>
       </c>
@@ -3911,10 +4153,13 @@
         <v>80</v>
       </c>
       <c r="J82" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K82" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D83" s="3">
         <v>167</v>
       </c>
@@ -3932,10 +4177,13 @@
         <v>81</v>
       </c>
       <c r="J83" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K83" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D84" s="3">
         <v>178</v>
       </c>
@@ -3953,10 +4201,13 @@
         <v>83</v>
       </c>
       <c r="J84" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K84" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D85" s="3">
         <v>219</v>
       </c>
@@ -3976,8 +4227,11 @@
       <c r="J85" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D86" s="3">
         <v>100</v>
       </c>
@@ -3995,10 +4249,13 @@
         <v>86</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D87" s="3">
         <v>199</v>
       </c>
@@ -4020,8 +4277,11 @@
       <c r="J87" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="88" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D88" s="3">
         <v>5</v>
       </c>
@@ -4039,10 +4299,13 @@
         <v>88</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D89" s="3">
         <v>215</v>
       </c>
@@ -4062,8 +4325,11 @@
       <c r="J89" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="90" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K89" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D90" s="3">
         <v>195</v>
       </c>
@@ -4083,8 +4349,11 @@
       <c r="J90" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K90" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D91" s="3">
         <v>9</v>
       </c>
@@ -4102,10 +4371,13 @@
         <v>91</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D92" s="3">
         <v>70</v>
       </c>
@@ -4123,10 +4395,13 @@
         <v>92</v>
       </c>
       <c r="J92" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K92" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D93" s="3">
         <v>205</v>
       </c>
@@ -4148,8 +4423,11 @@
       <c r="J93" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="94" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K93" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D94" s="3">
         <v>208</v>
       </c>
@@ -4169,8 +4447,11 @@
       <c r="J94" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="95" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K94" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D95" s="3">
         <v>56</v>
       </c>
@@ -4190,10 +4471,13 @@
         <v>95</v>
       </c>
       <c r="J95" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K95" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D96" s="3">
         <v>202</v>
       </c>
@@ -4215,8 +4499,11 @@
       <c r="J96" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="97" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K96" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D97" s="3">
         <v>221</v>
       </c>
@@ -4236,8 +4523,11 @@
       <c r="J97" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="98" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K97" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D98" s="3">
         <v>92</v>
       </c>
@@ -4255,10 +4545,13 @@
         <v>98</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D99" s="3">
         <v>176</v>
       </c>
@@ -4276,10 +4569,13 @@
         <v>99</v>
       </c>
       <c r="J99" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K99" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D100" s="3">
         <v>123</v>
       </c>
@@ -4297,10 +4593,13 @@
         <v>100</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K100" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D101" s="3">
         <v>28</v>
       </c>
@@ -4320,10 +4619,13 @@
         <v>101</v>
       </c>
       <c r="J101" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K101" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D102" s="3">
         <v>144</v>
       </c>
@@ -4341,10 +4643,13 @@
         <v>102</v>
       </c>
       <c r="J102" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K102" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D103" s="3">
         <v>217</v>
       </c>
@@ -4364,8 +4669,11 @@
       <c r="J103" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="104" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K103" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D104" s="3">
         <v>213</v>
       </c>
@@ -4385,8 +4693,11 @@
       <c r="J104" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K104" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="105" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D105" s="3">
         <v>80</v>
       </c>
@@ -4404,10 +4715,13 @@
         <v>105</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K105" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D106" s="3">
         <v>38</v>
       </c>
@@ -4427,10 +4741,13 @@
         <v>106</v>
       </c>
       <c r="J106" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K106" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D107" s="3">
         <v>223</v>
       </c>
@@ -4450,8 +4767,11 @@
       <c r="J107" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="108" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K107" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D108" s="3">
         <v>115</v>
       </c>
@@ -4469,10 +4789,13 @@
         <v>107</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K108" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D109" s="3">
         <v>185</v>
       </c>
@@ -4492,8 +4815,11 @@
       <c r="J109" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K109" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D110" s="3">
         <v>192</v>
       </c>
@@ -4513,8 +4839,11 @@
       <c r="J110" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="111" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K110" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D111" s="3">
         <v>156</v>
       </c>
@@ -4532,10 +4861,13 @@
         <v>111</v>
       </c>
       <c r="J111" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K111" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D112" s="3">
         <v>234</v>
       </c>
@@ -4555,8 +4887,11 @@
       <c r="J112" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="113" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K112" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D113" s="3">
         <v>148</v>
       </c>
@@ -4574,10 +4909,13 @@
         <v>112</v>
       </c>
       <c r="J113" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K113" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D114" s="3">
         <v>107</v>
       </c>
@@ -4595,10 +4933,13 @@
         <v>113</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D115" s="3">
         <v>172</v>
       </c>
@@ -4616,10 +4957,13 @@
         <v>114</v>
       </c>
       <c r="J115" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K115" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D116" s="3">
         <v>98</v>
       </c>
@@ -4637,10 +4981,13 @@
         <v>115</v>
       </c>
       <c r="J116" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D117" s="3">
         <v>201</v>
       </c>
@@ -4662,8 +5009,11 @@
       <c r="J117" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="118" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K117" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D118" s="3">
         <v>44</v>
       </c>
@@ -4683,10 +5033,13 @@
         <v>117</v>
       </c>
       <c r="J118" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K118" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D119" s="3">
         <v>129</v>
       </c>
@@ -4704,10 +5057,13 @@
         <v>118</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K119" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D120" s="3">
         <v>194</v>
       </c>
@@ -4727,8 +5083,11 @@
       <c r="J120" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="121" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K120" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D121" s="3">
         <v>30</v>
       </c>
@@ -4748,10 +5107,13 @@
         <v>119</v>
       </c>
       <c r="J121" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K121" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D122" s="3">
         <v>241</v>
       </c>
@@ -4771,8 +5133,11 @@
       <c r="J122" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K122" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D123" s="3">
         <v>74</v>
       </c>
@@ -4790,10 +5155,13 @@
         <v>120</v>
       </c>
       <c r="J123" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K123" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D124" s="3">
         <v>162</v>
       </c>
@@ -4811,10 +5179,13 @@
         <v>121</v>
       </c>
       <c r="J124" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K124" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D125" s="3">
         <v>236</v>
       </c>
@@ -4834,8 +5205,11 @@
       <c r="J125" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="126" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K125" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D126" s="3">
         <v>207</v>
       </c>
@@ -4855,8 +5229,11 @@
       <c r="J126" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="127" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K126" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D127" s="3">
         <v>135</v>
       </c>
@@ -4874,10 +5251,13 @@
         <v>123</v>
       </c>
       <c r="J127" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K127" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D128" s="3">
         <v>59</v>
       </c>
@@ -4897,10 +5277,13 @@
         <v>124</v>
       </c>
       <c r="J128" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K128" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D129" s="3">
         <v>214</v>
       </c>
@@ -4920,8 +5303,11 @@
       <c r="J129" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="130" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K129" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D130" s="3">
         <v>50</v>
       </c>
@@ -4941,10 +5327,13 @@
         <v>125</v>
       </c>
       <c r="J130" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K130" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D131" s="3">
         <v>243</v>
       </c>
@@ -4964,8 +5353,11 @@
       <c r="J131" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="132" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K131" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D132" s="3">
         <v>158</v>
       </c>
@@ -4983,10 +5375,13 @@
         <v>126</v>
       </c>
       <c r="J132" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K132" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D133" s="3">
         <v>216</v>
       </c>
@@ -5006,8 +5401,11 @@
       <c r="J133" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="134" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K133" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D134" s="3">
         <v>119</v>
       </c>
@@ -5025,10 +5423,13 @@
         <v>128</v>
       </c>
       <c r="J134" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D135" s="3">
         <v>245</v>
       </c>
@@ -5046,10 +5447,13 @@
         <v>128</v>
       </c>
       <c r="J135" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K135" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D136" s="3">
         <v>88</v>
       </c>
@@ -5067,10 +5471,13 @@
         <v>129</v>
       </c>
       <c r="J136" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D137" s="3">
         <v>139</v>
       </c>
@@ -5088,10 +5495,13 @@
         <v>130</v>
       </c>
       <c r="J137" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K137" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D138" s="3">
         <v>103</v>
       </c>
@@ -5109,10 +5519,13 @@
         <v>131</v>
       </c>
       <c r="J138" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K138" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D139" s="3">
         <v>35</v>
       </c>
@@ -5132,10 +5545,13 @@
         <v>132</v>
       </c>
       <c r="J139" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K139" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D140" s="3">
         <v>166</v>
       </c>
@@ -5153,10 +5569,13 @@
         <v>133</v>
       </c>
       <c r="J140" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K140" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D141" s="3">
         <v>84</v>
       </c>
@@ -5174,10 +5593,13 @@
         <v>134</v>
       </c>
       <c r="J141" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K141" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D142" s="3">
         <v>238</v>
       </c>
@@ -5197,8 +5619,11 @@
       <c r="J142" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="143" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K142" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D143" s="3">
         <v>125</v>
       </c>
@@ -5216,10 +5641,13 @@
         <v>135</v>
       </c>
       <c r="J143" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K143" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D144" s="3">
         <v>154</v>
       </c>
@@ -5237,10 +5665,13 @@
         <v>136</v>
       </c>
       <c r="J144" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K144" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D145" s="3">
         <v>54</v>
       </c>
@@ -5260,10 +5691,13 @@
         <v>137</v>
       </c>
       <c r="J145" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K145" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D146" s="3">
         <v>39</v>
       </c>
@@ -5283,10 +5717,13 @@
         <v>138</v>
       </c>
       <c r="J146" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K146" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D147" s="3">
         <v>111</v>
       </c>
@@ -5304,10 +5741,13 @@
         <v>140</v>
       </c>
       <c r="J147" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K147" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D148" s="3">
         <v>204</v>
       </c>
@@ -5329,8 +5769,11 @@
       <c r="J148" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="149" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K148" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D149" s="3">
         <v>4</v>
       </c>
@@ -5348,10 +5791,13 @@
         <v>142</v>
       </c>
       <c r="J149" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K149" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D150" s="3">
         <v>94</v>
       </c>
@@ -5369,10 +5815,13 @@
         <v>143</v>
       </c>
       <c r="J150" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K150" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D151" s="3">
         <v>181</v>
       </c>
@@ -5390,10 +5839,13 @@
         <v>144</v>
       </c>
       <c r="J151" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="K151" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D152" s="3">
         <v>187</v>
       </c>
@@ -5413,8 +5865,11 @@
       <c r="J152" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="153" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K152" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D153" s="3">
         <v>76</v>
       </c>
@@ -5432,10 +5887,13 @@
         <v>146</v>
       </c>
       <c r="J153" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K153" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D154" s="3">
         <v>146</v>
       </c>
@@ -5453,10 +5911,13 @@
         <v>147</v>
       </c>
       <c r="J154" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="K154" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D155" s="3">
         <v>220</v>
       </c>
@@ -5476,8 +5937,11 @@
       <c r="J155" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="156" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K155" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="156" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D156" s="3">
         <v>82</v>
       </c>
@@ -5495,10 +5959,13 @@
         <v>148</v>
       </c>
       <c r="J156" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="4:10" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K156" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D157" s="3">
         <v>198</v>
       </c>
@@ -5520,8 +5987,11 @@
       <c r="J157" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="158" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K157" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D158" s="3">
         <v>31</v>
       </c>
@@ -5541,10 +6011,13 @@
         <v>150</v>
       </c>
       <c r="J158" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="K158" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D159" s="3">
         <v>131</v>
       </c>
@@ -5562,10 +6035,13 @@
         <v>151</v>
       </c>
       <c r="J159" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+      <c r="K159" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D160" s="3">
         <v>184</v>
       </c>
@@ -5576,9 +6052,10 @@
       <c r="I160" s="15">
         <v>72</v>
       </c>
-      <c r="J160" s="3"/>
-    </row>
-    <row r="161" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J160" s="15"/>
+      <c r="K160" s="3"/>
+    </row>
+    <row r="161" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D161" s="3">
         <v>189</v>
       </c>
@@ -5595,11 +6072,14 @@
       <c r="I161" s="15">
         <v>152</v>
       </c>
-      <c r="J161" s="3" t="s">
+      <c r="J161" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="162" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K161" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D162" s="3">
         <v>186</v>
       </c>
@@ -5610,9 +6090,10 @@
       <c r="I162" s="15">
         <v>82</v>
       </c>
-      <c r="J162" s="3"/>
-    </row>
-    <row r="163" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J162" s="15"/>
+      <c r="K162" s="3"/>
+    </row>
+    <row r="163" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D163" s="3">
         <v>105</v>
       </c>
@@ -5629,11 +6110,14 @@
       <c r="I163" s="15">
         <v>153</v>
       </c>
-      <c r="J163" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J163" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K163" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D164" s="3">
         <v>121</v>
       </c>
@@ -5650,11 +6134,14 @@
       <c r="I164" s="15">
         <v>154</v>
       </c>
-      <c r="J164" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J164" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K164" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D165" s="3">
         <v>164</v>
       </c>
@@ -5671,11 +6158,14 @@
       <c r="I165" s="15">
         <v>155</v>
       </c>
-      <c r="J165" s="3" t="s">
+      <c r="J165" s="15" t="s">
+        <v>562</v>
+      </c>
+      <c r="K165" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D166" s="3">
         <v>179</v>
       </c>
@@ -5692,11 +6182,14 @@
       <c r="I166" s="15">
         <v>156</v>
       </c>
-      <c r="J166" s="3" t="s">
+      <c r="J166" s="15" t="s">
+        <v>563</v>
+      </c>
+      <c r="K166" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D167" s="3">
         <v>57</v>
       </c>
@@ -5715,11 +6208,14 @@
       <c r="I167" s="15">
         <v>157</v>
       </c>
-      <c r="J167" s="3" t="s">
+      <c r="J167" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K167" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D168" s="3">
         <v>193</v>
       </c>
@@ -5730,9 +6226,10 @@
       <c r="I168" s="15">
         <v>79</v>
       </c>
-      <c r="J168" s="3"/>
-    </row>
-    <row r="169" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J168" s="15"/>
+      <c r="K168" s="3"/>
+    </row>
+    <row r="169" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D169" s="3">
         <v>61</v>
       </c>
@@ -5751,11 +6248,14 @@
       <c r="I169" s="15">
         <v>158</v>
       </c>
-      <c r="J169" s="3" t="s">
+      <c r="J169" s="15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="170" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K169" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D170" s="3">
         <v>141</v>
       </c>
@@ -5772,11 +6272,14 @@
       <c r="I170" s="15">
         <v>159</v>
       </c>
-      <c r="J170" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J170" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K170" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D171" s="3">
         <v>113</v>
       </c>
@@ -5793,11 +6296,14 @@
       <c r="I171" s="15">
         <v>160</v>
       </c>
-      <c r="J171" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="172" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J171" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K171" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D172" s="3">
         <v>90</v>
       </c>
@@ -5814,11 +6320,14 @@
       <c r="I172" s="15">
         <v>161</v>
       </c>
-      <c r="J172" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="173" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J172" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K172" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D173" s="3">
         <v>174</v>
       </c>
@@ -5835,11 +6344,14 @@
       <c r="I173" s="15">
         <v>162</v>
       </c>
-      <c r="J173" s="3" t="s">
+      <c r="J173" s="15" t="s">
+        <v>563</v>
+      </c>
+      <c r="K173" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D174" s="3">
         <v>71</v>
       </c>
@@ -5856,11 +6368,14 @@
       <c r="I174" s="15">
         <v>163</v>
       </c>
-      <c r="J174" s="3" t="s">
+      <c r="J174" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K174" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D175" s="3">
         <v>137</v>
       </c>
@@ -5877,11 +6392,14 @@
       <c r="I175" s="15">
         <v>164</v>
       </c>
-      <c r="J175" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="176" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J175" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K175" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D176" s="3">
         <v>27</v>
       </c>
@@ -5900,11 +6418,14 @@
       <c r="I176" s="15">
         <v>165</v>
       </c>
-      <c r="J176" s="3" t="s">
+      <c r="J176" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K176" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D177" s="3">
         <v>127</v>
       </c>
@@ -5921,11 +6442,14 @@
       <c r="I177" s="15">
         <v>166</v>
       </c>
-      <c r="J177" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="178" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J177" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K177" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D178" s="3">
         <v>96</v>
       </c>
@@ -5942,11 +6466,14 @@
       <c r="I178" s="15">
         <v>167</v>
       </c>
-      <c r="J178" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J178" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K178" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D179" s="3">
         <v>209</v>
       </c>
@@ -5963,11 +6490,14 @@
       <c r="I179" s="15">
         <v>167</v>
       </c>
-      <c r="J179" s="3" t="s">
+      <c r="J179" s="15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="180" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K179" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D180" s="3">
         <v>41</v>
       </c>
@@ -5986,11 +6516,14 @@
       <c r="I180" s="15">
         <v>168</v>
       </c>
-      <c r="J180" s="3" t="s">
+      <c r="J180" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K180" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D181" s="3">
         <v>225</v>
       </c>
@@ -6007,11 +6540,14 @@
       <c r="I181" s="15">
         <v>168</v>
       </c>
-      <c r="J181" s="3" t="s">
+      <c r="J181" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="182" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K181" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D182" s="3">
         <v>160</v>
       </c>
@@ -6028,11 +6564,14 @@
       <c r="I182" s="15">
         <v>170</v>
       </c>
-      <c r="J182" s="3" t="s">
+      <c r="J182" s="15" t="s">
+        <v>562</v>
+      </c>
+      <c r="K182" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D183" s="3">
         <v>48</v>
       </c>
@@ -6051,11 +6590,14 @@
       <c r="I183" s="15">
         <v>171</v>
       </c>
-      <c r="J183" s="3" t="s">
+      <c r="J183" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K183" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D184" s="3">
         <v>117</v>
       </c>
@@ -6072,11 +6614,14 @@
       <c r="I184" s="15">
         <v>172</v>
       </c>
-      <c r="J184" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="185" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J184" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K184" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D185" s="3">
         <v>237</v>
       </c>
@@ -6093,11 +6638,14 @@
       <c r="I185" s="15">
         <v>172</v>
       </c>
-      <c r="J185" s="3" t="s">
+      <c r="J185" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="186" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K185" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="186" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D186" s="3">
         <v>170</v>
       </c>
@@ -6114,11 +6662,14 @@
       <c r="I186" s="15">
         <v>173</v>
       </c>
-      <c r="J186" s="3" t="s">
+      <c r="J186" s="15" t="s">
+        <v>563</v>
+      </c>
+      <c r="K186" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D187" s="3">
         <v>240</v>
       </c>
@@ -6135,11 +6686,14 @@
       <c r="I187" s="15">
         <v>173</v>
       </c>
-      <c r="J187" s="3" t="s">
+      <c r="J187" s="15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="188" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K187" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D188" s="3">
         <v>86</v>
       </c>
@@ -6156,11 +6710,14 @@
       <c r="I188" s="15">
         <v>174</v>
       </c>
-      <c r="J188" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J188" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K188" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D189" s="3">
         <v>133</v>
       </c>
@@ -6177,11 +6734,14 @@
       <c r="I189" s="15">
         <v>175</v>
       </c>
-      <c r="J189" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J189" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K189" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D190" s="3">
         <v>7</v>
       </c>
@@ -6198,11 +6758,14 @@
       <c r="I190" s="15">
         <v>176</v>
       </c>
-      <c r="J190" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J190" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K190" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D191" s="3">
         <v>78</v>
       </c>
@@ -6219,11 +6782,14 @@
       <c r="I191" s="15">
         <v>177</v>
       </c>
-      <c r="J191" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J191" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K191" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D192" s="3">
         <v>101</v>
       </c>
@@ -6240,11 +6806,14 @@
       <c r="I192" s="15">
         <v>178</v>
       </c>
-      <c r="J192" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="193" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="J192" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K192" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D193" s="3">
         <v>235</v>
       </c>
@@ -6261,11 +6830,14 @@
       <c r="I193" s="15">
         <v>179</v>
       </c>
-      <c r="J193" s="3" t="s">
+      <c r="J193" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="194" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K193" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="194" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D194" s="3">
         <v>222</v>
       </c>
@@ -6282,11 +6854,14 @@
       <c r="I194" s="15">
         <v>180</v>
       </c>
-      <c r="J194" s="3" t="s">
+      <c r="J194" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="195" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K194" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D195" s="3">
         <v>33</v>
       </c>
@@ -6305,11 +6880,14 @@
       <c r="I195" s="15">
         <v>181</v>
       </c>
-      <c r="J195" s="3" t="s">
+      <c r="J195" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K195" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D196" s="3">
         <v>109</v>
       </c>
@@ -6326,11 +6904,14 @@
       <c r="I196" s="15">
         <v>182</v>
       </c>
-      <c r="J196" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J196" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K196" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D197" s="3">
         <v>244</v>
       </c>
@@ -6347,11 +6928,14 @@
       <c r="I197" s="15">
         <v>182</v>
       </c>
-      <c r="J197" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J197" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="K197" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D198" s="3">
         <v>52</v>
       </c>
@@ -6370,11 +6954,14 @@
       <c r="I198" s="15">
         <v>183</v>
       </c>
-      <c r="J198" s="3" t="s">
+      <c r="J198" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K198" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D199" s="3">
         <v>242</v>
       </c>
@@ -6391,11 +6978,14 @@
       <c r="I199" s="15">
         <v>183</v>
       </c>
-      <c r="J199" s="3" t="s">
+      <c r="J199" s="15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="200" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="K199" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D200" s="3">
         <v>152</v>
       </c>
@@ -6412,11 +7002,14 @@
       <c r="I200" s="15">
         <v>184</v>
       </c>
-      <c r="J200" s="3" t="s">
+      <c r="J200" s="15" t="s">
+        <v>562</v>
+      </c>
+      <c r="K200" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="4:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D201" s="3">
         <v>46</v>
       </c>
@@ -6435,11 +7028,14 @@
       <c r="I201" s="15">
         <v>185</v>
       </c>
-      <c r="J201" s="3" t="s">
+      <c r="J201" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K201" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D202" s="3">
         <v>218</v>
       </c>
@@ -6456,11 +7052,14 @@
       <c r="I202" s="15">
         <v>186</v>
       </c>
-      <c r="J202" s="3" t="s">
+      <c r="J202" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="203" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="K202" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D203" s="5">
         <v>1</v>
       </c>
@@ -6475,11 +7074,12 @@
         <v>555</v>
       </c>
       <c r="I203" s="14"/>
-      <c r="J203" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J203" s="14"/>
+      <c r="K203" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D204" s="5">
         <v>10</v>
       </c>
@@ -6496,11 +7096,12 @@
         <v>555</v>
       </c>
       <c r="I204" s="14"/>
-      <c r="J204" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="205" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J204" s="14"/>
+      <c r="K204" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D205" s="5">
         <v>11</v>
       </c>
@@ -6517,11 +7118,12 @@
         <v>555</v>
       </c>
       <c r="I205" s="14"/>
-      <c r="J205" s="5" t="s">
+      <c r="J205" s="14"/>
+      <c r="K205" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D206" s="5">
         <v>12</v>
       </c>
@@ -6538,11 +7140,12 @@
         <v>555</v>
       </c>
       <c r="I206" s="14"/>
-      <c r="J206" s="5" t="s">
+      <c r="J206" s="14"/>
+      <c r="K206" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D207" s="5">
         <v>13</v>
       </c>
@@ -6559,11 +7162,12 @@
         <v>555</v>
       </c>
       <c r="I207" s="14"/>
-      <c r="J207" s="5" t="s">
+      <c r="J207" s="14"/>
+      <c r="K207" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D208" s="5">
         <v>14</v>
       </c>
@@ -6580,11 +7184,12 @@
         <v>555</v>
       </c>
       <c r="I208" s="14"/>
-      <c r="J208" s="5" t="s">
+      <c r="J208" s="14"/>
+      <c r="K208" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D209" s="5">
         <v>15</v>
       </c>
@@ -6601,11 +7206,12 @@
         <v>555</v>
       </c>
       <c r="I209" s="14"/>
-      <c r="J209" s="5" t="s">
+      <c r="J209" s="14"/>
+      <c r="K209" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D210" s="5">
         <v>16</v>
       </c>
@@ -6622,11 +7228,12 @@
         <v>555</v>
       </c>
       <c r="I210" s="14"/>
-      <c r="J210" s="5" t="s">
+      <c r="J210" s="14"/>
+      <c r="K210" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D211" s="5">
         <v>17</v>
       </c>
@@ -6643,11 +7250,12 @@
         <v>555</v>
       </c>
       <c r="I211" s="14"/>
-      <c r="J211" s="5" t="s">
+      <c r="J211" s="14"/>
+      <c r="K211" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D212" s="5">
         <v>18</v>
       </c>
@@ -6664,11 +7272,12 @@
         <v>555</v>
       </c>
       <c r="I212" s="14"/>
-      <c r="J212" s="5" t="s">
+      <c r="J212" s="14"/>
+      <c r="K212" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D213" s="5">
         <v>19</v>
       </c>
@@ -6685,11 +7294,12 @@
         <v>555</v>
       </c>
       <c r="I213" s="14"/>
-      <c r="J213" s="5" t="s">
+      <c r="J213" s="14"/>
+      <c r="K213" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D214" s="5">
         <v>20</v>
       </c>
@@ -6706,11 +7316,12 @@
         <v>555</v>
       </c>
       <c r="I214" s="14"/>
-      <c r="J214" s="5" t="s">
+      <c r="J214" s="14"/>
+      <c r="K214" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D215" s="5">
         <v>21</v>
       </c>
@@ -6727,11 +7338,12 @@
         <v>555</v>
       </c>
       <c r="I215" s="14"/>
-      <c r="J215" s="5" t="s">
+      <c r="J215" s="14"/>
+      <c r="K215" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D216" s="5">
         <v>22</v>
       </c>
@@ -6748,11 +7360,12 @@
         <v>555</v>
       </c>
       <c r="I216" s="14"/>
-      <c r="J216" s="5" t="s">
+      <c r="J216" s="14"/>
+      <c r="K216" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D217" s="5">
         <v>23</v>
       </c>
@@ -6769,11 +7382,12 @@
         <v>555</v>
       </c>
       <c r="I217" s="14"/>
-      <c r="J217" s="5" t="s">
+      <c r="J217" s="14"/>
+      <c r="K217" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D218" s="5">
         <v>24</v>
       </c>
@@ -6790,11 +7404,12 @@
         <v>555</v>
       </c>
       <c r="I218" s="14"/>
-      <c r="J218" s="5" t="s">
+      <c r="J218" s="14"/>
+      <c r="K218" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D219" s="5">
         <v>26</v>
       </c>
@@ -6811,11 +7426,12 @@
         <v>555</v>
       </c>
       <c r="I219" s="14"/>
-      <c r="J219" s="5" t="s">
+      <c r="J219" s="14"/>
+      <c r="K219" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D220" s="5">
         <v>143</v>
       </c>
@@ -6830,11 +7446,12 @@
         <v>555</v>
       </c>
       <c r="I220" s="14"/>
-      <c r="J220" s="5" t="s">
+      <c r="J220" s="14"/>
+      <c r="K220" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D221" s="5">
         <v>149</v>
       </c>
@@ -6849,11 +7466,12 @@
         <v>555</v>
       </c>
       <c r="I221" s="14"/>
-      <c r="J221" s="5" t="s">
+      <c r="J221" s="14"/>
+      <c r="K221" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D222" s="5">
         <v>150</v>
       </c>
@@ -6868,11 +7486,12 @@
         <v>555</v>
       </c>
       <c r="I222" s="14"/>
-      <c r="J222" s="5" t="s">
+      <c r="J222" s="14"/>
+      <c r="K222" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D223" s="5">
         <v>168</v>
       </c>
@@ -6887,11 +7506,12 @@
         <v>555</v>
       </c>
       <c r="I223" s="14"/>
-      <c r="J223" s="5" t="s">
+      <c r="J223" s="14"/>
+      <c r="K223" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="224" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D224" s="5">
         <v>169</v>
       </c>
@@ -6906,11 +7526,12 @@
         <v>555</v>
       </c>
       <c r="I224" s="14"/>
-      <c r="J224" s="5" t="s">
+      <c r="J224" s="14"/>
+      <c r="K224" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="225" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D225" s="5">
         <v>177</v>
       </c>
@@ -6925,11 +7546,12 @@
         <v>555</v>
       </c>
       <c r="I225" s="14"/>
-      <c r="J225" s="5" t="s">
+      <c r="J225" s="14"/>
+      <c r="K225" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D226" s="5">
         <v>182</v>
       </c>
@@ -6944,11 +7566,12 @@
         <v>555</v>
       </c>
       <c r="I226" s="14"/>
-      <c r="J226" s="5" t="s">
+      <c r="J226" s="14"/>
+      <c r="K226" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D227" s="5">
         <v>183</v>
       </c>
@@ -6963,11 +7586,12 @@
         <v>555</v>
       </c>
       <c r="I227" s="14"/>
-      <c r="J227" s="5" t="s">
+      <c r="J227" s="14"/>
+      <c r="K227" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D228" s="5">
         <v>191</v>
       </c>
@@ -6982,11 +7606,12 @@
         <v>555</v>
       </c>
       <c r="I228" s="14"/>
-      <c r="J228" s="5" t="s">
+      <c r="J228" s="14"/>
+      <c r="K228" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="229" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D229" s="5">
         <v>196</v>
       </c>
@@ -7001,11 +7626,12 @@
         <v>555</v>
       </c>
       <c r="I229" s="14"/>
-      <c r="J229" s="5" t="s">
+      <c r="J229" s="14"/>
+      <c r="K229" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D230" s="5">
         <v>197</v>
       </c>
@@ -7022,11 +7648,12 @@
         <v>555</v>
       </c>
       <c r="I230" s="14"/>
-      <c r="J230" s="5" t="s">
+      <c r="J230" s="14"/>
+      <c r="K230" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="231" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D231" s="5">
         <v>200</v>
       </c>
@@ -7043,11 +7670,12 @@
         <v>555</v>
       </c>
       <c r="I231" s="14"/>
-      <c r="J231" s="5" t="s">
+      <c r="J231" s="14"/>
+      <c r="K231" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="232" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D232" s="5">
         <v>203</v>
       </c>
@@ -7064,11 +7692,12 @@
         <v>555</v>
       </c>
       <c r="I232" s="14"/>
-      <c r="J232" s="5" t="s">
+      <c r="J232" s="14"/>
+      <c r="K232" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D233" s="5">
         <v>206</v>
       </c>
@@ -7083,11 +7712,12 @@
         <v>555</v>
       </c>
       <c r="I233" s="14"/>
-      <c r="J233" s="5" t="s">
+      <c r="J233" s="14"/>
+      <c r="K233" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="234" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D234" s="5">
         <v>210</v>
       </c>
@@ -7102,11 +7732,12 @@
         <v>555</v>
       </c>
       <c r="I234" s="14"/>
-      <c r="J234" s="5" t="s">
+      <c r="J234" s="14"/>
+      <c r="K234" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="235" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D235" s="5">
         <v>211</v>
       </c>
@@ -7121,11 +7752,12 @@
         <v>555</v>
       </c>
       <c r="I235" s="14"/>
-      <c r="J235" s="5" t="s">
+      <c r="J235" s="14"/>
+      <c r="K235" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="236" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D236" s="5">
         <v>212</v>
       </c>
@@ -7140,11 +7772,12 @@
         <v>555</v>
       </c>
       <c r="I236" s="14"/>
-      <c r="J236" s="5" t="s">
+      <c r="J236" s="14"/>
+      <c r="K236" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="237" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D237" s="5">
         <v>224</v>
       </c>
@@ -7159,11 +7792,12 @@
         <v>555</v>
       </c>
       <c r="I237" s="14"/>
-      <c r="J237" s="5" t="s">
+      <c r="J237" s="14"/>
+      <c r="K237" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D238" s="5">
         <v>226</v>
       </c>
@@ -7180,11 +7814,12 @@
         <v>555</v>
       </c>
       <c r="I238" s="14"/>
-      <c r="J238" s="5" t="s">
+      <c r="J238" s="14"/>
+      <c r="K238" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D239" s="5">
         <v>227</v>
       </c>
@@ -7201,11 +7836,12 @@
         <v>555</v>
       </c>
       <c r="I239" s="14"/>
-      <c r="J239" s="5" t="s">
+      <c r="J239" s="14"/>
+      <c r="K239" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D240" s="5">
         <v>228</v>
       </c>
@@ -7222,11 +7858,12 @@
         <v>555</v>
       </c>
       <c r="I240" s="14"/>
-      <c r="J240" s="5" t="s">
+      <c r="J240" s="14"/>
+      <c r="K240" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D241" s="5">
         <v>229</v>
       </c>
@@ -7243,11 +7880,12 @@
         <v>555</v>
       </c>
       <c r="I241" s="14"/>
-      <c r="J241" s="5" t="s">
+      <c r="J241" s="14"/>
+      <c r="K241" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D242" s="5">
         <v>230</v>
       </c>
@@ -7264,11 +7902,12 @@
         <v>555</v>
       </c>
       <c r="I242" s="14"/>
-      <c r="J242" s="5" t="s">
+      <c r="J242" s="14"/>
+      <c r="K242" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D243" s="5">
         <v>231</v>
       </c>
@@ -7285,11 +7924,12 @@
         <v>555</v>
       </c>
       <c r="I243" s="14"/>
-      <c r="J243" s="5" t="s">
+      <c r="J243" s="14"/>
+      <c r="K243" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D244" s="5">
         <v>232</v>
       </c>
@@ -7304,11 +7944,12 @@
         <v>555</v>
       </c>
       <c r="I244" s="14"/>
-      <c r="J244" s="5" t="s">
+      <c r="J244" s="14"/>
+      <c r="K244" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D245" s="5">
         <v>233</v>
       </c>
@@ -7323,11 +7964,12 @@
         <v>555</v>
       </c>
       <c r="I245" s="14"/>
-      <c r="J245" s="5" t="s">
+      <c r="J245" s="14"/>
+      <c r="K245" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="4:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="4:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D246" s="5">
         <v>239</v>
       </c>
@@ -7342,11 +7984,12 @@
         <v>555</v>
       </c>
       <c r="I246" s="14"/>
-      <c r="J246" s="5" t="s">
+      <c r="J246" s="14"/>
+      <c r="K246" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D247" s="5">
         <v>246</v>
       </c>
@@ -7361,11 +8004,12 @@
         <v>555</v>
       </c>
       <c r="I247" s="14"/>
-      <c r="J247" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J247" s="14"/>
+      <c r="K247" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D248" s="5">
         <v>247</v>
       </c>
@@ -7380,11 +8024,12 @@
         <v>555</v>
       </c>
       <c r="I248" s="14"/>
-      <c r="J248" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J248" s="14"/>
+      <c r="K248" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D249" s="5">
         <v>248</v>
       </c>
@@ -7399,11 +8044,12 @@
         <v>555</v>
       </c>
       <c r="I249" s="14"/>
-      <c r="J249" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J249" s="14"/>
+      <c r="K249" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D250" s="5">
         <v>248</v>
       </c>
@@ -7418,9 +8064,10 @@
         <v>555</v>
       </c>
       <c r="I250" s="14"/>
-      <c r="J250" s="5"/>
-    </row>
-    <row r="251" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J250" s="14"/>
+      <c r="K250" s="5"/>
+    </row>
+    <row r="251" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D251" s="5">
         <v>249</v>
       </c>
@@ -7435,11 +8082,12 @@
         <v>555</v>
       </c>
       <c r="I251" s="14"/>
-      <c r="J251" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" spans="4:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J251" s="14"/>
+      <c r="K251" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="4:11" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="D252" s="5">
         <v>250</v>
       </c>
@@ -7454,12 +8102,13 @@
         <v>555</v>
       </c>
       <c r="I252" s="14"/>
-      <c r="J252" s="5" t="s">
+      <c r="J252" s="14"/>
+      <c r="K252" s="5" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:J252" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
+  <autoFilter ref="D1:K252" xr:uid="{8768AB1F-9B5E-4B0D-B67A-BDB839544586}">
     <filterColumn colId="1">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7470,7 +8119,7 @@
         <filter val="NÃO"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:J202">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:K202">
       <sortCondition ref="I1:I252"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
todos os produtos na loja
</commit_message>
<xml_diff>
--- a/Controle dos produtos dentro do código.xlsx
+++ b/Controle dos produtos dentro do código.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinicius.macedo\OneDrive - Sinergy RH\Desktop\Coding\Anil-clean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\anil-clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBB2D06-B1AA-479D-8010-401CC45A4864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEDF590-032F-4BED-9EEF-0C720813CF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="823" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="823" xr2:uid="{7DD408A1-9F78-440C-9088-979E9C3A1D92}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="570">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -1731,6 +1731,24 @@
   </si>
   <si>
     <t>triciclos</t>
+  </si>
+  <si>
+    <t>materiais-esportivos</t>
+  </si>
+  <si>
+    <t>tecidos</t>
+  </si>
+  <si>
+    <t>redes-de-descanso</t>
+  </si>
+  <si>
+    <t>variedades</t>
+  </si>
+  <si>
+    <t>brinquedos-de-madeira</t>
+  </si>
+  <si>
+    <t>bonecas-diversidade</t>
   </si>
 </sst>
 </file>
@@ -1855,28 +1873,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2209,8 +2206,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2223,7 +2220,7 @@
     <col min="8" max="8" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="25.5703125" style="2" customWidth="1"/>
     <col min="11" max="11" width="26.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="0" style="2" hidden="1"/>
+    <col min="12" max="12" width="0" style="2" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="10.85546875" style="2" hidden="1"/>
   </cols>
   <sheetData>
@@ -2254,100 +2251,100 @@
       </c>
     </row>
     <row r="2" spans="4:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>99</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>296</v>
       </c>
       <c r="G2" s="8"/>
-      <c r="H2" s="15" t="s">
-        <v>557</v>
-      </c>
-      <c r="I2" s="15">
-        <v>1</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="I2" s="14">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>55</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>462</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>557</v>
-      </c>
-      <c r="I3" s="15">
+      <c r="H3" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="I3" s="14">
         <v>2</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="5" t="s">
         <v>559</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="6" t="s">
         <v>266</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="15" t="s">
-        <v>557</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="H4" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="I4" s="14">
         <v>3</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="3">
+      <c r="D5" s="5">
         <v>130</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>327</v>
       </c>
       <c r="G5" s="8"/>
-      <c r="H5" s="15" t="s">
-        <v>557</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="H5" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="I5" s="14">
         <v>4</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="5" t="s">
         <v>561</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3783,7 +3780,7 @@
         <v>62</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K67" s="3" t="s">
         <v>2</v>
@@ -3955,7 +3952,7 @@
         <v>70</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>2</v>
@@ -4225,7 +4222,7 @@
         <v>85</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K85" s="3" t="s">
         <v>9</v>
@@ -4275,7 +4272,7 @@
         <v>87</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>7</v>
+        <v>564</v>
       </c>
       <c r="K87" s="3" t="s">
         <v>7</v>
@@ -4323,7 +4320,7 @@
         <v>89</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K89" s="3" t="s">
         <v>9</v>
@@ -4347,7 +4344,7 @@
         <v>90</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K90" s="3" t="s">
         <v>2</v>
@@ -4421,7 +4418,7 @@
         <v>93</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>7</v>
+        <v>564</v>
       </c>
       <c r="K93" s="3" t="s">
         <v>7</v>
@@ -4445,7 +4442,7 @@
         <v>94</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>8</v>
+        <v>566</v>
       </c>
       <c r="K94" s="3" t="s">
         <v>8</v>
@@ -4497,7 +4494,7 @@
         <v>96</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>7</v>
+        <v>564</v>
       </c>
       <c r="K96" s="3" t="s">
         <v>7</v>
@@ -4521,7 +4518,7 @@
         <v>97</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K97" s="3" t="s">
         <v>9</v>
@@ -4667,7 +4664,7 @@
         <v>103</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K103" s="3" t="s">
         <v>9</v>
@@ -4691,7 +4688,7 @@
         <v>104</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K104" s="3" t="s">
         <v>9</v>
@@ -4765,7 +4762,7 @@
         <v>106</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K107" s="3" t="s">
         <v>9</v>
@@ -4813,7 +4810,7 @@
         <v>108</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K109" s="3" t="s">
         <v>2</v>
@@ -4837,7 +4834,7 @@
         <v>109</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K110" s="3" t="s">
         <v>2</v>
@@ -4885,7 +4882,7 @@
         <v>111</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="K112" s="3" t="s">
         <v>6</v>
@@ -5007,7 +5004,7 @@
         <v>116</v>
       </c>
       <c r="J117" s="3" t="s">
-        <v>7</v>
+        <v>564</v>
       </c>
       <c r="K117" s="3" t="s">
         <v>7</v>
@@ -5081,7 +5078,7 @@
         <v>118</v>
       </c>
       <c r="J120" s="3" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K120" s="3" t="s">
         <v>2</v>
@@ -5131,7 +5128,7 @@
         <v>119</v>
       </c>
       <c r="J122" s="3" t="s">
-        <v>5</v>
+        <v>568</v>
       </c>
       <c r="K122" s="3" t="s">
         <v>5</v>
@@ -5203,7 +5200,7 @@
         <v>121</v>
       </c>
       <c r="J125" s="3" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="K125" s="3" t="s">
         <v>6</v>
@@ -5227,7 +5224,7 @@
         <v>122</v>
       </c>
       <c r="J126" s="3" t="s">
-        <v>8</v>
+        <v>566</v>
       </c>
       <c r="K126" s="3" t="s">
         <v>8</v>
@@ -5301,7 +5298,7 @@
         <v>124</v>
       </c>
       <c r="J129" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K129" s="3" t="s">
         <v>9</v>
@@ -5351,7 +5348,7 @@
         <v>125</v>
       </c>
       <c r="J131" s="3" t="s">
-        <v>5</v>
+        <v>568</v>
       </c>
       <c r="K131" s="3" t="s">
         <v>5</v>
@@ -5399,7 +5396,7 @@
         <v>127</v>
       </c>
       <c r="J133" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K133" s="3" t="s">
         <v>9</v>
@@ -5617,7 +5614,7 @@
         <v>134</v>
       </c>
       <c r="J142" s="3" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="K142" s="3" t="s">
         <v>6</v>
@@ -5767,7 +5764,7 @@
         <v>141</v>
       </c>
       <c r="J148" s="3" t="s">
-        <v>7</v>
+        <v>564</v>
       </c>
       <c r="K148" s="3" t="s">
         <v>7</v>
@@ -5863,7 +5860,7 @@
         <v>145</v>
       </c>
       <c r="J152" s="3" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K152" s="3" t="s">
         <v>2</v>
@@ -5935,7 +5932,7 @@
         <v>147</v>
       </c>
       <c r="J155" s="3" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K155" s="3" t="s">
         <v>9</v>
@@ -5985,7 +5982,7 @@
         <v>149</v>
       </c>
       <c r="J157" s="3" t="s">
-        <v>7</v>
+        <v>564</v>
       </c>
       <c r="K157" s="3" t="s">
         <v>7</v>
@@ -6073,7 +6070,7 @@
         <v>152</v>
       </c>
       <c r="J161" s="15" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K161" s="3" t="s">
         <v>2</v>
@@ -6249,7 +6246,7 @@
         <v>158</v>
       </c>
       <c r="J169" s="15" t="s">
-        <v>2</v>
+        <v>567</v>
       </c>
       <c r="K169" s="3" t="s">
         <v>2</v>
@@ -6491,7 +6488,7 @@
         <v>167</v>
       </c>
       <c r="J179" s="15" t="s">
-        <v>8</v>
+        <v>566</v>
       </c>
       <c r="K179" s="3" t="s">
         <v>8</v>
@@ -6541,7 +6538,7 @@
         <v>168</v>
       </c>
       <c r="J181" s="15" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K181" s="3" t="s">
         <v>9</v>
@@ -6639,7 +6636,7 @@
         <v>172</v>
       </c>
       <c r="J185" s="15" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="K185" s="3" t="s">
         <v>6</v>
@@ -6687,7 +6684,7 @@
         <v>173</v>
       </c>
       <c r="J187" s="15" t="s">
-        <v>5</v>
+        <v>568</v>
       </c>
       <c r="K187" s="3" t="s">
         <v>5</v>
@@ -6831,7 +6828,7 @@
         <v>179</v>
       </c>
       <c r="J193" s="15" t="s">
-        <v>6</v>
+        <v>569</v>
       </c>
       <c r="K193" s="3" t="s">
         <v>6</v>
@@ -6855,7 +6852,7 @@
         <v>180</v>
       </c>
       <c r="J194" s="15" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K194" s="3" t="s">
         <v>9</v>
@@ -6979,7 +6976,7 @@
         <v>183</v>
       </c>
       <c r="J199" s="15" t="s">
-        <v>5</v>
+        <v>568</v>
       </c>
       <c r="K199" s="3" t="s">
         <v>5</v>
@@ -7053,7 +7050,7 @@
         <v>186</v>
       </c>
       <c r="J202" s="15" t="s">
-        <v>9</v>
+        <v>565</v>
       </c>
       <c r="K202" s="3" t="s">
         <v>9</v>

</xml_diff>